<commit_message>
Added new fields in Degree
</commit_message>
<xml_diff>
--- a/Docs/Project05.xlsx
+++ b/Docs/Project05.xlsx
@@ -686,8 +686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -776,6 +776,10 @@
       <c r="E3" t="s">
         <v>104</v>
       </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F5" si="0">D3&amp;$A$1&amp;"="&amp;A3&amp;", "&amp;$B$1&amp;"="&amp;$B$2&amp;", "&amp;$C$1&amp;" ="&amp;C3&amp;E3</f>
+        <v>new Degree {DegreeId=2, DegreeAbrrev(unique,max 6 characters)=ACS+2, DegreeName(unique, max 20 characters) =MS ACS +DB},</v>
+      </c>
     </row>
     <row r="4" spans="1:26">
       <c r="A4">
@@ -793,6 +797,10 @@
       <c r="E4" t="s">
         <v>104</v>
       </c>
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>new Degree {DegreeId=3, DegreeAbrrev(unique,max 6 characters)=ACS+2, DegreeName(unique, max 20 characters) =MS ACS+NF},</v>
+      </c>
     </row>
     <row r="5" spans="1:26">
       <c r="A5">
@@ -809,6 +817,10 @@
       </c>
       <c r="E5" t="s">
         <v>104</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>new Degree {DegreeId=4, DegreeAbrrev(unique,max 6 characters)=ACS+2, DegreeName(unique, max 20 characters) =MS ACS},</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Created all Model classes
</commit_message>
<xml_diff>
--- a/Docs/Project05.xlsx
+++ b/Docs/Project05.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Degree" sheetId="1" r:id="rId1"/>
@@ -25,13 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="105">
-  <si>
-    <t>DegreeRequirementId</t>
-  </si>
-  <si>
-    <t>DegreeId</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="104">
   <si>
     <t>RequirementId</t>
   </si>
@@ -340,6 +334,9 @@
   </si>
   <si>
     <t>},</t>
+  </si>
+  <si>
+    <t>DegreeRequirementID</t>
   </si>
 </sst>
 </file>
@@ -686,37 +683,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="29.7109375" customWidth="1"/>
     <col min="2" max="2" width="36.7109375" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" customWidth="1"/>
     <col min="4" max="4" width="58.42578125" customWidth="1"/>
     <col min="5" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="D1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>102</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -744,20 +741,20 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F2" t="str">
         <f>D2&amp;$A$1&amp;"="&amp;A2&amp;", "&amp;$B$1&amp;"="&amp;$B$2&amp;", "&amp;$C$1&amp;" ="&amp;C2&amp;E2</f>
-        <v>new Degree {DegreeId=1, DegreeAbrrev(unique,max 6 characters)=ACS+2, DegreeName(unique, max 20 characters) =MS ACS +2 },</v>
+        <v>new Degree {DegreeID=1, DegreeAbrrev(unique,max 6 characters)=ACS+2, DegreeName(unique, max 20 characters) =MS ACS +2 },</v>
       </c>
     </row>
     <row r="3" spans="1:26">
@@ -765,20 +762,20 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" ref="F3:F5" si="0">D3&amp;$A$1&amp;"="&amp;A3&amp;", "&amp;$B$1&amp;"="&amp;$B$2&amp;", "&amp;$C$1&amp;" ="&amp;C3&amp;E3</f>
-        <v>new Degree {DegreeId=2, DegreeAbrrev(unique,max 6 characters)=ACS+2, DegreeName(unique, max 20 characters) =MS ACS +DB},</v>
+        <v>new Degree {DegreeID=2, DegreeAbrrev(unique,max 6 characters)=ACS+2, DegreeName(unique, max 20 characters) =MS ACS +DB},</v>
       </c>
     </row>
     <row r="4" spans="1:26">
@@ -786,20 +783,20 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="0"/>
-        <v>new Degree {DegreeId=3, DegreeAbrrev(unique,max 6 characters)=ACS+2, DegreeName(unique, max 20 characters) =MS ACS+NF},</v>
+        <v>new Degree {DegreeID=3, DegreeAbrrev(unique,max 6 characters)=ACS+2, DegreeName(unique, max 20 characters) =MS ACS+NF},</v>
       </c>
     </row>
     <row r="5" spans="1:26">
@@ -807,20 +804,20 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
         <v>25</v>
       </c>
-      <c r="C5" t="s">
-        <v>27</v>
-      </c>
       <c r="D5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="0"/>
-        <v>new Degree {DegreeId=4, DegreeAbrrev(unique,max 6 characters)=ACS+2, DegreeName(unique, max 20 characters) =MS ACS},</v>
+        <v>new Degree {DegreeID=4, DegreeAbrrev(unique,max 6 characters)=ACS+2, DegreeName(unique, max 20 characters) =MS ACS},</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -1813,25 +1810,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" customWidth="1"/>
-    <col min="2" max="2" width="34.85546875" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" customWidth="1"/>
+    <col min="2" max="2" width="50.140625" customWidth="1"/>
+    <col min="3" max="3" width="43.140625" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1839,10 +1838,10 @@
         <v>460</v>
       </c>
       <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1850,10 +1849,10 @@
         <v>356</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1861,10 +1860,10 @@
         <v>542</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1872,10 +1871,10 @@
         <v>563</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1883,10 +1882,10 @@
         <v>560</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1894,10 +1893,10 @@
         <v>555</v>
       </c>
       <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
         <v>24</v>
-      </c>
-      <c r="C7" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1905,10 +1904,10 @@
         <v>618</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1916,10 +1915,10 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1927,10 +1926,10 @@
         <v>664</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1938,10 +1937,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1949,10 +1948,10 @@
         <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1960,10 +1959,10 @@
         <v>691</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1971,10 +1970,10 @@
         <v>692</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -2967,7 +2966,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -2979,13 +2980,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>103</v>
       </c>
       <c r="B1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -4490,16 +4491,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" t="s">
         <v>48</v>
       </c>
-      <c r="C1" t="s">
-        <v>50</v>
-      </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -7214,19 +7215,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s">
         <v>40</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>41</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>42</v>
-      </c>
-      <c r="D1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -7237,13 +7238,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -7254,13 +7255,13 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -7271,13 +7272,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -7288,13 +7289,13 @@
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -7305,13 +7306,13 @@
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -7322,13 +7323,13 @@
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -7339,13 +7340,13 @@
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -7356,13 +7357,13 @@
         <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -7373,13 +7374,13 @@
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -7390,13 +7391,13 @@
         <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -8402,16 +8403,16 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" t="s">
         <v>47</v>
-      </c>
-      <c r="D1" t="s">
-        <v>49</v>
       </c>
       <c r="E1">
         <v>919</v>
@@ -8422,13 +8423,13 @@
         <v>531494</v>
       </c>
       <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
         <v>51</v>
-      </c>
-      <c r="C2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D2" t="s">
-        <v>53</v>
       </c>
       <c r="E2">
         <v>919564348</v>
@@ -8439,13 +8440,13 @@
         <v>531503</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="E3" s="2">
         <v>919561527</v>
@@ -8456,13 +8457,13 @@
         <v>531384</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E4" s="2">
         <v>919561950</v>
@@ -8473,13 +8474,13 @@
         <v>533707</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>67</v>
       </c>
       <c r="E5" s="2">
         <v>919571235</v>
@@ -8490,13 +8491,13 @@
         <v>531507</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>70</v>
       </c>
       <c r="E6" s="2">
         <v>919564693</v>
@@ -9492,7 +9493,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E995"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -9504,19 +9505,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" t="s">
         <v>72</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>74</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -9530,10 +9531,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -9547,10 +9548,10 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -9564,10 +9565,10 @@
         <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -9581,10 +9582,10 @@
         <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -9598,10 +9599,10 @@
         <v>5</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -9615,10 +9616,10 @@
         <v>1</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -9632,10 +9633,10 @@
         <v>2</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -9649,10 +9650,10 @@
         <v>3</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -9666,10 +9667,10 @@
         <v>4</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -9683,10 +9684,10 @@
         <v>5</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -9700,10 +9701,10 @@
         <v>1</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -9717,10 +9718,10 @@
         <v>2</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -9734,10 +9735,10 @@
         <v>3</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -9751,10 +9752,10 @@
         <v>4</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" customHeight="1">
@@ -9768,10 +9769,10 @@
         <v>5</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1">
@@ -9785,10 +9786,10 @@
         <v>1</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1">
@@ -9802,10 +9803,10 @@
         <v>2</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1">
@@ -9819,10 +9820,10 @@
         <v>3</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1">
@@ -9836,10 +9837,10 @@
         <v>4</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1">
@@ -9853,10 +9854,10 @@
         <v>5</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1">
@@ -9870,10 +9871,10 @@
         <v>1</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1">
@@ -9887,10 +9888,10 @@
         <v>2</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1">
@@ -9904,10 +9905,10 @@
         <v>3</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1">
@@ -9921,10 +9922,10 @@
         <v>4</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1">
@@ -9938,10 +9939,10 @@
         <v>5</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Added fully functionalities for all the Models
</commit_message>
<xml_diff>
--- a/Docs/Project05.xlsx
+++ b/Docs/Project05.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Degree" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="105">
   <si>
     <t>RequirementId</t>
   </si>
@@ -159,12 +159,6 @@
     <t>DegreePlanTermRequirementId</t>
   </si>
   <si>
-    <t>First</t>
-  </si>
-  <si>
-    <t>Last</t>
-  </si>
-  <si>
     <t>DegreePlanID</t>
   </si>
   <si>
@@ -241,15 +235,6 @@
   </si>
   <si>
     <t>StudentID</t>
-  </si>
-  <si>
-    <t>Term</t>
-  </si>
-  <si>
-    <t>TermAbbr</t>
-  </si>
-  <si>
-    <t>Term Label</t>
   </si>
   <si>
     <t>S18</t>
@@ -337,6 +322,24 @@
   </si>
   <si>
     <t>DegreeRequirementID</t>
+  </si>
+  <si>
+    <t>TermAbbrev</t>
+  </si>
+  <si>
+    <t>TermLabel</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>NineOneNineNumber</t>
+  </si>
+  <si>
+    <t>TermID</t>
   </si>
 </sst>
 </file>
@@ -684,7 +687,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -707,13 +710,13 @@
         <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -747,10 +750,10 @@
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="F2" t="str">
         <f>D2&amp;$A$1&amp;"="&amp;A2&amp;", "&amp;$B$1&amp;"="&amp;$B$2&amp;", "&amp;$C$1&amp;" ="&amp;C2&amp;E2</f>
@@ -768,10 +771,10 @@
         <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E3" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" ref="F3:F5" si="0">D3&amp;$A$1&amp;"="&amp;A3&amp;", "&amp;$B$1&amp;"="&amp;$B$2&amp;", "&amp;$C$1&amp;" ="&amp;C3&amp;E3</f>
@@ -789,10 +792,10 @@
         <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E4" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="0"/>
@@ -810,10 +813,10 @@
         <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E5" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="0"/>
@@ -1810,8 +1813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2980,7 +2983,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B1" t="s">
         <v>39</v>
@@ -4478,7 +4481,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -4494,10 +4499,10 @@
         <v>43</v>
       </c>
       <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s">
         <v>46</v>
-      </c>
-      <c r="C1" t="s">
-        <v>48</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -7238,13 +7243,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -7255,13 +7260,13 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -7272,13 +7277,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -7289,13 +7294,13 @@
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -7306,13 +7311,13 @@
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -7323,13 +7328,13 @@
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -7340,13 +7345,13 @@
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -7357,13 +7362,13 @@
         <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -7374,13 +7379,13 @@
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -7391,13 +7396,13 @@
         <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -8390,7 +8395,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -8406,16 +8413,16 @@
         <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>44</v>
+        <v>101</v>
       </c>
       <c r="C1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" t="s">
         <v>45</v>
       </c>
-      <c r="D1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E1">
-        <v>919</v>
+      <c r="E1" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -8423,13 +8430,13 @@
         <v>531494</v>
       </c>
       <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" t="s">
         <v>49</v>
-      </c>
-      <c r="C2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2" t="s">
-        <v>51</v>
       </c>
       <c r="E2">
         <v>919564348</v>
@@ -8440,13 +8447,13 @@
         <v>531503</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="E3" s="2">
         <v>919561527</v>
@@ -8457,13 +8464,13 @@
         <v>531384</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E4" s="2">
         <v>919561950</v>
@@ -8474,13 +8481,13 @@
         <v>533707</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>65</v>
       </c>
       <c r="E5" s="2">
         <v>919571235</v>
@@ -8491,13 +8498,13 @@
         <v>531507</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="E6" s="2">
         <v>919564693</v>
@@ -9493,7 +9500,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E995"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -9505,19 +9514,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C1" t="s">
-        <v>72</v>
+        <v>104</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>73</v>
+        <v>99</v>
       </c>
       <c r="E1" t="s">
-        <v>74</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -9531,10 +9540,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -9548,10 +9557,10 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -9565,10 +9574,10 @@
         <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E4" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -9582,10 +9591,10 @@
         <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -9599,10 +9608,10 @@
         <v>5</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E6" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -9616,10 +9625,10 @@
         <v>1</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="E7" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -9633,10 +9642,10 @@
         <v>2</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E8" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -9650,10 +9659,10 @@
         <v>3</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E9" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -9667,10 +9676,10 @@
         <v>4</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E10" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -9684,10 +9693,10 @@
         <v>5</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E11" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -9701,10 +9710,10 @@
         <v>1</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -9718,10 +9727,10 @@
         <v>2</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -9735,10 +9744,10 @@
         <v>3</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -9752,10 +9761,10 @@
         <v>4</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" customHeight="1">
@@ -9769,10 +9778,10 @@
         <v>5</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1">
@@ -9786,10 +9795,10 @@
         <v>1</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1">
@@ -9803,10 +9812,10 @@
         <v>2</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1">
@@ -9820,10 +9829,10 @@
         <v>3</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1">
@@ -9837,10 +9846,10 @@
         <v>4</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1">
@@ -9854,10 +9863,10 @@
         <v>5</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1">
@@ -9871,10 +9880,10 @@
         <v>1</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1">
@@ -9888,10 +9897,10 @@
         <v>2</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1">
@@ -9905,10 +9914,10 @@
         <v>3</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1">
@@ -9922,10 +9931,10 @@
         <v>4</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1">
@@ -9939,10 +9948,10 @@
         <v>5</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Added seed data for Requirements and DegreePlanTermRequirements
</commit_message>
<xml_diff>
--- a/Docs/Project05.xlsx
+++ b/Docs/Project05.xlsx
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="105">
-  <si>
-    <t>RequirementId</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="105">
   <si>
     <t>RequirementID</t>
   </si>
@@ -163,9 +160,6 @@
   </si>
   <si>
     <t>Snumber</t>
-  </si>
-  <si>
-    <t>TermId</t>
   </si>
   <si>
     <t>Shivani</t>
@@ -340,6 +334,12 @@
   </si>
   <si>
     <t>TermID</t>
+  </si>
+  <si>
+    <t>new Requirement {</t>
+  </si>
+  <si>
+    <t>new DegreePlanTermRequirement {</t>
   </si>
 </sst>
 </file>
@@ -686,8 +686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -701,22 +701,22 @@
   <sheetData>
     <row r="1" spans="1:26">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -744,16 +744,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
       <c r="D2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F2" t="str">
         <f>D2&amp;$A$1&amp;"="&amp;A2&amp;", "&amp;$B$1&amp;"="&amp;$B$2&amp;", "&amp;$C$1&amp;" ="&amp;C2&amp;E2</f>
@@ -765,20 +765,20 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
       <c r="D3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3:F5" si="0">D3&amp;$A$1&amp;"="&amp;A3&amp;", "&amp;$B$1&amp;"="&amp;$B$2&amp;", "&amp;$C$1&amp;" ="&amp;C3&amp;E3</f>
-        <v>new Degree {DegreeID=2, DegreeAbrrev(unique,max 6 characters)=ACS+2, DegreeName(unique, max 20 characters) =MS ACS +DB},</v>
+        <f>D3&amp;$A$1&amp;"="&amp;D11&amp;", "&amp;$B$1&amp;"="&amp;$B$3&amp;", "&amp;$C$1&amp;" ="&amp;C3&amp;E3</f>
+        <v>new Degree {DegreeID=, DegreeAbrrev(unique,max 6 characters)=ACS+DB, DegreeName(unique, max 20 characters) =MS ACS +DB},</v>
       </c>
     </row>
     <row r="4" spans="1:26">
@@ -786,20 +786,20 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
         <v>20</v>
       </c>
-      <c r="C4" t="s">
-        <v>21</v>
-      </c>
       <c r="D4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F4" t="str">
-        <f t="shared" si="0"/>
-        <v>new Degree {DegreeID=3, DegreeAbrrev(unique,max 6 characters)=ACS+2, DegreeName(unique, max 20 characters) =MS ACS+NF},</v>
+        <f>D4&amp;$A$1&amp;"="&amp;A4&amp;", "&amp;$B$1&amp;"="&amp;$B$4&amp;", "&amp;$C$1&amp;" ="&amp;C4&amp;E4</f>
+        <v>new Degree {DegreeID=3, DegreeAbrrev(unique,max 6 characters)=ACS+NF, DegreeName(unique, max 20 characters) =MS ACS+NF},</v>
       </c>
     </row>
     <row r="5" spans="1:26">
@@ -807,20 +807,20 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F5" t="str">
-        <f t="shared" si="0"/>
-        <v>new Degree {DegreeID=4, DegreeAbrrev(unique,max 6 characters)=ACS+2, DegreeName(unique, max 20 characters) =MS ACS},</v>
+        <f>D5&amp;$A$1&amp;"="&amp;A5&amp;", "&amp;$B$1&amp;"="&amp;$B$5&amp;", "&amp;$C$1&amp;" ="&amp;C5&amp;E5</f>
+        <v>new Degree {DegreeID=4, DegreeAbrrev(unique,max 6 characters)=ACS, DegreeName(unique, max 20 characters) =MS ACS},</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -1811,10 +1811,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1000"/>
+  <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1822,161 +1822,301 @@
     <col min="1" max="1" width="24.85546875" customWidth="1"/>
     <col min="2" max="2" width="50.140625" customWidth="1"/>
     <col min="3" max="3" width="43.140625" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="4" max="4" width="29.7109375" customWidth="1"/>
+    <col min="5" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>460</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F2" t="str">
+        <f>D2&amp;$A$1&amp;"="&amp;$A$2&amp;","&amp;$B$1&amp;"="&amp;$B$2&amp;","&amp;$C$1&amp;"="&amp;$C$2&amp;$E$2</f>
+        <v>new Requirement {RequirementID=460,RequirementAbbrev(unique,max 6)=DB,RequirementName(unique, max 20)=44-460 Database},</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>356</v>
       </c>
       <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F3" t="str">
+        <f>D3&amp;$A$1&amp;"="&amp;$A$3&amp;","&amp;$B$1&amp;"="&amp;$B$3&amp;","&amp;$C$1&amp;"="&amp;$C$3&amp;$E$2</f>
+        <v>new Requirement {RequirementID=356,RequirementAbbrev(unique,max 6)=NF,RequirementName(unique, max 20)=44-356 Network Fundamemtals},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>542</v>
       </c>
       <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F4" t="str">
+        <f>D4&amp;$A$1&amp;"="&amp;$A$4&amp;","&amp;$B$1&amp;"="&amp;$B$4&amp;","&amp;$C$1&amp;"="&amp;$C$4&amp;$E$2</f>
+        <v>new Requirement {RequirementID=542,RequirementAbbrev(unique,max 6)=OOP,RequirementName(unique, max 20)=44-542 OOP with Java},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>563</v>
       </c>
       <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F5" t="str">
+        <f>D5&amp;$A$1&amp;"="&amp;$A$5&amp;","&amp;$B$1&amp;"="&amp;$B$5&amp;","&amp;$C$1&amp;"="&amp;$C$5&amp;$E$2</f>
+        <v>new Requirement {RequirementID=563,RequirementAbbrev(unique,max 6)=Web apps,RequirementName(unique, max 20)=44-563 Web apps},</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>560</v>
       </c>
       <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
         <v>18</v>
       </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6" t="s">
+        <v>103</v>
+      </c>
+      <c r="E6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F6" t="str">
+        <f>D6&amp;$A$1&amp;"="&amp;$A$6&amp;","&amp;$B$1&amp;"="&amp;$B$6&amp;","&amp;$C$1&amp;"="&amp;$C$6&amp;$E$2</f>
+        <v>new Requirement {RequirementID=560,RequirementAbbrev(unique,max 6)=ADB,RequirementName(unique, max 20)=44-560 ADB},</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>555</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>103</v>
+      </c>
+      <c r="E7" t="s">
+        <v>95</v>
+      </c>
+      <c r="F7" t="str">
+        <f>D7&amp;$A$1&amp;"="&amp;$A$7&amp;","&amp;$B$1&amp;"="&amp;$B$7&amp;","&amp;$C$1&amp;"="&amp;$C$7&amp;$E$2</f>
+        <v>new Requirement {RequirementID=555,RequirementAbbrev(unique,max 6)=NS,RequirementName(unique, max 20)=44-555 Network Security},</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>618</v>
       </c>
       <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
         <v>26</v>
       </c>
-      <c r="C8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8" t="s">
+        <v>103</v>
+      </c>
+      <c r="E8" t="s">
+        <v>95</v>
+      </c>
+      <c r="F8" t="str">
+        <f>D8&amp;$A$1&amp;"="&amp;$A$8&amp;","&amp;$B$1&amp;"="&amp;$B$8&amp;","&amp;$C$1&amp;"="&amp;$C$8&amp;$E$2</f>
+        <v>new Requirement {RequirementID=618,RequirementAbbrev(unique,max 6)=PM,RequirementName(unique, max 20)=44-618 PM},</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>1</v>
       </c>
       <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
         <v>28</v>
       </c>
-      <c r="C9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="D9" t="s">
+        <v>103</v>
+      </c>
+      <c r="E9" t="s">
+        <v>95</v>
+      </c>
+      <c r="F9" t="str">
+        <f>D9&amp;$A$1&amp;"="&amp;$A$9&amp;","&amp;$B$1&amp;"="&amp;$B$9&amp;","&amp;$C$1&amp;"="&amp;$C$9&amp;$E$2</f>
+        <v>new Requirement {RequirementID=1,RequirementAbbrev(unique,max 6)=Mobile,RequirementName(unique, max 20)=44-643 or 44-644},</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>664</v>
       </c>
       <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
         <v>30</v>
       </c>
-      <c r="C10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="D10" t="s">
+        <v>103</v>
+      </c>
+      <c r="E10" t="s">
+        <v>95</v>
+      </c>
+      <c r="F10" t="str">
+        <f>D10&amp;$A$1&amp;"="&amp;$A$10&amp;","&amp;$B$1&amp;"="&amp;$B$10&amp;","&amp;$C$1&amp;"="&amp;$C$10&amp;$E$2</f>
+        <v>new Requirement {RequirementID=664,RequirementAbbrev(unique,max 6)=UX,RequirementName(unique, max 20)=44-664 UX},</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" t="s">
         <v>32</v>
       </c>
-      <c r="C11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="D11" t="s">
+        <v>103</v>
+      </c>
+      <c r="E11" t="s">
+        <v>95</v>
+      </c>
+      <c r="F11" t="str">
+        <f>D11&amp;$A$1&amp;"="&amp;$A$11&amp;","&amp;$B$1&amp;"="&amp;$B$11&amp;","&amp;$C$1&amp;"="&amp;$C$11&amp;$E$2</f>
+        <v>new Requirement {RequirementID=10,RequirementAbbrev(unique,max 6)=E1,RequirementName(unique, max 20)=Elective 1},</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>20</v>
       </c>
       <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" t="s">
         <v>34</v>
       </c>
-      <c r="C12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="D12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E12" t="s">
+        <v>95</v>
+      </c>
+      <c r="F12" t="str">
+        <f>D12&amp;$A$1&amp;"="&amp;$A$12&amp;","&amp;$B$1&amp;"="&amp;$B$12&amp;","&amp;$C$1&amp;"="&amp;$C$12&amp;$E$2</f>
+        <v>new Requirement {RequirementID=20,RequirementAbbrev(unique,max 6)=E2,RequirementName(unique, max 20)=Elective 2},</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>691</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>35</v>
+      </c>
+      <c r="D13" t="s">
+        <v>103</v>
+      </c>
+      <c r="E13" t="s">
+        <v>95</v>
+      </c>
+      <c r="F13" t="str">
+        <f>D13&amp;$A$1&amp;"="&amp;$A$13&amp;","&amp;$B$1&amp;"="&amp;$B$13&amp;","&amp;$C$1&amp;"="&amp;$C$13&amp;$E$2</f>
+        <v>new Requirement {RequirementID=691,RequirementAbbrev(unique,max 6)=GDP1,RequirementName(unique, max 20)=GDP1},</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>692</v>
       </c>
       <c r="B14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="D14" t="s">
+        <v>103</v>
+      </c>
+      <c r="E14" t="s">
+        <v>95</v>
+      </c>
+      <c r="F14" t="str">
+        <f>D14&amp;$A$1&amp;"="&amp;$A$14&amp;","&amp;$B$1&amp;"="&amp;$B$14&amp;","&amp;$C$1&amp;"="&amp;$C$14&amp;$E$2</f>
+        <v>new Requirement {RequirementID=692,RequirementAbbrev(unique,max 6)=GDP2,RequirementName(unique, max 20)=GDP2},</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -2983,13 +3123,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -4479,10 +4619,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1000"/>
+  <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -4491,24 +4631,36 @@
     <col min="2" max="2" width="30.7109375" customWidth="1"/>
     <col min="3" max="3" width="8.7109375" customWidth="1"/>
     <col min="4" max="4" width="25.85546875" customWidth="1"/>
-    <col min="5" max="26" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" customWidth="1"/>
+    <col min="8" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
         <v>43</v>
       </c>
-      <c r="B1" t="s">
-        <v>44</v>
-      </c>
       <c r="C1" t="s">
-        <v>46</v>
+        <v>102</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4521,8 +4673,18 @@
       <c r="D2">
         <v>460</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G2" t="str">
+        <f>E2&amp;$A$1&amp;"="&amp;$A$2&amp;","&amp;$B$1&amp;"="&amp;$B$2&amp;","&amp;$C$1&amp;"="&amp;$C$2&amp;","&amp;$D$1&amp;"="&amp;$D$2&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=1,DegreePlanID=20,TermID=1,RequirementID=460},</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -4535,8 +4697,18 @@
       <c r="D3">
         <v>356</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" t="s">
+        <v>104</v>
+      </c>
+      <c r="F3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G3" t="str">
+        <f>E3&amp;$A$1&amp;"="&amp;$A$3&amp;","&amp;$B$1&amp;"="&amp;$B$3&amp;","&amp;$C$1&amp;"="&amp;$C$3&amp;","&amp;$D$1&amp;"="&amp;$D$3&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4549,8 +4721,14 @@
       <c r="D4">
         <v>542</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4" t="s">
+        <v>104</v>
+      </c>
+      <c r="F4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -4563,8 +4741,14 @@
       <c r="D5">
         <v>563</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5" t="s">
+        <v>104</v>
+      </c>
+      <c r="F5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4577,8 +4761,14 @@
       <c r="D6">
         <v>560</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6" t="s">
+        <v>104</v>
+      </c>
+      <c r="F6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -4591,8 +4781,14 @@
       <c r="D7">
         <v>555</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7" t="s">
+        <v>104</v>
+      </c>
+      <c r="F7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4605,8 +4801,14 @@
       <c r="D8">
         <v>618</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8" t="s">
+        <v>104</v>
+      </c>
+      <c r="F8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -4619,8 +4821,14 @@
       <c r="D9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4633,8 +4841,14 @@
       <c r="D10">
         <v>664</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10" t="s">
+        <v>104</v>
+      </c>
+      <c r="F10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -4647,8 +4861,14 @@
       <c r="D11">
         <v>691</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11" t="s">
+        <v>104</v>
+      </c>
+      <c r="F11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>11</v>
       </c>
@@ -4661,8 +4881,14 @@
       <c r="D12">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12" t="s">
+        <v>104</v>
+      </c>
+      <c r="F12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -4675,8 +4901,14 @@
       <c r="D13">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="E13" t="s">
+        <v>104</v>
+      </c>
+      <c r="F13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>13</v>
       </c>
@@ -4689,8 +4921,14 @@
       <c r="D14">
         <v>692</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="E14" t="s">
+        <v>104</v>
+      </c>
+      <c r="F14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -4703,8 +4941,14 @@
       <c r="D15">
         <v>460</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="E15" t="s">
+        <v>104</v>
+      </c>
+      <c r="F15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4717,8 +4961,14 @@
       <c r="D16">
         <v>356</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16" t="s">
+        <v>104</v>
+      </c>
+      <c r="F16" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -4731,8 +4981,14 @@
       <c r="D17">
         <v>542</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17" t="s">
+        <v>104</v>
+      </c>
+      <c r="F17" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4745,8 +5001,14 @@
       <c r="D18">
         <v>563</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18" t="s">
+        <v>104</v>
+      </c>
+      <c r="F18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -4759,8 +5021,14 @@
       <c r="D19">
         <v>560</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19" t="s">
+        <v>104</v>
+      </c>
+      <c r="F19" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20">
         <v>19</v>
       </c>
@@ -4773,8 +5041,14 @@
       <c r="D20">
         <v>555</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E20" t="s">
+        <v>104</v>
+      </c>
+      <c r="F20" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" customHeight="1">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -4787,8 +5061,14 @@
       <c r="D21">
         <v>618</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E21" t="s">
+        <v>104</v>
+      </c>
+      <c r="F21" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" customHeight="1">
       <c r="A22">
         <v>21</v>
       </c>
@@ -4801,8 +5081,14 @@
       <c r="D22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E22" t="s">
+        <v>104</v>
+      </c>
+      <c r="F22" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" customHeight="1">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -4815,8 +5101,14 @@
       <c r="D23">
         <v>664</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E23" t="s">
+        <v>104</v>
+      </c>
+      <c r="F23" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15.75" customHeight="1">
       <c r="A24">
         <v>23</v>
       </c>
@@ -4829,8 +5121,14 @@
       <c r="D24">
         <v>691</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E24" t="s">
+        <v>104</v>
+      </c>
+      <c r="F24" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" customHeight="1">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -4843,8 +5141,14 @@
       <c r="D25">
         <v>10</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E25" t="s">
+        <v>104</v>
+      </c>
+      <c r="F25" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" customHeight="1">
       <c r="A26">
         <v>25</v>
       </c>
@@ -4857,8 +5161,14 @@
       <c r="D26">
         <v>20</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E26" t="s">
+        <v>104</v>
+      </c>
+      <c r="F26" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15.75" customHeight="1">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -4871,8 +5181,14 @@
       <c r="D27">
         <v>692</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E27" t="s">
+        <v>104</v>
+      </c>
+      <c r="F27" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15.75" customHeight="1">
       <c r="A28">
         <v>27</v>
       </c>
@@ -4885,8 +5201,14 @@
       <c r="D28">
         <v>460</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E28" t="s">
+        <v>104</v>
+      </c>
+      <c r="F28" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15.75" customHeight="1">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -4899,8 +5221,14 @@
       <c r="D29">
         <v>356</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E29" t="s">
+        <v>104</v>
+      </c>
+      <c r="F29" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15.75" customHeight="1">
       <c r="A30">
         <v>29</v>
       </c>
@@ -4913,8 +5241,14 @@
       <c r="D30">
         <v>542</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E30" t="s">
+        <v>104</v>
+      </c>
+      <c r="F30" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="15.75" customHeight="1">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -4927,8 +5261,14 @@
       <c r="D31">
         <v>563</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E31" t="s">
+        <v>104</v>
+      </c>
+      <c r="F31" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="15.75" customHeight="1">
       <c r="A32">
         <v>31</v>
       </c>
@@ -4941,8 +5281,14 @@
       <c r="D32">
         <v>560</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E32" t="s">
+        <v>104</v>
+      </c>
+      <c r="F32" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="15.75" customHeight="1">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -4955,8 +5301,14 @@
       <c r="D33">
         <v>555</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E33" t="s">
+        <v>104</v>
+      </c>
+      <c r="F33" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="15.75" customHeight="1">
       <c r="A34">
         <v>33</v>
       </c>
@@ -4969,8 +5321,14 @@
       <c r="D34">
         <v>618</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E34" t="s">
+        <v>104</v>
+      </c>
+      <c r="F34" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="15.75" customHeight="1">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -4983,8 +5341,14 @@
       <c r="D35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E35" t="s">
+        <v>104</v>
+      </c>
+      <c r="F35" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="15.75" customHeight="1">
       <c r="A36">
         <v>35</v>
       </c>
@@ -4997,8 +5361,14 @@
       <c r="D36">
         <v>664</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E36" t="s">
+        <v>104</v>
+      </c>
+      <c r="F36" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="15.75" customHeight="1">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -5011,8 +5381,14 @@
       <c r="D37">
         <v>691</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E37" t="s">
+        <v>104</v>
+      </c>
+      <c r="F37" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="15.75" customHeight="1">
       <c r="A38">
         <v>37</v>
       </c>
@@ -5025,8 +5401,14 @@
       <c r="D38">
         <v>10</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E38" t="s">
+        <v>104</v>
+      </c>
+      <c r="F38" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="15.75" customHeight="1">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -5039,8 +5421,14 @@
       <c r="D39">
         <v>20</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E39" t="s">
+        <v>104</v>
+      </c>
+      <c r="F39" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="15.75" customHeight="1">
       <c r="A40">
         <v>39</v>
       </c>
@@ -5053,8 +5441,14 @@
       <c r="D40">
         <v>692</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E40" t="s">
+        <v>104</v>
+      </c>
+      <c r="F40" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="15.75" customHeight="1">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -5067,8 +5461,14 @@
       <c r="D41">
         <v>460</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E41" t="s">
+        <v>104</v>
+      </c>
+      <c r="F41" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="15.75" customHeight="1">
       <c r="A42">
         <v>41</v>
       </c>
@@ -5081,8 +5481,14 @@
       <c r="D42">
         <v>356</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E42" t="s">
+        <v>104</v>
+      </c>
+      <c r="F42" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="15.75" customHeight="1">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -5095,8 +5501,14 @@
       <c r="D43">
         <v>542</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E43" t="s">
+        <v>104</v>
+      </c>
+      <c r="F43" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="15.75" customHeight="1">
       <c r="A44">
         <v>43</v>
       </c>
@@ -5109,8 +5521,14 @@
       <c r="D44">
         <v>563</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E44" t="s">
+        <v>104</v>
+      </c>
+      <c r="F44" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="15.75" customHeight="1">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -5123,8 +5541,14 @@
       <c r="D45">
         <v>560</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E45" t="s">
+        <v>104</v>
+      </c>
+      <c r="F45" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="15.75" customHeight="1">
       <c r="A46">
         <v>45</v>
       </c>
@@ -5137,8 +5561,14 @@
       <c r="D46">
         <v>555</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E46" t="s">
+        <v>104</v>
+      </c>
+      <c r="F46" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="15.75" customHeight="1">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -5151,8 +5581,14 @@
       <c r="D47">
         <v>618</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E47" t="s">
+        <v>104</v>
+      </c>
+      <c r="F47" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="15.75" customHeight="1">
       <c r="A48">
         <v>47</v>
       </c>
@@ -5165,8 +5601,14 @@
       <c r="D48">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E48" t="s">
+        <v>104</v>
+      </c>
+      <c r="F48" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="15.75" customHeight="1">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -5179,8 +5621,14 @@
       <c r="D49">
         <v>664</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E49" t="s">
+        <v>104</v>
+      </c>
+      <c r="F49" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="15.75" customHeight="1">
       <c r="A50">
         <v>49</v>
       </c>
@@ -5193,8 +5641,14 @@
       <c r="D50">
         <v>691</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E50" t="s">
+        <v>104</v>
+      </c>
+      <c r="F50" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="15.75" customHeight="1">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -5207,8 +5661,14 @@
       <c r="D51">
         <v>10</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E51" t="s">
+        <v>104</v>
+      </c>
+      <c r="F51" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="15.75" customHeight="1">
       <c r="A52">
         <v>51</v>
       </c>
@@ -5221,8 +5681,14 @@
       <c r="D52">
         <v>20</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E52" t="s">
+        <v>104</v>
+      </c>
+      <c r="F52" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="15.75" customHeight="1">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -5235,8 +5701,14 @@
       <c r="D53">
         <v>692</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E53" t="s">
+        <v>104</v>
+      </c>
+      <c r="F53" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="15.75" customHeight="1">
       <c r="A54">
         <v>53</v>
       </c>
@@ -5249,8 +5721,14 @@
       <c r="D54">
         <v>460</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E54" t="s">
+        <v>104</v>
+      </c>
+      <c r="F54" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="15.75" customHeight="1">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -5263,8 +5741,14 @@
       <c r="D55">
         <v>356</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E55" t="s">
+        <v>104</v>
+      </c>
+      <c r="F55" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="15.75" customHeight="1">
       <c r="A56">
         <v>55</v>
       </c>
@@ -5277,8 +5761,14 @@
       <c r="D56">
         <v>542</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E56" t="s">
+        <v>104</v>
+      </c>
+      <c r="F56" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="15.75" customHeight="1">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -5291,8 +5781,14 @@
       <c r="D57">
         <v>563</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E57" t="s">
+        <v>104</v>
+      </c>
+      <c r="F57" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="15.75" customHeight="1">
       <c r="A58">
         <v>57</v>
       </c>
@@ -5305,8 +5801,14 @@
       <c r="D58">
         <v>560</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E58" t="s">
+        <v>104</v>
+      </c>
+      <c r="F58" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="15.75" customHeight="1">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -5319,8 +5821,14 @@
       <c r="D59">
         <v>555</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E59" t="s">
+        <v>104</v>
+      </c>
+      <c r="F59" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="15.75" customHeight="1">
       <c r="A60">
         <v>59</v>
       </c>
@@ -5333,8 +5841,14 @@
       <c r="D60">
         <v>618</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E60" t="s">
+        <v>104</v>
+      </c>
+      <c r="F60" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="15.75" customHeight="1">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -5347,8 +5861,14 @@
       <c r="D61">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E61" t="s">
+        <v>104</v>
+      </c>
+      <c r="F61" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="15.75" customHeight="1">
       <c r="A62">
         <v>61</v>
       </c>
@@ -5361,8 +5881,14 @@
       <c r="D62">
         <v>664</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E62" t="s">
+        <v>104</v>
+      </c>
+      <c r="F62" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="15.75" customHeight="1">
       <c r="A63" s="2">
         <v>62</v>
       </c>
@@ -5375,8 +5901,14 @@
       <c r="D63">
         <v>691</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E63" t="s">
+        <v>104</v>
+      </c>
+      <c r="F63" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="15.75" customHeight="1">
       <c r="A64">
         <v>63</v>
       </c>
@@ -5389,8 +5921,14 @@
       <c r="D64">
         <v>10</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E64" t="s">
+        <v>104</v>
+      </c>
+      <c r="F64" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="15.75" customHeight="1">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -5403,8 +5941,14 @@
       <c r="D65">
         <v>20</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E65" t="s">
+        <v>104</v>
+      </c>
+      <c r="F65" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="15.75" customHeight="1">
       <c r="A66">
         <v>65</v>
       </c>
@@ -5417,8 +5961,14 @@
       <c r="D66">
         <v>692</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E66" t="s">
+        <v>104</v>
+      </c>
+      <c r="F66" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="15.75" customHeight="1">
       <c r="A67" s="2">
         <v>66</v>
       </c>
@@ -5431,8 +5981,14 @@
       <c r="D67">
         <v>460</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E67" t="s">
+        <v>104</v>
+      </c>
+      <c r="F67" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="15.75" customHeight="1">
       <c r="A68">
         <v>67</v>
       </c>
@@ -5445,8 +6001,14 @@
       <c r="D68">
         <v>356</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E68" t="s">
+        <v>104</v>
+      </c>
+      <c r="F68" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="15.75" customHeight="1">
       <c r="A69" s="2">
         <v>68</v>
       </c>
@@ -5459,8 +6021,14 @@
       <c r="D69">
         <v>542</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E69" t="s">
+        <v>104</v>
+      </c>
+      <c r="F69" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="15.75" customHeight="1">
       <c r="A70">
         <v>69</v>
       </c>
@@ -5473,8 +6041,14 @@
       <c r="D70">
         <v>563</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E70" t="s">
+        <v>104</v>
+      </c>
+      <c r="F70" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="15.75" customHeight="1">
       <c r="A71" s="2">
         <v>70</v>
       </c>
@@ -5487,8 +6061,14 @@
       <c r="D71">
         <v>560</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E71" t="s">
+        <v>104</v>
+      </c>
+      <c r="F71" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="15.75" customHeight="1">
       <c r="A72">
         <v>71</v>
       </c>
@@ -5501,8 +6081,14 @@
       <c r="D72">
         <v>555</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E72" t="s">
+        <v>104</v>
+      </c>
+      <c r="F72" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="15.75" customHeight="1">
       <c r="A73" s="2">
         <v>72</v>
       </c>
@@ -5515,8 +6101,14 @@
       <c r="D73">
         <v>618</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E73" t="s">
+        <v>104</v>
+      </c>
+      <c r="F73" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="15.75" customHeight="1">
       <c r="A74">
         <v>73</v>
       </c>
@@ -5529,8 +6121,14 @@
       <c r="D74">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E74" t="s">
+        <v>104</v>
+      </c>
+      <c r="F74" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="15.75" customHeight="1">
       <c r="A75" s="2">
         <v>74</v>
       </c>
@@ -5543,8 +6141,14 @@
       <c r="D75">
         <v>664</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E75" t="s">
+        <v>104</v>
+      </c>
+      <c r="F75" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="15.75" customHeight="1">
       <c r="A76">
         <v>75</v>
       </c>
@@ -5557,8 +6161,14 @@
       <c r="D76">
         <v>691</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E76" t="s">
+        <v>104</v>
+      </c>
+      <c r="F76" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="15.75" customHeight="1">
       <c r="A77" s="2">
         <v>76</v>
       </c>
@@ -5571,8 +6181,14 @@
       <c r="D77">
         <v>10</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E77" t="s">
+        <v>104</v>
+      </c>
+      <c r="F77" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="15.75" customHeight="1">
       <c r="A78">
         <v>77</v>
       </c>
@@ -5585,8 +6201,14 @@
       <c r="D78">
         <v>20</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E78" t="s">
+        <v>104</v>
+      </c>
+      <c r="F78" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="15.75" customHeight="1">
       <c r="A79" s="2">
         <v>78</v>
       </c>
@@ -5599,8 +6221,14 @@
       <c r="D79">
         <v>692</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E79" t="s">
+        <v>104</v>
+      </c>
+      <c r="F79" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="15.75" customHeight="1">
       <c r="A80">
         <v>79</v>
       </c>
@@ -5613,8 +6241,14 @@
       <c r="D80">
         <v>460</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E80" t="s">
+        <v>104</v>
+      </c>
+      <c r="F80" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="15.75" customHeight="1">
       <c r="A81" s="2">
         <v>80</v>
       </c>
@@ -5627,8 +6261,14 @@
       <c r="D81">
         <v>356</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E81" t="s">
+        <v>104</v>
+      </c>
+      <c r="F81" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="15.75" customHeight="1">
       <c r="A82">
         <v>81</v>
       </c>
@@ -5641,8 +6281,14 @@
       <c r="D82">
         <v>542</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E82" t="s">
+        <v>104</v>
+      </c>
+      <c r="F82" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="15.75" customHeight="1">
       <c r="A83" s="2">
         <v>82</v>
       </c>
@@ -5655,8 +6301,14 @@
       <c r="D83">
         <v>563</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E83" t="s">
+        <v>104</v>
+      </c>
+      <c r="F83" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="15.75" customHeight="1">
       <c r="A84">
         <v>83</v>
       </c>
@@ -5669,8 +6321,14 @@
       <c r="D84">
         <v>560</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E84" t="s">
+        <v>104</v>
+      </c>
+      <c r="F84" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="15.75" customHeight="1">
       <c r="A85" s="2">
         <v>84</v>
       </c>
@@ -5683,8 +6341,14 @@
       <c r="D85">
         <v>555</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E85" t="s">
+        <v>104</v>
+      </c>
+      <c r="F85" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="15.75" customHeight="1">
       <c r="A86">
         <v>85</v>
       </c>
@@ -5697,8 +6361,14 @@
       <c r="D86">
         <v>618</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E86" t="s">
+        <v>104</v>
+      </c>
+      <c r="F86" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" ht="15.75" customHeight="1">
       <c r="A87" s="2">
         <v>86</v>
       </c>
@@ -5711,8 +6381,14 @@
       <c r="D87">
         <v>1</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E87" t="s">
+        <v>104</v>
+      </c>
+      <c r="F87" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" ht="15.75" customHeight="1">
       <c r="A88">
         <v>87</v>
       </c>
@@ -5725,8 +6401,14 @@
       <c r="D88">
         <v>664</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E88" t="s">
+        <v>104</v>
+      </c>
+      <c r="F88" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" ht="15.75" customHeight="1">
       <c r="A89" s="2">
         <v>88</v>
       </c>
@@ -5739,8 +6421,14 @@
       <c r="D89">
         <v>691</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E89" t="s">
+        <v>104</v>
+      </c>
+      <c r="F89" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" ht="15.75" customHeight="1">
       <c r="A90">
         <v>89</v>
       </c>
@@ -5753,8 +6441,14 @@
       <c r="D90">
         <v>10</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E90" t="s">
+        <v>104</v>
+      </c>
+      <c r="F90" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" ht="15.75" customHeight="1">
       <c r="A91" s="2">
         <v>90</v>
       </c>
@@ -5767,8 +6461,14 @@
       <c r="D91">
         <v>20</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E91" t="s">
+        <v>104</v>
+      </c>
+      <c r="F91" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" ht="15.75" customHeight="1">
       <c r="A92">
         <v>91</v>
       </c>
@@ -5781,8 +6481,14 @@
       <c r="D92">
         <v>692</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E92" t="s">
+        <v>104</v>
+      </c>
+      <c r="F92" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" ht="15.75" customHeight="1">
       <c r="A93" s="2">
         <v>92</v>
       </c>
@@ -5795,8 +6501,14 @@
       <c r="D93">
         <v>460</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E93" t="s">
+        <v>104</v>
+      </c>
+      <c r="F93" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" ht="15.75" customHeight="1">
       <c r="A94">
         <v>93</v>
       </c>
@@ -5809,8 +6521,14 @@
       <c r="D94">
         <v>356</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E94" t="s">
+        <v>104</v>
+      </c>
+      <c r="F94" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" ht="15.75" customHeight="1">
       <c r="A95" s="2">
         <v>94</v>
       </c>
@@ -5823,8 +6541,14 @@
       <c r="D95">
         <v>542</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E95" t="s">
+        <v>104</v>
+      </c>
+      <c r="F95" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" ht="15.75" customHeight="1">
       <c r="A96">
         <v>95</v>
       </c>
@@ -5837,8 +6561,14 @@
       <c r="D96">
         <v>563</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E96" t="s">
+        <v>104</v>
+      </c>
+      <c r="F96" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" ht="15.75" customHeight="1">
       <c r="A97" s="2">
         <v>96</v>
       </c>
@@ -5851,8 +6581,14 @@
       <c r="D97">
         <v>560</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E97" t="s">
+        <v>104</v>
+      </c>
+      <c r="F97" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" ht="15.75" customHeight="1">
       <c r="A98">
         <v>97</v>
       </c>
@@ -5865,8 +6601,14 @@
       <c r="D98">
         <v>555</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E98" t="s">
+        <v>104</v>
+      </c>
+      <c r="F98" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" ht="15.75" customHeight="1">
       <c r="A99" s="2">
         <v>98</v>
       </c>
@@ -5879,8 +6621,14 @@
       <c r="D99">
         <v>618</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E99" t="s">
+        <v>104</v>
+      </c>
+      <c r="F99" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" ht="15.75" customHeight="1">
       <c r="A100">
         <v>99</v>
       </c>
@@ -5893,8 +6641,14 @@
       <c r="D100">
         <v>1</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E100" t="s">
+        <v>104</v>
+      </c>
+      <c r="F100" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" ht="15.75" customHeight="1">
       <c r="A101" s="2">
         <v>100</v>
       </c>
@@ -5907,8 +6661,14 @@
       <c r="D101">
         <v>664</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E101" t="s">
+        <v>104</v>
+      </c>
+      <c r="F101" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" ht="15.75" customHeight="1">
       <c r="A102">
         <v>101</v>
       </c>
@@ -5921,8 +6681,14 @@
       <c r="D102">
         <v>691</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E102" t="s">
+        <v>104</v>
+      </c>
+      <c r="F102" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" ht="15.75" customHeight="1">
       <c r="A103" s="2">
         <v>102</v>
       </c>
@@ -5935,8 +6701,14 @@
       <c r="D103">
         <v>10</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E103" t="s">
+        <v>104</v>
+      </c>
+      <c r="F103" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" ht="15.75" customHeight="1">
       <c r="A104">
         <v>103</v>
       </c>
@@ -5949,8 +6721,14 @@
       <c r="D104">
         <v>20</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E104" t="s">
+        <v>104</v>
+      </c>
+      <c r="F104" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" ht="15.75" customHeight="1">
       <c r="A105" s="2">
         <v>104</v>
       </c>
@@ -5963,8 +6741,14 @@
       <c r="D105">
         <v>692</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E105" t="s">
+        <v>104</v>
+      </c>
+      <c r="F105" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" ht="15.75" customHeight="1">
       <c r="A106">
         <v>105</v>
       </c>
@@ -5977,8 +6761,14 @@
       <c r="D106">
         <v>460</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E106" t="s">
+        <v>104</v>
+      </c>
+      <c r="F106" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" ht="15.75" customHeight="1">
       <c r="A107" s="2">
         <v>106</v>
       </c>
@@ -5991,8 +6781,14 @@
       <c r="D107">
         <v>356</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E107" t="s">
+        <v>104</v>
+      </c>
+      <c r="F107" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" ht="15.75" customHeight="1">
       <c r="A108">
         <v>107</v>
       </c>
@@ -6005,8 +6801,14 @@
       <c r="D108">
         <v>542</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E108" t="s">
+        <v>104</v>
+      </c>
+      <c r="F108" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" ht="15.75" customHeight="1">
       <c r="A109" s="2">
         <v>108</v>
       </c>
@@ -6019,8 +6821,14 @@
       <c r="D109">
         <v>563</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E109" t="s">
+        <v>104</v>
+      </c>
+      <c r="F109" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" ht="15.75" customHeight="1">
       <c r="A110">
         <v>109</v>
       </c>
@@ -6033,8 +6841,14 @@
       <c r="D110">
         <v>560</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E110" t="s">
+        <v>104</v>
+      </c>
+      <c r="F110" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" ht="15.75" customHeight="1">
       <c r="A111" s="2">
         <v>110</v>
       </c>
@@ -6047,8 +6861,14 @@
       <c r="D111">
         <v>555</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E111" t="s">
+        <v>104</v>
+      </c>
+      <c r="F111" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" ht="15.75" customHeight="1">
       <c r="A112">
         <v>111</v>
       </c>
@@ -6061,8 +6881,14 @@
       <c r="D112">
         <v>618</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E112" t="s">
+        <v>104</v>
+      </c>
+      <c r="F112" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" ht="15.75" customHeight="1">
       <c r="A113" s="2">
         <v>112</v>
       </c>
@@ -6075,8 +6901,14 @@
       <c r="D113">
         <v>1</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E113" t="s">
+        <v>104</v>
+      </c>
+      <c r="F113" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" ht="15.75" customHeight="1">
       <c r="A114">
         <v>113</v>
       </c>
@@ -6089,8 +6921,14 @@
       <c r="D114">
         <v>664</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E114" t="s">
+        <v>104</v>
+      </c>
+      <c r="F114" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" ht="15.75" customHeight="1">
       <c r="A115" s="2">
         <v>114</v>
       </c>
@@ -6103,8 +6941,14 @@
       <c r="D115">
         <v>691</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E115" t="s">
+        <v>104</v>
+      </c>
+      <c r="F115" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" ht="15.75" customHeight="1">
       <c r="A116">
         <v>115</v>
       </c>
@@ -6117,8 +6961,14 @@
       <c r="D116">
         <v>10</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E116" t="s">
+        <v>104</v>
+      </c>
+      <c r="F116" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" ht="15.75" customHeight="1">
       <c r="A117" s="2">
         <v>116</v>
       </c>
@@ -6131,8 +6981,14 @@
       <c r="D117">
         <v>20</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E117" t="s">
+        <v>104</v>
+      </c>
+      <c r="F117" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" ht="15.75" customHeight="1">
       <c r="A118">
         <v>117</v>
       </c>
@@ -6145,8 +7001,14 @@
       <c r="D118">
         <v>692</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E118" t="s">
+        <v>104</v>
+      </c>
+      <c r="F118" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" ht="15.75" customHeight="1">
       <c r="A119" s="2">
         <v>118</v>
       </c>
@@ -6159,8 +7021,14 @@
       <c r="D119">
         <v>460</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E119" t="s">
+        <v>104</v>
+      </c>
+      <c r="F119" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" ht="15.75" customHeight="1">
       <c r="A120">
         <v>119</v>
       </c>
@@ -6173,8 +7041,14 @@
       <c r="D120">
         <v>356</v>
       </c>
-    </row>
-    <row r="121" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E120" t="s">
+        <v>104</v>
+      </c>
+      <c r="F120" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" ht="15.75" customHeight="1">
       <c r="A121" s="2">
         <v>120</v>
       </c>
@@ -6187,8 +7061,14 @@
       <c r="D121">
         <v>542</v>
       </c>
-    </row>
-    <row r="122" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E121" t="s">
+        <v>104</v>
+      </c>
+      <c r="F121" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" ht="15.75" customHeight="1">
       <c r="A122">
         <v>121</v>
       </c>
@@ -6201,8 +7081,14 @@
       <c r="D122">
         <v>563</v>
       </c>
-    </row>
-    <row r="123" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E122" t="s">
+        <v>104</v>
+      </c>
+      <c r="F122" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" ht="15.75" customHeight="1">
       <c r="A123" s="2">
         <v>122</v>
       </c>
@@ -6215,8 +7101,14 @@
       <c r="D123">
         <v>560</v>
       </c>
-    </row>
-    <row r="124" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E123" t="s">
+        <v>104</v>
+      </c>
+      <c r="F123" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" ht="15.75" customHeight="1">
       <c r="A124">
         <v>123</v>
       </c>
@@ -6229,8 +7121,14 @@
       <c r="D124">
         <v>555</v>
       </c>
-    </row>
-    <row r="125" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E124" t="s">
+        <v>104</v>
+      </c>
+      <c r="F124" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" ht="15.75" customHeight="1">
       <c r="A125" s="2">
         <v>124</v>
       </c>
@@ -6243,8 +7141,14 @@
       <c r="D125">
         <v>618</v>
       </c>
-    </row>
-    <row r="126" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E125" t="s">
+        <v>104</v>
+      </c>
+      <c r="F125" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" ht="15.75" customHeight="1">
       <c r="A126">
         <v>125</v>
       </c>
@@ -6257,8 +7161,14 @@
       <c r="D126">
         <v>1</v>
       </c>
-    </row>
-    <row r="127" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E126" t="s">
+        <v>104</v>
+      </c>
+      <c r="F126" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" ht="15.75" customHeight="1">
       <c r="A127" s="2">
         <v>126</v>
       </c>
@@ -6271,8 +7181,14 @@
       <c r="D127">
         <v>664</v>
       </c>
-    </row>
-    <row r="128" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E127" t="s">
+        <v>104</v>
+      </c>
+      <c r="F127" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" ht="15.75" customHeight="1">
       <c r="A128">
         <v>127</v>
       </c>
@@ -6285,8 +7201,14 @@
       <c r="D128">
         <v>691</v>
       </c>
-    </row>
-    <row r="129" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E128" t="s">
+        <v>104</v>
+      </c>
+      <c r="F128" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" ht="15.75" customHeight="1">
       <c r="A129" s="2">
         <v>128</v>
       </c>
@@ -6299,8 +7221,14 @@
       <c r="D129">
         <v>10</v>
       </c>
-    </row>
-    <row r="130" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E129" t="s">
+        <v>104</v>
+      </c>
+      <c r="F129" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" ht="15.75" customHeight="1">
       <c r="A130">
         <v>129</v>
       </c>
@@ -6313,8 +7241,14 @@
       <c r="D130">
         <v>20</v>
       </c>
-    </row>
-    <row r="131" spans="1:4" ht="15.75" customHeight="1">
+      <c r="E130" t="s">
+        <v>104</v>
+      </c>
+      <c r="F130" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" ht="15.75" customHeight="1">
       <c r="A131" s="2">
         <v>130</v>
       </c>
@@ -6327,20 +7261,26 @@
       <c r="D131">
         <v>692</v>
       </c>
-    </row>
-    <row r="132" spans="1:4" ht="15.75" customHeight="1"/>
-    <row r="133" spans="1:4" ht="15.75" customHeight="1"/>
-    <row r="134" spans="1:4" ht="15.75" customHeight="1"/>
-    <row r="135" spans="1:4" ht="15.75" customHeight="1"/>
-    <row r="136" spans="1:4" ht="15.75" customHeight="1"/>
-    <row r="137" spans="1:4" ht="15.75" customHeight="1"/>
-    <row r="138" spans="1:4" ht="15.75" customHeight="1"/>
-    <row r="139" spans="1:4" ht="15.75" customHeight="1"/>
-    <row r="140" spans="1:4" ht="15.75" customHeight="1"/>
-    <row r="141" spans="1:4" ht="15.75" customHeight="1"/>
-    <row r="142" spans="1:4" ht="15.75" customHeight="1"/>
-    <row r="143" spans="1:4" ht="15.75" customHeight="1"/>
-    <row r="144" spans="1:4" ht="15.75" customHeight="1"/>
+      <c r="E131" t="s">
+        <v>104</v>
+      </c>
+      <c r="F131" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="133" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="134" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="135" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="136" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="137" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="138" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="139" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="140" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="141" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="142" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="143" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="144" spans="1:6" ht="15.75" customHeight="1"/>
     <row r="145" ht="15.75" customHeight="1"/>
     <row r="146" ht="15.75" customHeight="1"/>
     <row r="147" ht="15.75" customHeight="1"/>
@@ -7220,19 +8160,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s">
         <v>38</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>39</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>40</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>41</v>
-      </c>
-      <c r="E1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -7243,13 +8183,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -7260,13 +8200,13 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -7277,13 +8217,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -7294,13 +8234,13 @@
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -7311,13 +8251,13 @@
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -7328,13 +8268,13 @@
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -7345,13 +8285,13 @@
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -7362,13 +8302,13 @@
         <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -7379,13 +8319,13 @@
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -7396,13 +8336,13 @@
         <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -8410,19 +9350,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" t="s">
         <v>101</v>
-      </c>
-      <c r="C1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E1" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -8430,13 +9370,13 @@
         <v>531494</v>
       </c>
       <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" t="s">
         <v>47</v>
-      </c>
-      <c r="C2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" t="s">
-        <v>49</v>
       </c>
       <c r="E2">
         <v>919564348</v>
@@ -8447,13 +9387,13 @@
         <v>531503</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="E3" s="2">
         <v>919561527</v>
@@ -8464,13 +9404,13 @@
         <v>531384</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E4" s="2">
         <v>919561950</v>
@@ -8481,13 +9421,13 @@
         <v>533707</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>63</v>
       </c>
       <c r="E5" s="2">
         <v>919571235</v>
@@ -8498,13 +9438,13 @@
         <v>531507</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="E6" s="2">
         <v>919564693</v>
@@ -9514,19 +10454,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -9540,10 +10480,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -9557,10 +10497,10 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -9574,10 +10514,10 @@
         <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -9591,10 +10531,10 @@
         <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -9608,10 +10548,10 @@
         <v>5</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -9625,10 +10565,10 @@
         <v>1</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -9642,10 +10582,10 @@
         <v>2</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -9659,10 +10599,10 @@
         <v>3</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -9676,10 +10616,10 @@
         <v>4</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -9693,10 +10633,10 @@
         <v>5</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -9710,10 +10650,10 @@
         <v>1</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -9727,10 +10667,10 @@
         <v>2</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -9744,10 +10684,10 @@
         <v>3</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -9761,10 +10701,10 @@
         <v>4</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" customHeight="1">
@@ -9778,10 +10718,10 @@
         <v>5</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1">
@@ -9795,10 +10735,10 @@
         <v>1</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1">
@@ -9812,10 +10752,10 @@
         <v>2</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1">
@@ -9829,10 +10769,10 @@
         <v>3</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1">
@@ -9846,10 +10786,10 @@
         <v>4</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1">
@@ -9863,10 +10803,10 @@
         <v>5</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1">
@@ -9880,10 +10820,10 @@
         <v>1</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1">
@@ -9897,10 +10837,10 @@
         <v>2</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1">
@@ -9914,10 +10854,10 @@
         <v>3</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1">
@@ -9931,10 +10871,10 @@
         <v>4</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1">
@@ -9948,10 +10888,10 @@
         <v>5</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
added seed data for student
</commit_message>
<xml_diff>
--- a/Docs/Project05.xlsx
+++ b/Docs/Project05.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S531494\Documents\44663\Project\Masters\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S531384\Documents\Masters\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB8AF919-0DFE-4A4F-A1DF-64948A6CB87F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Degree" sheetId="1" r:id="rId1"/>
@@ -20,12 +21,19 @@
     <sheet name="Student" sheetId="6" r:id="rId6"/>
     <sheet name="StudentTerm" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="106">
   <si>
     <t>RequirementID</t>
   </si>
@@ -341,11 +349,14 @@
   <si>
     <t>new DegreePlanTermRequirement {</t>
   </si>
+  <si>
+    <t>new Student{</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -683,7 +694,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -1810,10 +1821,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="F2" sqref="F2:F14"/>
     </sheetView>
   </sheetViews>
@@ -3106,7 +3117,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4618,11 +4629,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView topLeftCell="E15" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -4727,6 +4738,10 @@
       <c r="F4" t="s">
         <v>95</v>
       </c>
+      <c r="G4" t="str">
+        <f>E4&amp;$A$1&amp;"="&amp;$A$4&amp;","&amp;$B$1&amp;"="&amp;$B$4&amp;","&amp;$C$1&amp;"="&amp;$C$4&amp;","&amp;$D$1&amp;"="&amp;$D$4&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=3,DegreePlanID=20,TermID=1,RequirementID=542},</v>
+      </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="2">
@@ -4747,6 +4762,10 @@
       <c r="F5" t="s">
         <v>95</v>
       </c>
+      <c r="G5" t="str">
+        <f t="shared" ref="G4:G67" si="0">E5&amp;$A$1&amp;"="&amp;$A$3&amp;","&amp;$B$1&amp;"="&amp;$B$3&amp;","&amp;$C$1&amp;"="&amp;$C$3&amp;","&amp;$D$1&amp;"="&amp;$D$3&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6">
@@ -4767,6 +4786,10 @@
       <c r="F6" t="s">
         <v>95</v>
       </c>
+      <c r="G6" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="2">
@@ -4787,6 +4810,10 @@
       <c r="F7" t="s">
         <v>95</v>
       </c>
+      <c r="G7" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8">
@@ -4807,6 +4834,10 @@
       <c r="F8" t="s">
         <v>95</v>
       </c>
+      <c r="G8" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="2">
@@ -4827,6 +4858,10 @@
       <c r="F9" t="s">
         <v>95</v>
       </c>
+      <c r="G9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10">
@@ -4847,6 +4882,10 @@
       <c r="F10" t="s">
         <v>95</v>
       </c>
+      <c r="G10" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="2">
@@ -4867,6 +4906,10 @@
       <c r="F11" t="s">
         <v>95</v>
       </c>
+      <c r="G11" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12">
@@ -4887,6 +4930,10 @@
       <c r="F12" t="s">
         <v>95</v>
       </c>
+      <c r="G12" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="2">
@@ -4907,6 +4954,10 @@
       <c r="F13" t="s">
         <v>95</v>
       </c>
+      <c r="G13" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14">
@@ -4927,6 +4978,10 @@
       <c r="F14" t="s">
         <v>95</v>
       </c>
+      <c r="G14" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="2">
@@ -4947,6 +5002,10 @@
       <c r="F15" t="s">
         <v>95</v>
       </c>
+      <c r="G15" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16">
@@ -4967,8 +5026,12 @@
       <c r="F16" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="G16" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -4987,8 +5050,12 @@
       <c r="F17" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="G17" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18">
         <v>17</v>
       </c>
@@ -5007,8 +5074,12 @@
       <c r="F18" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="G18" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -5027,8 +5098,12 @@
       <c r="F19" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="G19" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20">
         <v>19</v>
       </c>
@@ -5047,8 +5122,12 @@
       <c r="F20" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G20" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" customHeight="1">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -5067,8 +5146,12 @@
       <c r="F21" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G21" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" customHeight="1">
       <c r="A22">
         <v>21</v>
       </c>
@@ -5087,8 +5170,12 @@
       <c r="F22" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G22" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" customHeight="1">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -5107,8 +5194,12 @@
       <c r="F23" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G23" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" customHeight="1">
       <c r="A24">
         <v>23</v>
       </c>
@@ -5127,8 +5218,12 @@
       <c r="F24" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G24" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" customHeight="1">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -5147,8 +5242,12 @@
       <c r="F25" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G25" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" customHeight="1">
       <c r="A26">
         <v>25</v>
       </c>
@@ -5167,8 +5266,12 @@
       <c r="F26" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G26" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" customHeight="1">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -5187,8 +5290,12 @@
       <c r="F27" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G27" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" customHeight="1">
       <c r="A28">
         <v>27</v>
       </c>
@@ -5207,8 +5314,12 @@
       <c r="F28" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G28" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" customHeight="1">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -5227,8 +5338,12 @@
       <c r="F29" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G29" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="15.75" customHeight="1">
       <c r="A30">
         <v>29</v>
       </c>
@@ -5247,8 +5362,12 @@
       <c r="F30" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G30" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="15.75" customHeight="1">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -5267,8 +5386,12 @@
       <c r="F31" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G31" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="15.75" customHeight="1">
       <c r="A32">
         <v>31</v>
       </c>
@@ -5287,8 +5410,12 @@
       <c r="F32" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G32" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="15.75" customHeight="1">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -5307,8 +5434,12 @@
       <c r="F33" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G33" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="15.75" customHeight="1">
       <c r="A34">
         <v>33</v>
       </c>
@@ -5327,8 +5458,12 @@
       <c r="F34" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G34" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="15.75" customHeight="1">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -5347,8 +5482,12 @@
       <c r="F35" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G35" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="15.75" customHeight="1">
       <c r="A36">
         <v>35</v>
       </c>
@@ -5367,8 +5506,12 @@
       <c r="F36" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G36" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="15.75" customHeight="1">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -5387,8 +5530,12 @@
       <c r="F37" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G37" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="15.75" customHeight="1">
       <c r="A38">
         <v>37</v>
       </c>
@@ -5407,8 +5554,12 @@
       <c r="F38" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G38" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="15.75" customHeight="1">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -5427,8 +5578,12 @@
       <c r="F39" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G39" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="15.75" customHeight="1">
       <c r="A40">
         <v>39</v>
       </c>
@@ -5447,8 +5602,12 @@
       <c r="F40" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G40" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="15.75" customHeight="1">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -5467,8 +5626,12 @@
       <c r="F41" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G41" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="15.75" customHeight="1">
       <c r="A42">
         <v>41</v>
       </c>
@@ -5487,8 +5650,12 @@
       <c r="F42" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G42" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="15.75" customHeight="1">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -5507,8 +5674,12 @@
       <c r="F43" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G43" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="15.75" customHeight="1">
       <c r="A44">
         <v>43</v>
       </c>
@@ -5527,8 +5698,12 @@
       <c r="F44" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G44" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="15.75" customHeight="1">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -5547,8 +5722,12 @@
       <c r="F45" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G45" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="15.75" customHeight="1">
       <c r="A46">
         <v>45</v>
       </c>
@@ -5567,8 +5746,12 @@
       <c r="F46" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G46" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="15.75" customHeight="1">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -5587,8 +5770,12 @@
       <c r="F47" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G47" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="15.75" customHeight="1">
       <c r="A48">
         <v>47</v>
       </c>
@@ -5607,8 +5794,12 @@
       <c r="F48" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G48" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="15.75" customHeight="1">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -5627,8 +5818,12 @@
       <c r="F49" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G49" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="15.75" customHeight="1">
       <c r="A50">
         <v>49</v>
       </c>
@@ -5647,8 +5842,12 @@
       <c r="F50" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G50" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="15.75" customHeight="1">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -5667,8 +5866,12 @@
       <c r="F51" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G51" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="15.75" customHeight="1">
       <c r="A52">
         <v>51</v>
       </c>
@@ -5687,8 +5890,12 @@
       <c r="F52" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G52" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="15.75" customHeight="1">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -5707,8 +5914,12 @@
       <c r="F53" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G53" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="15.75" customHeight="1">
       <c r="A54">
         <v>53</v>
       </c>
@@ -5727,8 +5938,12 @@
       <c r="F54" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G54" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="15.75" customHeight="1">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -5747,8 +5962,12 @@
       <c r="F55" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G55" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="15.75" customHeight="1">
       <c r="A56">
         <v>55</v>
       </c>
@@ -5767,8 +5986,12 @@
       <c r="F56" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G56" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="15.75" customHeight="1">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -5787,8 +6010,12 @@
       <c r="F57" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G57" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="15.75" customHeight="1">
       <c r="A58">
         <v>57</v>
       </c>
@@ -5807,8 +6034,12 @@
       <c r="F58" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G58" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="15.75" customHeight="1">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -5827,8 +6058,12 @@
       <c r="F59" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G59" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="15.75" customHeight="1">
       <c r="A60">
         <v>59</v>
       </c>
@@ -5847,8 +6082,12 @@
       <c r="F60" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G60" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="15.75" customHeight="1">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -5867,8 +6106,12 @@
       <c r="F61" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G61" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="15.75" customHeight="1">
       <c r="A62">
         <v>61</v>
       </c>
@@ -5887,8 +6130,12 @@
       <c r="F62" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G62" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="15.75" customHeight="1">
       <c r="A63" s="2">
         <v>62</v>
       </c>
@@ -5907,8 +6154,12 @@
       <c r="F63" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G63" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="15.75" customHeight="1">
       <c r="A64">
         <v>63</v>
       </c>
@@ -5927,8 +6178,12 @@
       <c r="F64" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G64" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="15.75" customHeight="1">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -5947,8 +6202,12 @@
       <c r="F65" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G65" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="15.75" customHeight="1">
       <c r="A66">
         <v>65</v>
       </c>
@@ -5967,8 +6226,12 @@
       <c r="F66" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G66" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="15.75" customHeight="1">
       <c r="A67" s="2">
         <v>66</v>
       </c>
@@ -5987,8 +6250,12 @@
       <c r="F67" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G67" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="15.75" customHeight="1">
       <c r="A68">
         <v>67</v>
       </c>
@@ -6007,8 +6274,12 @@
       <c r="F68" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G68" t="str">
+        <f t="shared" ref="G68:G131" si="1">E68&amp;$A$1&amp;"="&amp;$A$3&amp;","&amp;$B$1&amp;"="&amp;$B$3&amp;","&amp;$C$1&amp;"="&amp;$C$3&amp;","&amp;$D$1&amp;"="&amp;$D$3&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="15.75" customHeight="1">
       <c r="A69" s="2">
         <v>68</v>
       </c>
@@ -6027,8 +6298,12 @@
       <c r="F69" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G69" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="15.75" customHeight="1">
       <c r="A70">
         <v>69</v>
       </c>
@@ -6047,8 +6322,12 @@
       <c r="F70" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G70" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="15.75" customHeight="1">
       <c r="A71" s="2">
         <v>70</v>
       </c>
@@ -6067,8 +6346,12 @@
       <c r="F71" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G71" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="15.75" customHeight="1">
       <c r="A72">
         <v>71</v>
       </c>
@@ -6087,8 +6370,12 @@
       <c r="F72" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G72" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="15.75" customHeight="1">
       <c r="A73" s="2">
         <v>72</v>
       </c>
@@ -6107,8 +6394,12 @@
       <c r="F73" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G73" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="15.75" customHeight="1">
       <c r="A74">
         <v>73</v>
       </c>
@@ -6127,8 +6418,12 @@
       <c r="F74" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G74" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="15.75" customHeight="1">
       <c r="A75" s="2">
         <v>74</v>
       </c>
@@ -6147,8 +6442,12 @@
       <c r="F75" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G75" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="15.75" customHeight="1">
       <c r="A76">
         <v>75</v>
       </c>
@@ -6167,8 +6466,12 @@
       <c r="F76" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G76" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="15.75" customHeight="1">
       <c r="A77" s="2">
         <v>76</v>
       </c>
@@ -6187,8 +6490,12 @@
       <c r="F77" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G77" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="15.75" customHeight="1">
       <c r="A78">
         <v>77</v>
       </c>
@@ -6207,8 +6514,12 @@
       <c r="F78" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G78" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="15.75" customHeight="1">
       <c r="A79" s="2">
         <v>78</v>
       </c>
@@ -6227,8 +6538,12 @@
       <c r="F79" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G79" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="15.75" customHeight="1">
       <c r="A80">
         <v>79</v>
       </c>
@@ -6247,8 +6562,12 @@
       <c r="F80" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G80" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="15.75" customHeight="1">
       <c r="A81" s="2">
         <v>80</v>
       </c>
@@ -6267,8 +6586,12 @@
       <c r="F81" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G81" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="15.75" customHeight="1">
       <c r="A82">
         <v>81</v>
       </c>
@@ -6287,8 +6610,12 @@
       <c r="F82" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G82" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="15.75" customHeight="1">
       <c r="A83" s="2">
         <v>82</v>
       </c>
@@ -6307,8 +6634,12 @@
       <c r="F83" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G83" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="15.75" customHeight="1">
       <c r="A84">
         <v>83</v>
       </c>
@@ -6327,8 +6658,12 @@
       <c r="F84" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G84" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="15.75" customHeight="1">
       <c r="A85" s="2">
         <v>84</v>
       </c>
@@ -6347,8 +6682,12 @@
       <c r="F85" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G85" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="15.75" customHeight="1">
       <c r="A86">
         <v>85</v>
       </c>
@@ -6367,8 +6706,12 @@
       <c r="F86" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G86" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="15.75" customHeight="1">
       <c r="A87" s="2">
         <v>86</v>
       </c>
@@ -6387,8 +6730,12 @@
       <c r="F87" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G87" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="15.75" customHeight="1">
       <c r="A88">
         <v>87</v>
       </c>
@@ -6407,8 +6754,12 @@
       <c r="F88" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G88" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="15.75" customHeight="1">
       <c r="A89" s="2">
         <v>88</v>
       </c>
@@ -6427,8 +6778,12 @@
       <c r="F89" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G89" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="15.75" customHeight="1">
       <c r="A90">
         <v>89</v>
       </c>
@@ -6447,8 +6802,12 @@
       <c r="F90" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G90" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" ht="15.75" customHeight="1">
       <c r="A91" s="2">
         <v>90</v>
       </c>
@@ -6467,8 +6826,12 @@
       <c r="F91" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G91" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" ht="15.75" customHeight="1">
       <c r="A92">
         <v>91</v>
       </c>
@@ -6487,8 +6850,12 @@
       <c r="F92" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G92" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" ht="15.75" customHeight="1">
       <c r="A93" s="2">
         <v>92</v>
       </c>
@@ -6507,8 +6874,12 @@
       <c r="F93" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G93" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" ht="15.75" customHeight="1">
       <c r="A94">
         <v>93</v>
       </c>
@@ -6527,8 +6898,12 @@
       <c r="F94" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G94" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" ht="15.75" customHeight="1">
       <c r="A95" s="2">
         <v>94</v>
       </c>
@@ -6547,8 +6922,12 @@
       <c r="F95" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G95" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" ht="15.75" customHeight="1">
       <c r="A96">
         <v>95</v>
       </c>
@@ -6567,8 +6946,12 @@
       <c r="F96" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G96" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" ht="15.75" customHeight="1">
       <c r="A97" s="2">
         <v>96</v>
       </c>
@@ -6587,8 +6970,12 @@
       <c r="F97" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G97" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" ht="15.75" customHeight="1">
       <c r="A98">
         <v>97</v>
       </c>
@@ -6607,8 +6994,12 @@
       <c r="F98" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G98" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" ht="15.75" customHeight="1">
       <c r="A99" s="2">
         <v>98</v>
       </c>
@@ -6627,8 +7018,12 @@
       <c r="F99" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G99" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" ht="15.75" customHeight="1">
       <c r="A100">
         <v>99</v>
       </c>
@@ -6647,8 +7042,12 @@
       <c r="F100" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G100" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" ht="15.75" customHeight="1">
       <c r="A101" s="2">
         <v>100</v>
       </c>
@@ -6667,8 +7066,12 @@
       <c r="F101" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="102" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G101" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" ht="15.75" customHeight="1">
       <c r="A102">
         <v>101</v>
       </c>
@@ -6687,8 +7090,12 @@
       <c r="F102" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="103" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G102" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" ht="15.75" customHeight="1">
       <c r="A103" s="2">
         <v>102</v>
       </c>
@@ -6707,8 +7114,12 @@
       <c r="F103" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="104" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G103" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" ht="15.75" customHeight="1">
       <c r="A104">
         <v>103</v>
       </c>
@@ -6727,8 +7138,12 @@
       <c r="F104" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="105" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G104" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" ht="15.75" customHeight="1">
       <c r="A105" s="2">
         <v>104</v>
       </c>
@@ -6747,8 +7162,12 @@
       <c r="F105" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="106" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G105" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" ht="15.75" customHeight="1">
       <c r="A106">
         <v>105</v>
       </c>
@@ -6767,8 +7186,12 @@
       <c r="F106" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="107" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G106" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" ht="15.75" customHeight="1">
       <c r="A107" s="2">
         <v>106</v>
       </c>
@@ -6787,8 +7210,12 @@
       <c r="F107" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="108" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G107" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" ht="15.75" customHeight="1">
       <c r="A108">
         <v>107</v>
       </c>
@@ -6807,8 +7234,12 @@
       <c r="F108" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="109" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G108" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" ht="15.75" customHeight="1">
       <c r="A109" s="2">
         <v>108</v>
       </c>
@@ -6827,8 +7258,12 @@
       <c r="F109" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="110" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G109" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" ht="15.75" customHeight="1">
       <c r="A110">
         <v>109</v>
       </c>
@@ -6847,8 +7282,12 @@
       <c r="F110" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="111" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G110" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" ht="15.75" customHeight="1">
       <c r="A111" s="2">
         <v>110</v>
       </c>
@@ -6867,8 +7306,12 @@
       <c r="F111" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="112" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G111" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" ht="15.75" customHeight="1">
       <c r="A112">
         <v>111</v>
       </c>
@@ -6887,8 +7330,12 @@
       <c r="F112" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="113" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G112" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" ht="15.75" customHeight="1">
       <c r="A113" s="2">
         <v>112</v>
       </c>
@@ -6907,8 +7354,12 @@
       <c r="F113" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="114" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G113" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" ht="15.75" customHeight="1">
       <c r="A114">
         <v>113</v>
       </c>
@@ -6927,8 +7378,12 @@
       <c r="F114" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="115" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G114" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" ht="15.75" customHeight="1">
       <c r="A115" s="2">
         <v>114</v>
       </c>
@@ -6947,8 +7402,12 @@
       <c r="F115" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="116" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G115" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" ht="15.75" customHeight="1">
       <c r="A116">
         <v>115</v>
       </c>
@@ -6967,8 +7426,12 @@
       <c r="F116" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="117" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G116" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" ht="15.75" customHeight="1">
       <c r="A117" s="2">
         <v>116</v>
       </c>
@@ -6987,8 +7450,12 @@
       <c r="F117" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="118" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G117" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" ht="15.75" customHeight="1">
       <c r="A118">
         <v>117</v>
       </c>
@@ -7007,8 +7474,12 @@
       <c r="F118" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="119" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G118" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" ht="15.75" customHeight="1">
       <c r="A119" s="2">
         <v>118</v>
       </c>
@@ -7027,8 +7498,12 @@
       <c r="F119" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="120" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G119" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" ht="15.75" customHeight="1">
       <c r="A120">
         <v>119</v>
       </c>
@@ -7047,8 +7522,12 @@
       <c r="F120" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="121" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G120" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" ht="15.75" customHeight="1">
       <c r="A121" s="2">
         <v>120</v>
       </c>
@@ -7067,8 +7546,12 @@
       <c r="F121" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="122" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G121" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" ht="15.75" customHeight="1">
       <c r="A122">
         <v>121</v>
       </c>
@@ -7087,8 +7570,12 @@
       <c r="F122" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="123" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G122" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" ht="15.75" customHeight="1">
       <c r="A123" s="2">
         <v>122</v>
       </c>
@@ -7107,8 +7594,12 @@
       <c r="F123" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="124" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G123" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" ht="15.75" customHeight="1">
       <c r="A124">
         <v>123</v>
       </c>
@@ -7127,8 +7618,12 @@
       <c r="F124" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="125" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G124" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" ht="15.75" customHeight="1">
       <c r="A125" s="2">
         <v>124</v>
       </c>
@@ -7147,8 +7642,12 @@
       <c r="F125" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="126" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G125" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" ht="15.75" customHeight="1">
       <c r="A126">
         <v>125</v>
       </c>
@@ -7167,8 +7666,12 @@
       <c r="F126" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="127" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G126" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" ht="15.75" customHeight="1">
       <c r="A127" s="2">
         <v>126</v>
       </c>
@@ -7187,8 +7690,12 @@
       <c r="F127" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="128" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G127" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" ht="15.75" customHeight="1">
       <c r="A128">
         <v>127</v>
       </c>
@@ -7207,8 +7714,12 @@
       <c r="F128" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="129" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G128" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" ht="15.75" customHeight="1">
       <c r="A129" s="2">
         <v>128</v>
       </c>
@@ -7227,8 +7738,12 @@
       <c r="F129" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="130" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G129" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" ht="15.75" customHeight="1">
       <c r="A130">
         <v>129</v>
       </c>
@@ -7247,8 +7762,12 @@
       <c r="F130" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="131" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G130" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" ht="15.75" customHeight="1">
       <c r="A131" s="2">
         <v>130</v>
       </c>
@@ -7267,20 +7786,24 @@
       <c r="F131" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="132" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="133" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="134" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="135" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="136" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="137" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="138" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="139" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="140" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="141" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="142" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="143" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="144" spans="1:6" ht="15.75" customHeight="1"/>
+      <c r="G131" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="133" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="134" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="135" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="136" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="137" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="138" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="139" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="140" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="141" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="142" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="143" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="144" spans="1:7" ht="15.75" customHeight="1"/>
     <row r="145" ht="15.75" customHeight="1"/>
     <row r="146" ht="15.75" customHeight="1"/>
     <row r="147" ht="15.75" customHeight="1"/>
@@ -8144,7 +8667,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E998"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -9332,11 +9855,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1000"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -9348,7 +9871,7 @@
     <col min="6" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -9364,8 +9887,17 @@
       <c r="E1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>531494</v>
       </c>
@@ -9381,8 +9913,18 @@
       <c r="E2">
         <v>919564348</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H2" t="str">
+        <f>$F$2&amp;$A$1&amp;"="&amp;$A$2&amp;","&amp;$B$1&amp;"="&amp;$B$2&amp;$C$1&amp;"="&amp;$C$2&amp;","&amp;$D$1&amp;"="&amp;$D$2&amp;","&amp;$E$1&amp;"="&amp;$E$2&amp;$G$2</f>
+        <v>new Student{StudentId=531494,FirstName=ShivaniLastName=Busireddy,Snumber=S531494,NineOneNineNumber=919564348},</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="2">
         <v>531503</v>
       </c>
@@ -9398,8 +9940,12 @@
       <c r="E3" s="2">
         <v>919561527</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="H3" t="str">
+        <f>$F$2&amp;$A$1&amp;"="&amp;$A$2&amp;","&amp;$B$1&amp;"="&amp;$B$2&amp;$C$1&amp;"="&amp;$C$2&amp;","&amp;$D$1&amp;"="&amp;$D$2&amp;","&amp;$E$1&amp;"="&amp;$E$2&amp;$G$2</f>
+        <v>new Student{StudentId=531494,FirstName=ShivaniLastName=Busireddy,Snumber=S531494,NineOneNineNumber=919564348},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="2">
         <v>531384</v>
       </c>
@@ -9415,8 +9961,12 @@
       <c r="E4" s="2">
         <v>919561950</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="H4" t="str">
+        <f t="shared" ref="H3:H6" si="0">$F$2&amp;$A$1&amp;"="&amp;$A$2&amp;","&amp;$B$1&amp;"="&amp;$B$2&amp;$C$1&amp;"="&amp;$C$2&amp;","&amp;$D$1&amp;"="&amp;$D$2&amp;","&amp;$E$1&amp;"="&amp;$E$2&amp;$G$2</f>
+        <v>new Student{StudentId=531494,FirstName=ShivaniLastName=Busireddy,Snumber=S531494,NineOneNineNumber=919564348},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="2">
         <v>533707</v>
       </c>
@@ -9432,8 +9982,12 @@
       <c r="E5" s="2">
         <v>919571235</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="H5" t="str">
+        <f t="shared" si="0"/>
+        <v>new Student{StudentId=531494,FirstName=ShivaniLastName=Busireddy,Snumber=S531494,NineOneNineNumber=919564348},</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="2">
         <v>531507</v>
       </c>
@@ -9448,6 +10002,10 @@
       </c>
       <c r="E6" s="2">
         <v>919564693</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="0"/>
+        <v>new Student{StudentId=531494,FirstName=ShivaniLastName=Busireddy,Snumber=S531494,NineOneNineNumber=919564348},</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -10437,10 +10995,10 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E995"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added models in DbInitializer
</commit_message>
<xml_diff>
--- a/Docs/Project05.xlsx
+++ b/Docs/Project05.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S531384\Documents\Masters\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB8AF919-0DFE-4A4F-A1DF-64948A6CB87F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D0E8DF5-29F6-4B99-955C-7D2C002EDFA8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Degree" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="108">
   <si>
     <t>RequirementID</t>
   </si>
@@ -351,6 +351,12 @@
   </si>
   <si>
     <t>new Student{</t>
+  </si>
+  <si>
+    <t>new Models.DegreeRequirement {</t>
+  </si>
+  <si>
+    <t>new Models.DegreePlan{</t>
   </si>
 </sst>
 </file>
@@ -697,8 +703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -788,8 +794,8 @@
         <v>95</v>
       </c>
       <c r="F3" t="str">
-        <f>D3&amp;$A$1&amp;"="&amp;D11&amp;", "&amp;$B$1&amp;"="&amp;$B$3&amp;", "&amp;$C$1&amp;" ="&amp;C3&amp;E3</f>
-        <v>new Degree {DegreeID=, DegreeAbrrev(unique,max 6 characters)=ACS+DB, DegreeName(unique, max 20 characters) =MS ACS +DB},</v>
+        <f>D3&amp;$A$1&amp;"="&amp;A3&amp;", "&amp;$B$1&amp;"="&amp;$B$3&amp;", "&amp;$C$1&amp;" ="&amp;C3&amp;E3</f>
+        <v>new Degree {DegreeID=2, DegreeAbrrev(unique,max 6 characters)=ACS+DB, DegreeName(unique, max 20 characters) =MS ACS +DB},</v>
       </c>
     </row>
     <row r="4" spans="1:26">
@@ -1825,7 +1831,7 @@
   <dimension ref="A1:F1000"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F14"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1834,7 +1840,9 @@
     <col min="2" max="2" width="50.140625" customWidth="1"/>
     <col min="3" max="3" width="43.140625" customWidth="1"/>
     <col min="4" max="4" width="29.7109375" customWidth="1"/>
-    <col min="5" max="26" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="101.140625" customWidth="1"/>
+    <col min="7" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1874,8 +1882,8 @@
         <v>95</v>
       </c>
       <c r="F2" t="str">
-        <f>D2&amp;$A$1&amp;"="&amp;$A$2&amp;","&amp;$B$1&amp;"="&amp;$B$2&amp;","&amp;$C$1&amp;"="&amp;$C$2&amp;$E$2</f>
-        <v>new Requirement {RequirementID=460,RequirementAbbrev(unique,max 6)=DB,RequirementName(unique, max 20)=44-460 Database},</v>
+        <f>Student!H:H</f>
+        <v>new Student{StudentId=531494,FirstName=Shivani,LastName=Busireddy,Snumber=S531494,NineOneNineNumber=919564348},</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -3118,10 +3126,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C1000"/>
+  <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="B40" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3129,10 +3137,11 @@
     <col min="1" max="1" width="22.85546875" customWidth="1"/>
     <col min="2" max="2" width="28.7109375" customWidth="1"/>
     <col min="3" max="3" width="29.7109375" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="4" max="4" width="34.5703125" customWidth="1"/>
+    <col min="5" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>96</v>
       </c>
@@ -3142,8 +3151,17 @@
       <c r="C1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3153,8 +3171,18 @@
       <c r="C2">
         <v>460</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F2" t="str">
+        <f>D2&amp;$A$1&amp;"="&amp;A2&amp;","&amp;$B$1&amp;"="&amp;B2&amp;","&amp;$C$1&amp;"="&amp;C2&amp;E3</f>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=1,DegreeID=1,RequirementID=460},</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3164,8 +3192,18 @@
       <c r="C3">
         <v>356</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F49" si="0">D3&amp;$A$1&amp;"="&amp;A3&amp;","&amp;$B$1&amp;"="&amp;B3&amp;","&amp;$C$1&amp;"="&amp;C3&amp;E4</f>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=2,DegreeID=1,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3175,8 +3213,18 @@
       <c r="C4">
         <v>542</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=3,DegreeID=1,RequirementID=542},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3186,8 +3234,18 @@
       <c r="C5">
         <v>563</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5" t="s">
+        <v>106</v>
+      </c>
+      <c r="E5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=4,DegreeID=1,RequirementID=563},</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3197,8 +3255,18 @@
       <c r="C6">
         <v>560</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6" t="s">
+        <v>106</v>
+      </c>
+      <c r="E6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=5,DegreeID=1,RequirementID=560},</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3208,8 +3276,18 @@
       <c r="C7">
         <v>555</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7" t="s">
+        <v>106</v>
+      </c>
+      <c r="E7" t="s">
+        <v>95</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=6,DegreeID=1,RequirementID=555},</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3219,8 +3297,18 @@
       <c r="C8">
         <v>618</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8" t="s">
+        <v>106</v>
+      </c>
+      <c r="E8" t="s">
+        <v>95</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=7,DegreeID=1,RequirementID=618},</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3230,8 +3318,18 @@
       <c r="C9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="D9" t="s">
+        <v>106</v>
+      </c>
+      <c r="E9" t="s">
+        <v>95</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=8,DegreeID=1,RequirementID=1},</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3241,8 +3339,18 @@
       <c r="C10">
         <v>664</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="D10" t="s">
+        <v>106</v>
+      </c>
+      <c r="E10" t="s">
+        <v>95</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=9,DegreeID=1,RequirementID=664},</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3252,8 +3360,18 @@
       <c r="C11">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="D11" t="s">
+        <v>106</v>
+      </c>
+      <c r="E11" t="s">
+        <v>95</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=10,DegreeID=1,RequirementID=10},</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3263,8 +3381,18 @@
       <c r="C12">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="D12" t="s">
+        <v>106</v>
+      </c>
+      <c r="E12" t="s">
+        <v>95</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=11,DegreeID=1,RequirementID=20},</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3274,8 +3402,18 @@
       <c r="C13">
         <v>691</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="D13" t="s">
+        <v>106</v>
+      </c>
+      <c r="E13" t="s">
+        <v>95</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=12,DegreeID=1,RequirementID=691},</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3285,8 +3423,18 @@
       <c r="C14">
         <v>692</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="D14" t="s">
+        <v>106</v>
+      </c>
+      <c r="E14" t="s">
+        <v>95</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=13,DegreeID=1,RequirementID=692},</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3296,8 +3444,18 @@
       <c r="C15">
         <v>460</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="D15" t="s">
+        <v>106</v>
+      </c>
+      <c r="E15" t="s">
+        <v>95</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=14,DegreeID=2,RequirementID=460},</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3307,8 +3465,18 @@
       <c r="C16">
         <v>542</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="D16" t="s">
+        <v>106</v>
+      </c>
+      <c r="E16" t="s">
+        <v>95</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=15,DegreeID=2,RequirementID=542},</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3318,8 +3486,18 @@
       <c r="C17">
         <v>563</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="D17" t="s">
+        <v>106</v>
+      </c>
+      <c r="E17" t="s">
+        <v>95</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=16,DegreeID=2,RequirementID=563},</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3329,8 +3507,18 @@
       <c r="C18">
         <v>560</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="D18" t="s">
+        <v>106</v>
+      </c>
+      <c r="E18" t="s">
+        <v>95</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=17,DegreeID=2,RequirementID=560},</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3340,8 +3528,18 @@
       <c r="C19">
         <v>555</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="D19" t="s">
+        <v>106</v>
+      </c>
+      <c r="E19" t="s">
+        <v>95</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=18,DegreeID=2,RequirementID=555},</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3351,8 +3549,18 @@
       <c r="C20">
         <v>618</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="15.75" customHeight="1">
+      <c r="D20" t="s">
+        <v>106</v>
+      </c>
+      <c r="E20" t="s">
+        <v>95</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=19,DegreeID=2,RequirementID=618},</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" customHeight="1">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3362,8 +3570,18 @@
       <c r="C21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="15.75" customHeight="1">
+      <c r="D21" t="s">
+        <v>106</v>
+      </c>
+      <c r="E21" t="s">
+        <v>95</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=20,DegreeID=2,RequirementID=1},</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" customHeight="1">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3373,8 +3591,18 @@
       <c r="C22">
         <v>664</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="15.75" customHeight="1">
+      <c r="D22" t="s">
+        <v>106</v>
+      </c>
+      <c r="E22" t="s">
+        <v>95</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=21,DegreeID=2,RequirementID=664},</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" customHeight="1">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3384,8 +3612,18 @@
       <c r="C23">
         <v>10</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="15.75" customHeight="1">
+      <c r="D23" t="s">
+        <v>106</v>
+      </c>
+      <c r="E23" t="s">
+        <v>95</v>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=22,DegreeID=2,RequirementID=10},</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15.75" customHeight="1">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3395,8 +3633,18 @@
       <c r="C24">
         <v>20</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="15.75" customHeight="1">
+      <c r="D24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E24" t="s">
+        <v>95</v>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=23,DegreeID=2,RequirementID=20},</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" customHeight="1">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3406,8 +3654,18 @@
       <c r="C25">
         <v>691</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="15.75" customHeight="1">
+      <c r="D25" t="s">
+        <v>106</v>
+      </c>
+      <c r="E25" t="s">
+        <v>95</v>
+      </c>
+      <c r="F25" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=24,DegreeID=2,RequirementID=691},</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" customHeight="1">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3417,8 +3675,18 @@
       <c r="C26">
         <v>692</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="15.75" customHeight="1">
+      <c r="D26" t="s">
+        <v>106</v>
+      </c>
+      <c r="E26" t="s">
+        <v>95</v>
+      </c>
+      <c r="F26" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=25,DegreeID=2,RequirementID=692},</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15.75" customHeight="1">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3428,8 +3696,18 @@
       <c r="C27">
         <v>356</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="15.75" customHeight="1">
+      <c r="D27" t="s">
+        <v>106</v>
+      </c>
+      <c r="E27" t="s">
+        <v>95</v>
+      </c>
+      <c r="F27" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=26,DegreeID=3,RequirementID=356},</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15.75" customHeight="1">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3439,8 +3717,18 @@
       <c r="C28">
         <v>542</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="15.75" customHeight="1">
+      <c r="D28" t="s">
+        <v>106</v>
+      </c>
+      <c r="E28" t="s">
+        <v>95</v>
+      </c>
+      <c r="F28" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=27,DegreeID=3,RequirementID=542},</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15.75" customHeight="1">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3450,8 +3738,18 @@
       <c r="C29">
         <v>563</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="15.75" customHeight="1">
+      <c r="D29" t="s">
+        <v>106</v>
+      </c>
+      <c r="E29" t="s">
+        <v>95</v>
+      </c>
+      <c r="F29" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=28,DegreeID=3,RequirementID=563},</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15.75" customHeight="1">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3461,8 +3759,18 @@
       <c r="C30">
         <v>560</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="15.75" customHeight="1">
+      <c r="D30" t="s">
+        <v>106</v>
+      </c>
+      <c r="E30" t="s">
+        <v>95</v>
+      </c>
+      <c r="F30" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=29,DegreeID=3,RequirementID=560},</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="15.75" customHeight="1">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3472,8 +3780,18 @@
       <c r="C31">
         <v>555</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" ht="15.75" customHeight="1">
+      <c r="D31" t="s">
+        <v>106</v>
+      </c>
+      <c r="E31" t="s">
+        <v>95</v>
+      </c>
+      <c r="F31" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=30,DegreeID=3,RequirementID=555},</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="15.75" customHeight="1">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3483,8 +3801,18 @@
       <c r="C32">
         <v>618</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" ht="15.75" customHeight="1">
+      <c r="D32" t="s">
+        <v>106</v>
+      </c>
+      <c r="E32" t="s">
+        <v>95</v>
+      </c>
+      <c r="F32" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=31,DegreeID=3,RequirementID=618},</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="15.75" customHeight="1">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3494,8 +3822,18 @@
       <c r="C33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="15.75" customHeight="1">
+      <c r="D33" t="s">
+        <v>106</v>
+      </c>
+      <c r="E33" t="s">
+        <v>95</v>
+      </c>
+      <c r="F33" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=32,DegreeID=3,RequirementID=1},</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="15.75" customHeight="1">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3505,8 +3843,18 @@
       <c r="C34">
         <v>664</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" ht="15.75" customHeight="1">
+      <c r="D34" t="s">
+        <v>106</v>
+      </c>
+      <c r="E34" t="s">
+        <v>95</v>
+      </c>
+      <c r="F34" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=33,DegreeID=3,RequirementID=664},</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="15.75" customHeight="1">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3516,8 +3864,18 @@
       <c r="C35">
         <v>10</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" ht="15.75" customHeight="1">
+      <c r="D35" t="s">
+        <v>106</v>
+      </c>
+      <c r="E35" t="s">
+        <v>95</v>
+      </c>
+      <c r="F35" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=34,DegreeID=3,RequirementID=10},</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="15.75" customHeight="1">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3527,8 +3885,18 @@
       <c r="C36">
         <v>20</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" ht="15.75" customHeight="1">
+      <c r="D36" t="s">
+        <v>106</v>
+      </c>
+      <c r="E36" t="s">
+        <v>95</v>
+      </c>
+      <c r="F36" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=35,DegreeID=3,RequirementID=20},</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="15.75" customHeight="1">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3538,8 +3906,18 @@
       <c r="C37">
         <v>691</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" ht="15.75" customHeight="1">
+      <c r="D37" t="s">
+        <v>106</v>
+      </c>
+      <c r="E37" t="s">
+        <v>95</v>
+      </c>
+      <c r="F37" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=36,DegreeID=3,RequirementID=691},</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="15.75" customHeight="1">
       <c r="A38">
         <v>37</v>
       </c>
@@ -3549,8 +3927,18 @@
       <c r="C38">
         <v>692</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" ht="15.75" customHeight="1">
+      <c r="D38" t="s">
+        <v>106</v>
+      </c>
+      <c r="E38" t="s">
+        <v>95</v>
+      </c>
+      <c r="F38" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=37,DegreeID=3,RequirementID=692},</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="15.75" customHeight="1">
       <c r="A39">
         <v>38</v>
       </c>
@@ -3560,8 +3948,18 @@
       <c r="C39">
         <v>542</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" ht="15.75" customHeight="1">
+      <c r="D39" t="s">
+        <v>106</v>
+      </c>
+      <c r="E39" t="s">
+        <v>95</v>
+      </c>
+      <c r="F39" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=38,DegreeID=4,RequirementID=542},</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="15.75" customHeight="1">
       <c r="A40">
         <v>39</v>
       </c>
@@ -3571,8 +3969,18 @@
       <c r="C40">
         <v>563</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" ht="15.75" customHeight="1">
+      <c r="D40" t="s">
+        <v>106</v>
+      </c>
+      <c r="E40" t="s">
+        <v>95</v>
+      </c>
+      <c r="F40" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=39,DegreeID=4,RequirementID=563},</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="15.75" customHeight="1">
       <c r="A41">
         <v>40</v>
       </c>
@@ -3582,8 +3990,18 @@
       <c r="C41">
         <v>560</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" ht="15.75" customHeight="1">
+      <c r="D41" t="s">
+        <v>106</v>
+      </c>
+      <c r="E41" t="s">
+        <v>95</v>
+      </c>
+      <c r="F41" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=40,DegreeID=4,RequirementID=560},</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="15.75" customHeight="1">
       <c r="A42">
         <v>41</v>
       </c>
@@ -3593,8 +4011,18 @@
       <c r="C42">
         <v>555</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" ht="15.75" customHeight="1">
+      <c r="D42" t="s">
+        <v>106</v>
+      </c>
+      <c r="E42" t="s">
+        <v>95</v>
+      </c>
+      <c r="F42" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=41,DegreeID=4,RequirementID=555},</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="15.75" customHeight="1">
       <c r="A43">
         <v>42</v>
       </c>
@@ -3604,8 +4032,18 @@
       <c r="C43">
         <v>618</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" ht="15.75" customHeight="1">
+      <c r="D43" t="s">
+        <v>106</v>
+      </c>
+      <c r="E43" t="s">
+        <v>95</v>
+      </c>
+      <c r="F43" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=42,DegreeID=4,RequirementID=618},</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="15.75" customHeight="1">
       <c r="A44">
         <v>43</v>
       </c>
@@ -3615,8 +4053,18 @@
       <c r="C44">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" ht="15.75" customHeight="1">
+      <c r="D44" t="s">
+        <v>106</v>
+      </c>
+      <c r="E44" t="s">
+        <v>95</v>
+      </c>
+      <c r="F44" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=43,DegreeID=4,RequirementID=1},</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="15.75" customHeight="1">
       <c r="A45">
         <v>44</v>
       </c>
@@ -3626,8 +4074,18 @@
       <c r="C45">
         <v>664</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" ht="15.75" customHeight="1">
+      <c r="D45" t="s">
+        <v>106</v>
+      </c>
+      <c r="E45" t="s">
+        <v>95</v>
+      </c>
+      <c r="F45" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=44,DegreeID=4,RequirementID=664},</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="15.75" customHeight="1">
       <c r="A46">
         <v>45</v>
       </c>
@@ -3637,8 +4095,18 @@
       <c r="C46">
         <v>10</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" ht="15.75" customHeight="1">
+      <c r="D46" t="s">
+        <v>106</v>
+      </c>
+      <c r="E46" t="s">
+        <v>95</v>
+      </c>
+      <c r="F46" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=45,DegreeID=4,RequirementID=10},</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="15.75" customHeight="1">
       <c r="A47">
         <v>46</v>
       </c>
@@ -3648,8 +4116,18 @@
       <c r="C47">
         <v>20</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" ht="15.75" customHeight="1">
+      <c r="D47" t="s">
+        <v>106</v>
+      </c>
+      <c r="E47" t="s">
+        <v>95</v>
+      </c>
+      <c r="F47" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=46,DegreeID=4,RequirementID=20},</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="15.75" customHeight="1">
       <c r="A48">
         <v>47</v>
       </c>
@@ -3659,8 +4137,18 @@
       <c r="C48">
         <v>691</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" ht="15.75" customHeight="1">
+      <c r="D48" t="s">
+        <v>106</v>
+      </c>
+      <c r="E48" t="s">
+        <v>95</v>
+      </c>
+      <c r="F48" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=47,DegreeID=4,RequirementID=691},</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="15.75" customHeight="1">
       <c r="A49">
         <v>48</v>
       </c>
@@ -3670,22 +4158,32 @@
       <c r="C49">
         <v>692</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="51" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="52" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="53" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="54" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="55" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="56" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="57" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="58" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="59" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="60" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="61" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="62" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="63" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="64" spans="1:3" ht="15.75" customHeight="1"/>
+      <c r="D49" t="s">
+        <v>106</v>
+      </c>
+      <c r="E49" t="s">
+        <v>95</v>
+      </c>
+      <c r="F49" t="str">
+        <f>D49&amp;$A$1&amp;"="&amp;A49&amp;","&amp;$B$1&amp;"="&amp;B49&amp;","&amp;$C$1&amp;"="&amp;C49&amp;E50</f>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=48,DegreeID=4,RequirementID=692</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="51" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="52" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="53" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="54" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="55" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="56" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="57" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="58" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="59" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="60" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="61" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="62" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="63" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="64" spans="1:6" ht="15.75" customHeight="1"/>
     <row r="65" ht="15.75" customHeight="1"/>
     <row r="66" ht="15.75" customHeight="1"/>
     <row r="67" ht="15.75" customHeight="1"/>
@@ -4632,8 +5130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView topLeftCell="E15" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView topLeftCell="C121" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -4763,8 +5261,8 @@
         <v>95</v>
       </c>
       <c r="G5" t="str">
-        <f t="shared" ref="G4:G67" si="0">E5&amp;$A$1&amp;"="&amp;$A$3&amp;","&amp;$B$1&amp;"="&amp;$B$3&amp;","&amp;$C$1&amp;"="&amp;$C$3&amp;","&amp;$D$1&amp;"="&amp;$D$3&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E5&amp;$A$1&amp;"="&amp;$A$5&amp;","&amp;$B$1&amp;"="&amp;$B$5&amp;","&amp;$C$1&amp;"="&amp;$C$5&amp;","&amp;$D$1&amp;"="&amp;$D$5&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=4,DegreePlanID=20,TermID=1,RequirementID=563},</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -4787,8 +5285,8 @@
         <v>95</v>
       </c>
       <c r="G6" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E6&amp;$A$1&amp;"="&amp;$A$6&amp;","&amp;$B$1&amp;"="&amp;$B$6&amp;","&amp;$C$1&amp;"="&amp;$C$6&amp;","&amp;$D$1&amp;"="&amp;$D$6&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=5,DegreePlanID=20,TermID=2,RequirementID=560},</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -4811,8 +5309,8 @@
         <v>95</v>
       </c>
       <c r="G7" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E7&amp;$A$1&amp;"="&amp;$A$7&amp;","&amp;$B$1&amp;"="&amp;$B$7&amp;","&amp;$C$1&amp;"="&amp;$C$7&amp;","&amp;$D$1&amp;"="&amp;$D$7&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=6,DegreePlanID=20,TermID=2,RequirementID=555},</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -4835,8 +5333,8 @@
         <v>95</v>
       </c>
       <c r="G8" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E8&amp;$A$1&amp;"="&amp;$A$8&amp;","&amp;$B$1&amp;"="&amp;$B$8&amp;","&amp;$C$1&amp;"="&amp;$C$8&amp;","&amp;$D$1&amp;"="&amp;$D$8&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=7,DegreePlanID=20,TermID=2,RequirementID=618},</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -4859,8 +5357,8 @@
         <v>95</v>
       </c>
       <c r="G9" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E9&amp;$A$1&amp;"="&amp;$A$9&amp;","&amp;$B$1&amp;"="&amp;$B$9&amp;","&amp;$C$1&amp;"="&amp;$C$9&amp;","&amp;$D$1&amp;"="&amp;$D$9&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=8,DegreePlanID=20,TermID=3,RequirementID=1},</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -4883,8 +5381,8 @@
         <v>95</v>
       </c>
       <c r="G10" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E10&amp;$A$1&amp;"="&amp;$A$10&amp;","&amp;$B$1&amp;"="&amp;$B$10&amp;","&amp;$C$1&amp;"="&amp;$C$10&amp;","&amp;$D$1&amp;"="&amp;$D$10&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=9,DegreePlanID=20,TermID=3,RequirementID=664},</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -4907,8 +5405,8 @@
         <v>95</v>
       </c>
       <c r="G11" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E11&amp;$A$1&amp;"="&amp;$A$11&amp;","&amp;$B$1&amp;"="&amp;$B$11&amp;","&amp;$C$1&amp;"="&amp;$C$11&amp;","&amp;$D$1&amp;"="&amp;$D$11&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=10,DegreePlanID=20,TermID=3,RequirementID=691},</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -4931,8 +5429,8 @@
         <v>95</v>
       </c>
       <c r="G12" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E12&amp;$A$1&amp;"="&amp;$A$12&amp;","&amp;$B$1&amp;"="&amp;$B$12&amp;","&amp;$C$1&amp;"="&amp;$C$12&amp;","&amp;$D$1&amp;"="&amp;$D$12&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=11,DegreePlanID=20,TermID=4,RequirementID=10},</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -4955,8 +5453,8 @@
         <v>95</v>
       </c>
       <c r="G13" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E13&amp;$A$1&amp;"="&amp;$A$13&amp;","&amp;$B$1&amp;"="&amp;$B$13&amp;","&amp;$C$1&amp;"="&amp;$C$13&amp;","&amp;$D$1&amp;"="&amp;$D$13&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=12,DegreePlanID=20,TermID=4,RequirementID=20},</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -4979,8 +5477,8 @@
         <v>95</v>
       </c>
       <c r="G14" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E14&amp;$A$1&amp;"="&amp;$A$14&amp;","&amp;$B$1&amp;"="&amp;$B$14&amp;","&amp;$C$1&amp;"="&amp;$C$14&amp;","&amp;$D$1&amp;"="&amp;$D$14&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=13,DegreePlanID=20,TermID=5,RequirementID=692},</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -5003,8 +5501,8 @@
         <v>95</v>
       </c>
       <c r="G15" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E15&amp;$A$1&amp;"="&amp;$A$15&amp;","&amp;$B$1&amp;"="&amp;$B$15&amp;","&amp;$C$1&amp;"="&amp;$C$15&amp;","&amp;$D$1&amp;"="&amp;$D$15&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=14,DegreePlanID=21,TermID=1,RequirementID=460},</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -5027,8 +5525,8 @@
         <v>95</v>
       </c>
       <c r="G16" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E16&amp;$A$1&amp;"="&amp;$A$16&amp;","&amp;$B$1&amp;"="&amp;$B$16&amp;","&amp;$C$1&amp;"="&amp;$C$16&amp;","&amp;$D$1&amp;"="&amp;$D$16&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=15,DegreePlanID=21,TermID=1,RequirementID=356},</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -5051,8 +5549,8 @@
         <v>95</v>
       </c>
       <c r="G17" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E17&amp;$A$1&amp;"="&amp;$A$17&amp;","&amp;$B$1&amp;"="&amp;$B$17&amp;","&amp;$C$1&amp;"="&amp;$C$17&amp;","&amp;$D$1&amp;"="&amp;$D$17&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=16,DegreePlanID=21,TermID=1,RequirementID=542},</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -5075,8 +5573,8 @@
         <v>95</v>
       </c>
       <c r="G18" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E18&amp;$A$1&amp;"="&amp;$A$18&amp;","&amp;$B$1&amp;"="&amp;$B$18&amp;","&amp;$C$1&amp;"="&amp;$C$18&amp;","&amp;$D$1&amp;"="&amp;$D$18&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=17,DegreePlanID=21,TermID=1,RequirementID=563},</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -5099,8 +5597,8 @@
         <v>95</v>
       </c>
       <c r="G19" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E19&amp;$A$1&amp;"="&amp;$A$19&amp;","&amp;$B$1&amp;"="&amp;$B$19&amp;","&amp;$C$1&amp;"="&amp;$C$19&amp;","&amp;$D$1&amp;"="&amp;$D$19&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=18,DegreePlanID=21,TermID=2,RequirementID=560},</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -5123,8 +5621,8 @@
         <v>95</v>
       </c>
       <c r="G20" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E20&amp;$A$1&amp;"="&amp;$A$20&amp;","&amp;$B$1&amp;"="&amp;$B$20&amp;","&amp;$C$1&amp;"="&amp;$C$20&amp;","&amp;$D$1&amp;"="&amp;$D$20&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=19,DegreePlanID=21,TermID=2,RequirementID=555},</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1">
@@ -5147,8 +5645,8 @@
         <v>95</v>
       </c>
       <c r="G21" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E21&amp;$A$1&amp;"="&amp;$A$21&amp;","&amp;$B$1&amp;"="&amp;$B$21&amp;","&amp;$C$1&amp;"="&amp;$C$21&amp;","&amp;$D$1&amp;"="&amp;$D$21&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=20,DegreePlanID=21,TermID=2,RequirementID=618},</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1">
@@ -5171,8 +5669,8 @@
         <v>95</v>
       </c>
       <c r="G22" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E22&amp;$A$1&amp;"="&amp;$A$22&amp;","&amp;$B$1&amp;"="&amp;$B$22&amp;","&amp;$C$1&amp;"="&amp;$C$22&amp;","&amp;$D$1&amp;"="&amp;$D$22&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=21,DegreePlanID=21,TermID=4,RequirementID=1},</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1">
@@ -5195,8 +5693,8 @@
         <v>95</v>
       </c>
       <c r="G23" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E23&amp;$A$1&amp;"="&amp;$A$23&amp;","&amp;$B$1&amp;"="&amp;$B$23&amp;","&amp;$C$1&amp;"="&amp;$C$23&amp;","&amp;$D$1&amp;"="&amp;$D$23&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=22,DegreePlanID=21,TermID=4,RequirementID=664},</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1">
@@ -5219,8 +5717,8 @@
         <v>95</v>
       </c>
       <c r="G24" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E24&amp;$A$1&amp;"="&amp;$A$24&amp;","&amp;$B$1&amp;"="&amp;$B$24&amp;","&amp;$C$1&amp;"="&amp;$C$24&amp;","&amp;$D$1&amp;"="&amp;$D$24&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=23,DegreePlanID=21,TermID=4,RequirementID=691},</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1">
@@ -5243,8 +5741,8 @@
         <v>95</v>
       </c>
       <c r="G25" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E25&amp;$A$1&amp;"="&amp;$A$25&amp;","&amp;$B$1&amp;"="&amp;$B$25&amp;","&amp;$C$1&amp;"="&amp;$C$25&amp;","&amp;$D$1&amp;"="&amp;$D$25&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=24,DegreePlanID=21,TermID=5,RequirementID=10},</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1">
@@ -5267,8 +5765,8 @@
         <v>95</v>
       </c>
       <c r="G26" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E26&amp;$A$1&amp;"="&amp;$A$26&amp;","&amp;$B$1&amp;"="&amp;$B$26&amp;","&amp;$C$1&amp;"="&amp;$C$26&amp;","&amp;$D$1&amp;"="&amp;$D$26&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=25,DegreePlanID=21,TermID=5,RequirementID=20},</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1">
@@ -5291,8 +5789,8 @@
         <v>95</v>
       </c>
       <c r="G27" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E27&amp;$A$1&amp;"="&amp;$A$27&amp;","&amp;$B$1&amp;"="&amp;$B$27&amp;","&amp;$C$1&amp;"="&amp;$C$27&amp;","&amp;$D$1&amp;"="&amp;$D$27&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=26,DegreePlanID=21,TermID=5,RequirementID=692},</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1">
@@ -5315,8 +5813,8 @@
         <v>95</v>
       </c>
       <c r="G28" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E28&amp;$A$1&amp;"="&amp;$A$28&amp;","&amp;$B$1&amp;"="&amp;$B$28&amp;","&amp;$C$1&amp;"="&amp;$C$28&amp;","&amp;$D$1&amp;"="&amp;$D$28&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=27,DegreePlanID=12,TermID=1,RequirementID=460},</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1">
@@ -5339,8 +5837,8 @@
         <v>95</v>
       </c>
       <c r="G29" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E29&amp;$A$1&amp;"="&amp;$A$29&amp;","&amp;$B$1&amp;"="&amp;$B$29&amp;","&amp;$C$1&amp;"="&amp;$C$29&amp;","&amp;$D$1&amp;"="&amp;$D$29&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=28,DegreePlanID=12,TermID=1,RequirementID=356},</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1">
@@ -5363,8 +5861,8 @@
         <v>95</v>
       </c>
       <c r="G30" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E30&amp;$A$1&amp;"="&amp;$A$30&amp;","&amp;$B$1&amp;"="&amp;$B$30&amp;","&amp;$C$1&amp;"="&amp;$C$30&amp;","&amp;$D$1&amp;"="&amp;$D$30&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=29,DegreePlanID=12,TermID=1,RequirementID=542},</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1">
@@ -5387,8 +5885,8 @@
         <v>95</v>
       </c>
       <c r="G31" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E31&amp;$A$1&amp;"="&amp;$A$31&amp;","&amp;$B$1&amp;"="&amp;$B$31&amp;","&amp;$C$1&amp;"="&amp;$C$31&amp;","&amp;$D$1&amp;"="&amp;$D$31&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=30,DegreePlanID=12,TermID=1,RequirementID=563},</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="15.75" customHeight="1">
@@ -5411,8 +5909,8 @@
         <v>95</v>
       </c>
       <c r="G32" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E32&amp;$A$1&amp;"="&amp;$A$32&amp;","&amp;$B$1&amp;"="&amp;$B$32&amp;","&amp;$C$1&amp;"="&amp;$C$32&amp;","&amp;$D$1&amp;"="&amp;$D$32&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=31,DegreePlanID=12,TermID=2,RequirementID=560},</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="15.75" customHeight="1">
@@ -5435,8 +5933,8 @@
         <v>95</v>
       </c>
       <c r="G33" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E33&amp;$A$1&amp;"="&amp;$A$33&amp;","&amp;$B$1&amp;"="&amp;$B$33&amp;","&amp;$C$1&amp;"="&amp;$C$33&amp;","&amp;$D$1&amp;"="&amp;$D$33&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=32,DegreePlanID=12,TermID=2,RequirementID=555},</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="15.75" customHeight="1">
@@ -5459,8 +5957,8 @@
         <v>95</v>
       </c>
       <c r="G34" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E34&amp;$A$1&amp;"="&amp;$A$34&amp;","&amp;$B$1&amp;"="&amp;$B$34&amp;","&amp;$C$1&amp;"="&amp;$C$34&amp;","&amp;$D$1&amp;"="&amp;$D$34&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=33,DegreePlanID=12,TermID=2,RequirementID=618},</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="15.75" customHeight="1">
@@ -5483,8 +5981,8 @@
         <v>95</v>
       </c>
       <c r="G35" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E35&amp;$A$1&amp;"="&amp;$A$35&amp;","&amp;$B$1&amp;"="&amp;$B$35&amp;","&amp;$C$1&amp;"="&amp;$C$35&amp;","&amp;$D$1&amp;"="&amp;$D$35&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=34,DegreePlanID=12,TermID=3,RequirementID=1},</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="15.75" customHeight="1">
@@ -5507,8 +6005,8 @@
         <v>95</v>
       </c>
       <c r="G36" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E36&amp;$A$1&amp;"="&amp;$A$36&amp;","&amp;$B$1&amp;"="&amp;$B$36&amp;","&amp;$C$1&amp;"="&amp;$C$36&amp;","&amp;$D$1&amp;"="&amp;$D$36&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=35,DegreePlanID=12,TermID=3,RequirementID=664},</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="15.75" customHeight="1">
@@ -5531,8 +6029,8 @@
         <v>95</v>
       </c>
       <c r="G37" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E37&amp;$A$1&amp;"="&amp;$A$37&amp;","&amp;$B$1&amp;"="&amp;$B$37&amp;","&amp;$C$1&amp;"="&amp;$C$37&amp;","&amp;$D$1&amp;"="&amp;$D$37&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=36,DegreePlanID=12,TermID=4,RequirementID=691},</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="15.75" customHeight="1">
@@ -5555,8 +6053,8 @@
         <v>95</v>
       </c>
       <c r="G38" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E38&amp;$A$1&amp;"="&amp;$A$38&amp;","&amp;$B$1&amp;"="&amp;$B$38&amp;","&amp;$C$1&amp;"="&amp;$C$38&amp;","&amp;$D$1&amp;"="&amp;$D$38&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=37,DegreePlanID=12,TermID=4,RequirementID=10},</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="15.75" customHeight="1">
@@ -5579,8 +6077,8 @@
         <v>95</v>
       </c>
       <c r="G39" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E39&amp;$A$1&amp;"="&amp;$A$39&amp;","&amp;$B$1&amp;"="&amp;$B$39&amp;","&amp;$C$1&amp;"="&amp;$C$39&amp;","&amp;$D$1&amp;"="&amp;$D$39&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=38,DegreePlanID=12,TermID=4,RequirementID=20},</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="15.75" customHeight="1">
@@ -5603,8 +6101,8 @@
         <v>95</v>
       </c>
       <c r="G40" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E40&amp;$A$1&amp;"="&amp;$A$40&amp;","&amp;$B$1&amp;"="&amp;$B$40&amp;","&amp;$C$1&amp;"="&amp;$C$40&amp;","&amp;$D$1&amp;"="&amp;$D$40&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=39,DegreePlanID=12,TermID=5,RequirementID=692},</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="15.75" customHeight="1">
@@ -5627,8 +6125,8 @@
         <v>95</v>
       </c>
       <c r="G41" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E41&amp;$A$1&amp;"="&amp;$A$41&amp;","&amp;$B$1&amp;"="&amp;$B$41&amp;","&amp;$C$1&amp;"="&amp;$C$41&amp;","&amp;$D$1&amp;"="&amp;$D$41&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=40,DegreePlanID=13,TermID=1,RequirementID=460},</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="15.75" customHeight="1">
@@ -5651,8 +6149,8 @@
         <v>95</v>
       </c>
       <c r="G42" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E42&amp;$A$1&amp;"="&amp;$A$42&amp;","&amp;$B$1&amp;"="&amp;$B$42&amp;","&amp;$C$1&amp;"="&amp;$C$42&amp;","&amp;$D$1&amp;"="&amp;$D$42&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=41,DegreePlanID=13,TermID=1,RequirementID=356},</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="15.75" customHeight="1">
@@ -5675,8 +6173,8 @@
         <v>95</v>
       </c>
       <c r="G43" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E43&amp;$A$1&amp;"="&amp;$A$43&amp;","&amp;$B$1&amp;"="&amp;$B$43&amp;","&amp;$C$1&amp;"="&amp;$C$43&amp;","&amp;$D$1&amp;"="&amp;$D$43&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=42,DegreePlanID=13,TermID=1,RequirementID=542},</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="15.75" customHeight="1">
@@ -5699,8 +6197,8 @@
         <v>95</v>
       </c>
       <c r="G44" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E44&amp;$A$1&amp;"="&amp;$A$44&amp;","&amp;$B$1&amp;"="&amp;$B$44&amp;","&amp;$C$1&amp;"="&amp;$C$44&amp;","&amp;$D$1&amp;"="&amp;$D$44&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=43,DegreePlanID=13,TermID=1,RequirementID=563},</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="15.75" customHeight="1">
@@ -5723,8 +6221,8 @@
         <v>95</v>
       </c>
       <c r="G45" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E45&amp;$A$1&amp;"="&amp;$A$45&amp;","&amp;$B$1&amp;"="&amp;$B$45&amp;","&amp;$C$1&amp;"="&amp;$C$45&amp;","&amp;$D$1&amp;"="&amp;$D$45&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=44,DegreePlanID=13,TermID=3,RequirementID=560},</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="15.75" customHeight="1">
@@ -5747,8 +6245,8 @@
         <v>95</v>
       </c>
       <c r="G46" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E46&amp;$A$1&amp;"="&amp;$A$46&amp;","&amp;$B$1&amp;"="&amp;$B$46&amp;","&amp;$C$1&amp;"="&amp;$C$46&amp;","&amp;$D$1&amp;"="&amp;$D$46&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=45,DegreePlanID=13,TermID=3,RequirementID=555},</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="15.75" customHeight="1">
@@ -5771,8 +6269,8 @@
         <v>95</v>
       </c>
       <c r="G47" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E47&amp;$A$1&amp;"="&amp;$A$47&amp;","&amp;$B$1&amp;"="&amp;$B$47&amp;","&amp;$C$1&amp;"="&amp;$C$47&amp;","&amp;$D$1&amp;"="&amp;$D$47&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=46,DegreePlanID=13,TermID=3,RequirementID=618},</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="15.75" customHeight="1">
@@ -5795,8 +6293,8 @@
         <v>95</v>
       </c>
       <c r="G48" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E48&amp;$A$1&amp;"="&amp;$A$48&amp;","&amp;$B$1&amp;"="&amp;$B$48&amp;","&amp;$C$1&amp;"="&amp;$C$48&amp;","&amp;$D$1&amp;"="&amp;$D$48&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=47,DegreePlanID=13,TermID=4,RequirementID=1},</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="15.75" customHeight="1">
@@ -5819,8 +6317,8 @@
         <v>95</v>
       </c>
       <c r="G49" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E49&amp;$A$1&amp;"="&amp;$A$49&amp;","&amp;$B$1&amp;"="&amp;$B$49&amp;","&amp;$C$1&amp;"="&amp;$C$49&amp;","&amp;$D$1&amp;"="&amp;$D$49&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=48,DegreePlanID=13,TermID=4,RequirementID=664},</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="15.75" customHeight="1">
@@ -5843,8 +6341,8 @@
         <v>95</v>
       </c>
       <c r="G50" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E50&amp;$A$1&amp;"="&amp;$A$50&amp;","&amp;$B$1&amp;"="&amp;$B$50&amp;","&amp;$C$1&amp;"="&amp;$C$50&amp;","&amp;$D$1&amp;"="&amp;$D$50&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=49,DegreePlanID=13,TermID=4,RequirementID=691},</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="15.75" customHeight="1">
@@ -5867,8 +6365,8 @@
         <v>95</v>
       </c>
       <c r="G51" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E51&amp;$A$1&amp;"="&amp;$A$51&amp;","&amp;$B$1&amp;"="&amp;$B$51&amp;","&amp;$C$1&amp;"="&amp;$C$51&amp;","&amp;$D$1&amp;"="&amp;$D$51&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=50,DegreePlanID=13,TermID=5,RequirementID=10},</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="15.75" customHeight="1">
@@ -5891,8 +6389,8 @@
         <v>95</v>
       </c>
       <c r="G52" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E52&amp;$A$1&amp;"="&amp;$A$52&amp;","&amp;$B$1&amp;"="&amp;$B$52&amp;","&amp;$C$1&amp; "="&amp;$C$52&amp;","&amp;$D$1&amp;"="&amp;$D$52&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=51,DegreePlanID=13,TermID=5,RequirementID=20},</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="15.75" customHeight="1">
@@ -5915,8 +6413,8 @@
         <v>95</v>
       </c>
       <c r="G53" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E53&amp;$A$1&amp;"="&amp;$A$53&amp;","&amp;$B$1&amp;"="&amp;$B$53&amp;","&amp;$C$1&amp;"="&amp;$C$53&amp;","&amp;$D$1&amp;"="&amp;$D$53&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=52,DegreePlanID=13,TermID=5,RequirementID=692},</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="15.75" customHeight="1">
@@ -5939,8 +6437,8 @@
         <v>95</v>
       </c>
       <c r="G54" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E54&amp;$A$1&amp;"="&amp;$A$54&amp;","&amp;$B$1&amp;"="&amp;$B$54&amp;","&amp;$C$1&amp;"="&amp;$C$54&amp;","&amp;$D$1&amp;"="&amp;$D$54&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=53,DegreePlanID=18,TermID=1,RequirementID=460},</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="15.75" customHeight="1">
@@ -5963,8 +6461,8 @@
         <v>95</v>
       </c>
       <c r="G55" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E55&amp;$A$1&amp;"="&amp;$A$55&amp;","&amp;$B$1&amp;"="&amp;$B$55&amp;","&amp;$C$1&amp;"="&amp;$C$55&amp;","&amp;$D$1&amp;"="&amp;$D$55&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=54,DegreePlanID=18,TermID=1,RequirementID=356},</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="15.75" customHeight="1">
@@ -5987,8 +6485,8 @@
         <v>95</v>
       </c>
       <c r="G56" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E56&amp;$A$1&amp;"="&amp;$A$56&amp;","&amp;$B$1&amp;"="&amp;$B$56&amp;","&amp;$C$1&amp;"="&amp;$C$56&amp;","&amp;$D$1&amp;"="&amp;$D$56&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=55,DegreePlanID=18,TermID=1,RequirementID=542},</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="15.75" customHeight="1">
@@ -6011,8 +6509,8 @@
         <v>95</v>
       </c>
       <c r="G57" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E57&amp;$A$1&amp;"="&amp;$A$57&amp;","&amp;$B$1&amp;"="&amp;$B$57&amp;","&amp;$C$1&amp;"="&amp;$C$57&amp;","&amp;$D$1&amp;"="&amp;$D$57&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=56,DegreePlanID=18,TermID=1,RequirementID=563},</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="15.75" customHeight="1">
@@ -6035,8 +6533,8 @@
         <v>95</v>
       </c>
       <c r="G58" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E58&amp;$A$1&amp;"="&amp;$A$58&amp;","&amp;$B$1&amp;"="&amp;$B$58&amp;","&amp;$C$1&amp;"="&amp;$C$58&amp;","&amp;$D$1&amp;"="&amp;$D$58&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=57,DegreePlanID=18,TermID=2,RequirementID=560},</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="15.75" customHeight="1">
@@ -6059,8 +6557,8 @@
         <v>95</v>
       </c>
       <c r="G59" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E59&amp;$A$1&amp;"="&amp;$A$59&amp;","&amp;$B$1&amp;"="&amp;$B$59&amp;","&amp;$C$1&amp;"="&amp;$C$59&amp;","&amp;$D$1&amp;"="&amp;$D$59&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=58,DegreePlanID=18,TermID=2,RequirementID=555},</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="15.75" customHeight="1">
@@ -6083,8 +6581,8 @@
         <v>95</v>
       </c>
       <c r="G60" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E60&amp;$A$1&amp;"="&amp;$A$60&amp;","&amp;$B$1&amp;"="&amp;$B$60&amp;","&amp;$C$1&amp;"="&amp;$C$60&amp;","&amp;$D$1&amp;"="&amp;$D$60&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=59,DegreePlanID=18,TermID=2,RequirementID=618},</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="15.75" customHeight="1">
@@ -6107,8 +6605,8 @@
         <v>95</v>
       </c>
       <c r="G61" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E61&amp;$A$1&amp;"="&amp;$A$61&amp;","&amp;$B$1&amp;"="&amp;$B$61&amp;","&amp;$C$1&amp;"="&amp;$C$61&amp;","&amp;$D$1&amp;"="&amp;$D$61&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=60,DegreePlanID=18,TermID=3,RequirementID=1},</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="15.75" customHeight="1">
@@ -6131,8 +6629,8 @@
         <v>95</v>
       </c>
       <c r="G62" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E62&amp;$A$1&amp;"="&amp;$A$62&amp;","&amp;$B$1&amp;"="&amp;$B$62&amp;","&amp;$C$1&amp;"="&amp;$C$62&amp;","&amp;$D$1&amp;"="&amp;$D$62&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=61,DegreePlanID=18,TermID=3,RequirementID=664},</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="15.75" customHeight="1">
@@ -6155,8 +6653,8 @@
         <v>95</v>
       </c>
       <c r="G63" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E63&amp;$A$1&amp;"="&amp;$A$63&amp;","&amp;$B$1&amp;"="&amp;$B$63&amp;","&amp;$C$1&amp;"="&amp;$C$63&amp;","&amp;$D$1&amp;"="&amp;$D$63&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=62,DegreePlanID=18,TermID=4,RequirementID=691},</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="15.75" customHeight="1">
@@ -6179,8 +6677,8 @@
         <v>95</v>
       </c>
       <c r="G64" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E64&amp;$A$1&amp;"="&amp;$A$64&amp;","&amp;$B$1&amp;"="&amp;$B$64&amp;","&amp;$C$1&amp;"="&amp;$C$64&amp;","&amp;$D$1&amp;"="&amp;$D$64&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=63,DegreePlanID=18,TermID=4,RequirementID=10},</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="15.75" customHeight="1">
@@ -6203,8 +6701,8 @@
         <v>95</v>
       </c>
       <c r="G65" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E65&amp;$A$1&amp;"="&amp;$A$65&amp;","&amp;$B$1&amp;"="&amp;$B$65&amp;","&amp;$C$1&amp;"="&amp;$C$65&amp;","&amp;$D$1&amp;"="&amp;$D$65&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=64,DegreePlanID=18,TermID=4,RequirementID=20},</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="15.75" customHeight="1">
@@ -6227,8 +6725,8 @@
         <v>95</v>
       </c>
       <c r="G66" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E66&amp;$A$1&amp;"="&amp;$A$66&amp;","&amp;$B$1&amp;"="&amp;$B$66&amp;","&amp;$C$1&amp;"="&amp;$C$66&amp;","&amp;$D$1&amp;"="&amp;$D$66&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=65,DegreePlanID=18,TermID=5,RequirementID=692},</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="15.75" customHeight="1">
@@ -6251,8 +6749,8 @@
         <v>95</v>
       </c>
       <c r="G67" t="str">
-        <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E67&amp;$A$1&amp;"="&amp;$A$67&amp;","&amp;$B$1&amp;"="&amp;$B$67&amp;","&amp;$C$1&amp;"="&amp;$C$67&amp;","&amp;$D$1&amp;"="&amp;$D$67&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=66,DegreePlanID=19,TermID=1,RequirementID=460},</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="15.75" customHeight="1">
@@ -6275,8 +6773,8 @@
         <v>95</v>
       </c>
       <c r="G68" t="str">
-        <f t="shared" ref="G68:G131" si="1">E68&amp;$A$1&amp;"="&amp;$A$3&amp;","&amp;$B$1&amp;"="&amp;$B$3&amp;","&amp;$C$1&amp;"="&amp;$C$3&amp;","&amp;$D$1&amp;"="&amp;$D$3&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E68&amp;$A$1&amp;"="&amp;$A$68&amp;","&amp;$B$1&amp;"="&amp;$B$68&amp;","&amp;$C$1&amp;"="&amp;$C$68&amp;","&amp;$D$1&amp;"="&amp;$D$68&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=67,DegreePlanID=19,TermID=1,RequirementID=356},</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="15.75" customHeight="1">
@@ -6299,8 +6797,8 @@
         <v>95</v>
       </c>
       <c r="G69" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E69&amp;$A$1&amp;"="&amp;$A$69&amp;","&amp;$B$1&amp;"="&amp;$B$69&amp;","&amp;$C$1&amp;"="&amp;$C$69&amp;","&amp;$D$1&amp;"="&amp;$D$69&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=68,DegreePlanID=19,TermID=1,RequirementID=542},</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="15.75" customHeight="1">
@@ -6323,8 +6821,8 @@
         <v>95</v>
       </c>
       <c r="G70" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E70&amp;$A$1&amp;"="&amp;$A$70&amp;","&amp;$B$1&amp;"="&amp;$B$70&amp;","&amp;$C$1&amp;"="&amp;$C$70&amp;","&amp;$D$1&amp;"="&amp;$D$70&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=69,DegreePlanID=19,TermID=1,RequirementID=563},</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="15.75" customHeight="1">
@@ -6347,8 +6845,8 @@
         <v>95</v>
       </c>
       <c r="G71" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E71&amp;$A$1&amp;"="&amp;$A$71&amp;","&amp;$B$1&amp;"="&amp;$B$71&amp;","&amp;$C$1&amp;"="&amp;$C$71&amp;","&amp;$D$1&amp;"="&amp;$D$71&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=70,DegreePlanID=19,TermID=3,RequirementID=560},</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="15.75" customHeight="1">
@@ -6371,8 +6869,8 @@
         <v>95</v>
       </c>
       <c r="G72" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E72&amp;$A$1&amp;"="&amp;$A$72&amp;","&amp;$B$1&amp;"="&amp;$B$72&amp;","&amp;$C$1&amp;"="&amp;$C$72&amp;","&amp;$D$1&amp;"="&amp;$D$72&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=71,DegreePlanID=19,TermID=3,RequirementID=555},</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="15.75" customHeight="1">
@@ -6395,8 +6893,8 @@
         <v>95</v>
       </c>
       <c r="G73" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E73&amp;$A$1&amp;"="&amp;$A$73&amp;","&amp;$B$1&amp;"="&amp;$B$73&amp;","&amp;$C$1&amp;"="&amp;$C$73&amp;","&amp;$D$1&amp;"="&amp;$D$73&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=72,DegreePlanID=19,TermID=3,RequirementID=618},</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="15.75" customHeight="1">
@@ -6419,8 +6917,8 @@
         <v>95</v>
       </c>
       <c r="G74" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E74&amp;$A$1&amp;"="&amp;$A$74&amp;","&amp;$B$1&amp;"="&amp;$B$74&amp;","&amp;$C$1&amp;"="&amp;$C$74&amp;","&amp;$D$1&amp;"="&amp;$D$74&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=73,DegreePlanID=19,TermID=4,RequirementID=1},</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="15.75" customHeight="1">
@@ -6443,8 +6941,8 @@
         <v>95</v>
       </c>
       <c r="G75" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E75&amp;$A$1&amp;"="&amp;$A$75&amp;","&amp;$B$1&amp;"="&amp;$B$75&amp;","&amp;$C$1&amp;"="&amp;$C$75&amp;","&amp;$D$1&amp;"="&amp;$D$75&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=74,DegreePlanID=19,TermID=4,RequirementID=664},</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="15.75" customHeight="1">
@@ -6467,8 +6965,8 @@
         <v>95</v>
       </c>
       <c r="G76" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E76&amp;$A$1&amp;"="&amp;$A$76&amp;","&amp;$B$1&amp;"="&amp;$B$76&amp;","&amp;$C$1&amp;"="&amp;$C$76&amp;","&amp;$D$1&amp;"="&amp;$D$76&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=75,DegreePlanID=19,TermID=4,RequirementID=691},</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="15.75" customHeight="1">
@@ -6491,8 +6989,8 @@
         <v>95</v>
       </c>
       <c r="G77" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E77&amp;$A$1&amp;"="&amp;$A$77&amp;","&amp;$B$1&amp;"="&amp;$B$77&amp;","&amp;$C$1&amp;"="&amp;$C$77&amp;","&amp;$D$1&amp;"="&amp;$D$77&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=76,DegreePlanID=19,TermID=5,RequirementID=10},</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="15.75" customHeight="1">
@@ -6515,8 +7013,8 @@
         <v>95</v>
       </c>
       <c r="G78" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E78&amp;$A$1&amp;"="&amp;$A$78&amp;","&amp;$B$1&amp;"="&amp;$B$78&amp;","&amp;$C$1&amp;"="&amp;$C$78&amp;","&amp;$D$1&amp;"="&amp;$D$78&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=77,DegreePlanID=19,TermID=5,RequirementID=20},</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="15.75" customHeight="1">
@@ -6539,8 +7037,8 @@
         <v>95</v>
       </c>
       <c r="G79" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E79&amp;$A$1&amp;"="&amp;$A$79&amp;","&amp;$B$1&amp;"="&amp;$B$79&amp;","&amp;$C$1&amp;"="&amp;$C$79&amp;","&amp;$D$1&amp;"="&amp;$D$79&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=78,DegreePlanID=19,TermID=5,RequirementID=692},</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="15.75" customHeight="1">
@@ -6563,8 +7061,8 @@
         <v>95</v>
       </c>
       <c r="G80" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E80&amp;$A$1&amp;"="&amp;$A$80&amp;","&amp;$B$1&amp;"="&amp;$B$80&amp;","&amp;$C$1&amp;"="&amp;$C$80&amp;","&amp;$D$1&amp;"="&amp;$D$80&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=79,DegreePlanID=16,TermID=1,RequirementID=460},</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="15.75" customHeight="1">
@@ -6587,8 +7085,8 @@
         <v>95</v>
       </c>
       <c r="G81" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E81&amp;$A$1&amp;"="&amp;$A$81&amp;","&amp;$B$1&amp;"="&amp;$B$81&amp;","&amp;$C$1&amp;"="&amp;$C$81&amp;","&amp;$D$1&amp;"="&amp;$D$81&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=80,DegreePlanID=16,TermID=1,RequirementID=356},</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="15.75" customHeight="1">
@@ -6611,8 +7109,8 @@
         <v>95</v>
       </c>
       <c r="G82" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E82&amp;$A$1&amp;"="&amp;$A$82&amp;","&amp;$B$1&amp;"="&amp;$B$82&amp;","&amp;$C$1&amp;"="&amp;$C$82&amp;","&amp;$D$1&amp;"="&amp;$D$82&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=81,DegreePlanID=16,TermID=1,RequirementID=542},</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="15.75" customHeight="1">
@@ -6635,8 +7133,8 @@
         <v>95</v>
       </c>
       <c r="G83" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E83&amp;$A$1&amp;"="&amp;$A$83&amp;","&amp;$B$1&amp;"="&amp;$B$83&amp;","&amp;$C$1&amp;"="&amp;$C$83&amp;","&amp;$D$1&amp;"="&amp;$D$83&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=82,DegreePlanID=16,TermID=1,RequirementID=563},</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="15.75" customHeight="1">
@@ -6659,8 +7157,8 @@
         <v>95</v>
       </c>
       <c r="G84" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E84&amp;$A$1&amp;"="&amp;$A$84&amp;","&amp;$B$1&amp;"="&amp;$B$84&amp;","&amp;$C$1&amp;"="&amp;$C$84&amp;","&amp;$D$1&amp;"="&amp;$D$84&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=83,DegreePlanID=16,TermID=2,RequirementID=560},</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="15.75" customHeight="1">
@@ -6683,8 +7181,8 @@
         <v>95</v>
       </c>
       <c r="G85" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E85&amp;$A$1&amp;"="&amp;$A$85&amp;","&amp;$B$1&amp;"="&amp;$B$85&amp;","&amp;$C$1&amp;"="&amp;$C$85&amp;","&amp;$D$1&amp;"="&amp;$D$85&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=84,DegreePlanID=16,TermID=2,RequirementID=555},</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="15.75" customHeight="1">
@@ -6707,8 +7205,8 @@
         <v>95</v>
       </c>
       <c r="G86" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E86&amp;$A$1&amp;"="&amp;$A$86&amp;","&amp;$B$1&amp;"="&amp;$B$86&amp;","&amp;$C$1&amp;"="&amp;$C$86&amp;","&amp;$D$1&amp;"="&amp;$D$86&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=85,DegreePlanID=16,TermID=2,RequirementID=618},</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="15.75" customHeight="1">
@@ -6731,8 +7229,8 @@
         <v>95</v>
       </c>
       <c r="G87" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E87&amp;$A$1&amp;"="&amp;$A$87&amp;","&amp;$B$1&amp;"="&amp;$B$87&amp;","&amp;$C$1&amp;"="&amp;$C$87&amp;","&amp;$D$1&amp;"="&amp;$D$87&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=86,DegreePlanID=16,TermID=3,RequirementID=1},</v>
       </c>
     </row>
     <row r="88" spans="1:7" ht="15.75" customHeight="1">
@@ -6755,8 +7253,8 @@
         <v>95</v>
       </c>
       <c r="G88" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E88&amp;$A$1&amp;"="&amp;$A$88&amp;","&amp;$B$1&amp;"="&amp;$B$88&amp;","&amp;$C$1&amp;"="&amp;$C$88&amp;","&amp;$D$1&amp;"="&amp;$D$88&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=87,DegreePlanID=16,TermID=3,RequirementID=664},</v>
       </c>
     </row>
     <row r="89" spans="1:7" ht="15.75" customHeight="1">
@@ -6779,8 +7277,8 @@
         <v>95</v>
       </c>
       <c r="G89" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E89&amp;$A$1&amp;"="&amp;$A$89&amp;","&amp;$B$1&amp;"="&amp;$B$89&amp;","&amp;$C$1&amp;"="&amp;$C$89&amp;","&amp;$D$1&amp;"="&amp;$D$89&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=88,DegreePlanID=16,TermID=3,RequirementID=691},</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="15.75" customHeight="1">
@@ -6803,8 +7301,8 @@
         <v>95</v>
       </c>
       <c r="G90" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E90&amp;$A$1&amp;"="&amp;$A$90&amp;","&amp;$B$1&amp;"="&amp;$B$90&amp;","&amp;$C$1&amp;"="&amp;$C$90&amp;","&amp;$D$1&amp;"="&amp;$D$90&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=89,DegreePlanID=16,TermID=4,RequirementID=10},</v>
       </c>
     </row>
     <row r="91" spans="1:7" ht="15.75" customHeight="1">
@@ -6827,8 +7325,8 @@
         <v>95</v>
       </c>
       <c r="G91" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E91&amp;$A$1&amp;"="&amp;$A$91&amp;","&amp;$B$1&amp;"="&amp;$B$91&amp;","&amp;$C$1&amp;"="&amp;$C$91&amp;","&amp;$D$1&amp;"="&amp;$D$91&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=90,DegreePlanID=16,TermID=4,RequirementID=20},</v>
       </c>
     </row>
     <row r="92" spans="1:7" ht="15.75" customHeight="1">
@@ -6851,8 +7349,8 @@
         <v>95</v>
       </c>
       <c r="G92" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E92&amp;$A$1&amp;"="&amp;$A$92&amp;","&amp;$B$1&amp;"="&amp;$B$92&amp;","&amp;$C$1&amp;"="&amp;$C$92&amp;","&amp;$D$1&amp;"="&amp;$D$92&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=91,DegreePlanID=16,TermID=5,RequirementID=692},</v>
       </c>
     </row>
     <row r="93" spans="1:7" ht="15.75" customHeight="1">
@@ -6875,8 +7373,8 @@
         <v>95</v>
       </c>
       <c r="G93" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E93&amp;$A$1&amp;"="&amp;$A$93&amp;","&amp;$B$1&amp;"="&amp;$B$93&amp;","&amp;$C$1&amp;"="&amp;$C$93&amp;","&amp;$D$1&amp;"="&amp;$D$93&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=92,DegreePlanID=17,TermID=1,RequirementID=460},</v>
       </c>
     </row>
     <row r="94" spans="1:7" ht="15.75" customHeight="1">
@@ -6899,8 +7397,8 @@
         <v>95</v>
       </c>
       <c r="G94" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E94&amp;$A$1&amp;"="&amp;$A$94&amp;","&amp;$B$1&amp;"="&amp;$B$94&amp;","&amp;$C$1&amp;"="&amp;$C$94&amp;","&amp;$D$1&amp;"="&amp;$D$94&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=93,DegreePlanID=17,TermID=1,RequirementID=356},</v>
       </c>
     </row>
     <row r="95" spans="1:7" ht="15.75" customHeight="1">
@@ -6923,8 +7421,8 @@
         <v>95</v>
       </c>
       <c r="G95" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E95&amp;$A$1&amp;"="&amp;$A$95&amp;","&amp;$B$1&amp;"="&amp;$B$95&amp;","&amp;$C$1&amp;"="&amp;$C$95&amp;","&amp;$D$1&amp;"="&amp;$D$95&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=94,DegreePlanID=17,TermID=1,RequirementID=542},</v>
       </c>
     </row>
     <row r="96" spans="1:7" ht="15.75" customHeight="1">
@@ -6947,8 +7445,8 @@
         <v>95</v>
       </c>
       <c r="G96" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E96&amp;$A$1&amp;"="&amp;$A$96&amp;","&amp;$B$1&amp;"="&amp;$B$96&amp;","&amp;$C$1&amp;"="&amp;$C$96&amp;","&amp;$D$1&amp;"="&amp;$D$96&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=95,DegreePlanID=17,TermID=1,RequirementID=563},</v>
       </c>
     </row>
     <row r="97" spans="1:7" ht="15.75" customHeight="1">
@@ -6971,8 +7469,8 @@
         <v>95</v>
       </c>
       <c r="G97" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E97&amp;$A$1&amp;"="&amp;$A$97&amp;","&amp;$B$1&amp;"="&amp;$B$97&amp;","&amp;$C$1&amp;"="&amp;$C$97&amp;","&amp;$D$1&amp;"="&amp;$D$97&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=96,DegreePlanID=17,TermID=2,RequirementID=560},</v>
       </c>
     </row>
     <row r="98" spans="1:7" ht="15.75" customHeight="1">
@@ -6995,8 +7493,8 @@
         <v>95</v>
       </c>
       <c r="G98" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E98&amp;$A$1&amp;"="&amp;$A$98&amp;","&amp;$B$1&amp;"="&amp;$B$98&amp;","&amp;$C$1&amp;"="&amp;$C$98&amp;","&amp;$D$1&amp;"="&amp;$D$98&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=97,DegreePlanID=17,TermID=2,RequirementID=555},</v>
       </c>
     </row>
     <row r="99" spans="1:7" ht="15.75" customHeight="1">
@@ -7019,8 +7517,8 @@
         <v>95</v>
       </c>
       <c r="G99" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E99&amp;$A$1&amp;"="&amp;$A$99&amp;","&amp;$B$1&amp;"="&amp;$B$99&amp;","&amp;$C$1&amp;"="&amp;$C$99&amp;","&amp;$D$1&amp;"="&amp;$D$99&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=98,DegreePlanID=17,TermID=2,RequirementID=618},</v>
       </c>
     </row>
     <row r="100" spans="1:7" ht="15.75" customHeight="1">
@@ -7043,8 +7541,8 @@
         <v>95</v>
       </c>
       <c r="G100" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E100&amp;$A$1&amp;"="&amp;$A$100&amp;","&amp;$B$1&amp;"="&amp;$B$100&amp;","&amp;$C$1&amp;"="&amp;$C$100&amp;","&amp;$D$1&amp;"="&amp;$D$100&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=99,DegreePlanID=17,TermID=4,RequirementID=1},</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="15.75" customHeight="1">
@@ -7067,8 +7565,8 @@
         <v>95</v>
       </c>
       <c r="G101" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E101&amp;$A$1&amp;"="&amp;$A$101&amp;","&amp;$B$1&amp;"="&amp;$B$101&amp;","&amp;$C$1&amp;"="&amp;$C$101&amp;","&amp;$D$1&amp;"="&amp;$D$101&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=100,DegreePlanID=17,TermID=4,RequirementID=664},</v>
       </c>
     </row>
     <row r="102" spans="1:7" ht="15.75" customHeight="1">
@@ -7091,8 +7589,8 @@
         <v>95</v>
       </c>
       <c r="G102" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E102&amp;$A$1&amp;"="&amp;$A$102&amp;","&amp;$B$1&amp;"="&amp;$B$102&amp;","&amp;$C$1&amp;"="&amp;$C$102&amp;","&amp;$D$1&amp;"="&amp;$D$102&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=101,DegreePlanID=17,TermID=4,RequirementID=691},</v>
       </c>
     </row>
     <row r="103" spans="1:7" ht="15.75" customHeight="1">
@@ -7115,8 +7613,8 @@
         <v>95</v>
       </c>
       <c r="G103" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E103&amp;$A$1&amp;"="&amp;$A$103&amp;","&amp;$B$1&amp;"="&amp;$B$103&amp;","&amp;$C$1&amp;"="&amp;$C$103&amp;","&amp;$D$1&amp;"="&amp;$D$103&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=102,DegreePlanID=17,TermID=5,RequirementID=10},</v>
       </c>
     </row>
     <row r="104" spans="1:7" ht="15.75" customHeight="1">
@@ -7139,8 +7637,8 @@
         <v>95</v>
       </c>
       <c r="G104" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E104&amp;$A$1&amp;"="&amp;$A$104&amp;","&amp;$B$1&amp;"="&amp;$B$104&amp;","&amp;$C$1&amp;"="&amp;$C$104&amp;","&amp;$D$1&amp;"="&amp;$D$104&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=103,DegreePlanID=17,TermID=5,RequirementID=20},</v>
       </c>
     </row>
     <row r="105" spans="1:7" ht="15.75" customHeight="1">
@@ -7163,8 +7661,8 @@
         <v>95</v>
       </c>
       <c r="G105" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E105&amp;$A$1&amp;"="&amp;$A$105&amp;","&amp;$B$1&amp;"="&amp;$B$105&amp;","&amp;$C$1&amp;"="&amp;$C$105&amp;","&amp;$D$1&amp;"="&amp;$D$105&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=104,DegreePlanID=17,TermID=5,RequirementID=692},</v>
       </c>
     </row>
     <row r="106" spans="1:7" ht="15.75" customHeight="1">
@@ -7187,8 +7685,8 @@
         <v>95</v>
       </c>
       <c r="G106" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E106&amp;$A$1&amp;"="&amp;$A$106&amp;","&amp;$B$1&amp;"="&amp;$B$106&amp;","&amp;$C$1&amp;"="&amp;$C$106&amp;","&amp;$D$1&amp;"="&amp;$D$106&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=105,DegreePlanID=14,TermID=1,RequirementID=460},</v>
       </c>
     </row>
     <row r="107" spans="1:7" ht="15.75" customHeight="1">
@@ -7211,8 +7709,8 @@
         <v>95</v>
       </c>
       <c r="G107" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E107&amp;$A$1&amp;"="&amp;$A$107&amp;","&amp;$B$1&amp;"="&amp;$B$107&amp;","&amp;$C$1&amp;"="&amp;$C$107&amp;","&amp;$D$1&amp;"="&amp;$D$107&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=106,DegreePlanID=14,TermID=1,RequirementID=356},</v>
       </c>
     </row>
     <row r="108" spans="1:7" ht="15.75" customHeight="1">
@@ -7220,7 +7718,7 @@
         <v>107</v>
       </c>
       <c r="B108" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C108">
         <v>1</v>
@@ -7235,8 +7733,8 @@
         <v>95</v>
       </c>
       <c r="G108" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E108&amp;$A$1&amp;"="&amp;$A$108&amp;","&amp;$B$1&amp;"="&amp;$B$108&amp;","&amp;$C$1&amp;"="&amp;$C$108&amp;","&amp;$D$1&amp;"="&amp;$D$108&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=107,DegreePlanID=15,TermID=1,RequirementID=542},</v>
       </c>
     </row>
     <row r="109" spans="1:7" ht="15.75" customHeight="1">
@@ -7244,7 +7742,7 @@
         <v>108</v>
       </c>
       <c r="B109" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C109">
         <v>1</v>
@@ -7259,8 +7757,8 @@
         <v>95</v>
       </c>
       <c r="G109" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E109&amp;$A$1&amp;"="&amp;$A$109&amp;","&amp;$B$1&amp;"="&amp;$B$109&amp;","&amp;$C$1&amp;"="&amp;$C$109&amp;","&amp;$D$1&amp;"="&amp;$D$109&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=108,DegreePlanID=15,TermID=1,RequirementID=563},</v>
       </c>
     </row>
     <row r="110" spans="1:7" ht="15.75" customHeight="1">
@@ -7268,7 +7766,7 @@
         <v>109</v>
       </c>
       <c r="B110" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C110">
         <v>2</v>
@@ -7283,8 +7781,8 @@
         <v>95</v>
       </c>
       <c r="G110" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E110&amp;$A$1&amp;"="&amp;$A$110&amp;","&amp;$B$1&amp;"="&amp;$B$110&amp;","&amp;$C$1&amp;"="&amp;$C$110&amp;","&amp;$D$1&amp;"="&amp;$D$110&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=109,DegreePlanID=15,TermID=2,RequirementID=560},</v>
       </c>
     </row>
     <row r="111" spans="1:7" ht="15.75" customHeight="1">
@@ -7292,7 +7790,7 @@
         <v>110</v>
       </c>
       <c r="B111" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C111">
         <v>2</v>
@@ -7307,8 +7805,8 @@
         <v>95</v>
       </c>
       <c r="G111" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E111&amp;$A$1&amp;"="&amp;$A$111&amp;","&amp;$B$1&amp;"="&amp;$B$111&amp;","&amp;$C$1&amp;"="&amp;$C$111&amp;","&amp;$D$1&amp;"="&amp;$D$111&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=110,DegreePlanID=15,TermID=2,RequirementID=555},</v>
       </c>
     </row>
     <row r="112" spans="1:7" ht="15.75" customHeight="1">
@@ -7316,7 +7814,7 @@
         <v>111</v>
       </c>
       <c r="B112" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C112">
         <v>2</v>
@@ -7331,8 +7829,8 @@
         <v>95</v>
       </c>
       <c r="G112" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E112&amp;$A$1&amp;"="&amp;$A$112&amp;","&amp;$B$1&amp;"="&amp;$B$112&amp;","&amp;$C$1&amp;"="&amp;$C$112&amp;","&amp;$D$1&amp;"="&amp;$D$112&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=111,DegreePlanID=15,TermID=2,RequirementID=618},</v>
       </c>
     </row>
     <row r="113" spans="1:7" ht="15.75" customHeight="1">
@@ -7340,7 +7838,7 @@
         <v>112</v>
       </c>
       <c r="B113" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C113">
         <v>3</v>
@@ -7355,8 +7853,8 @@
         <v>95</v>
       </c>
       <c r="G113" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E113&amp;$A$1&amp;"="&amp;$A$113&amp;","&amp;$B$1&amp;"="&amp;$B$113&amp;","&amp;$C$1&amp;"="&amp;$C$113&amp;","&amp;$D$1&amp;"="&amp;$D$113&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=112,DegreePlanID=15,TermID=3,RequirementID=1},</v>
       </c>
     </row>
     <row r="114" spans="1:7" ht="15.75" customHeight="1">
@@ -7364,7 +7862,7 @@
         <v>113</v>
       </c>
       <c r="B114" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C114">
         <v>3</v>
@@ -7379,8 +7877,8 @@
         <v>95</v>
       </c>
       <c r="G114" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E114&amp;$A$1&amp;"="&amp;$A$114&amp;","&amp;$B$1&amp;"="&amp;$B$114&amp;","&amp;$C$1&amp;"="&amp;$C$114&amp;","&amp;$D$1&amp;"="&amp;$D$114&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=113,DegreePlanID=15,TermID=3,RequirementID=664},</v>
       </c>
     </row>
     <row r="115" spans="1:7" ht="15.75" customHeight="1">
@@ -7388,7 +7886,7 @@
         <v>114</v>
       </c>
       <c r="B115" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C115">
         <v>4</v>
@@ -7403,8 +7901,8 @@
         <v>95</v>
       </c>
       <c r="G115" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E115&amp;$A$1&amp;"="&amp;$A$115&amp;","&amp;$B$1&amp;"="&amp;$B$115&amp;","&amp;$C$1&amp;"="&amp;$C$115&amp;","&amp;$D$1&amp;"="&amp;$D$115&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=114,DegreePlanID=15,TermID=4,RequirementID=691},</v>
       </c>
     </row>
     <row r="116" spans="1:7" ht="15.75" customHeight="1">
@@ -7412,7 +7910,7 @@
         <v>115</v>
       </c>
       <c r="B116" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C116">
         <v>4</v>
@@ -7427,8 +7925,8 @@
         <v>95</v>
       </c>
       <c r="G116" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E116&amp;$A$1&amp;"="&amp;$A$116&amp;","&amp;$B$1&amp;"="&amp;$B$116&amp;","&amp;$C$1&amp;"="&amp;$C$116&amp;","&amp;$D$1&amp;"="&amp;$D$116&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=115,DegreePlanID=15,TermID=4,RequirementID=10},</v>
       </c>
     </row>
     <row r="117" spans="1:7" ht="15.75" customHeight="1">
@@ -7436,7 +7934,7 @@
         <v>116</v>
       </c>
       <c r="B117" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C117">
         <v>4</v>
@@ -7451,8 +7949,8 @@
         <v>95</v>
       </c>
       <c r="G117" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E117&amp;$A$1&amp;"="&amp;$A$117&amp;","&amp;$B$1&amp;"="&amp;$B$117&amp;","&amp;$C$1&amp;"="&amp;$C$117&amp;","&amp;$D$1&amp;"="&amp;$D$117&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=116,DegreePlanID=15,TermID=4,RequirementID=20},</v>
       </c>
     </row>
     <row r="118" spans="1:7" ht="15.75" customHeight="1">
@@ -7460,7 +7958,7 @@
         <v>117</v>
       </c>
       <c r="B118" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C118">
         <v>5</v>
@@ -7475,8 +7973,8 @@
         <v>95</v>
       </c>
       <c r="G118" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E118&amp;$A$1&amp;"="&amp;$A$118&amp;","&amp;$B$1&amp;"="&amp;$B$118&amp;","&amp;$C$1&amp;"="&amp;$C$118&amp;","&amp;$D$1&amp;"="&amp;$D$118&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=117,DegreePlanID=15,TermID=5,RequirementID=692},</v>
       </c>
     </row>
     <row r="119" spans="1:7" ht="15.75" customHeight="1">
@@ -7499,8 +7997,8 @@
         <v>95</v>
       </c>
       <c r="G119" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E119&amp;$A$1&amp;"="&amp;$A$119&amp;","&amp;$B$1&amp;"="&amp;$B$119&amp;","&amp;$C$1&amp;"="&amp;$C$119&amp;","&amp;$D$1&amp;"="&amp;$D$119&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=118,DegreePlanID=15,TermID=1,RequirementID=460},</v>
       </c>
     </row>
     <row r="120" spans="1:7" ht="15.75" customHeight="1">
@@ -7523,8 +8021,8 @@
         <v>95</v>
       </c>
       <c r="G120" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E120&amp;$A$1&amp;"="&amp;$A$120&amp;","&amp;$B$1&amp;"="&amp;$B$120&amp;","&amp;$C$1&amp;"="&amp;$C$120&amp;","&amp;$D$1&amp;"="&amp;$D$120&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=119,DegreePlanID=15,TermID=1,RequirementID=356},</v>
       </c>
     </row>
     <row r="121" spans="1:7" ht="15.75" customHeight="1">
@@ -7547,8 +8045,8 @@
         <v>95</v>
       </c>
       <c r="G121" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E121&amp;$A$1&amp;"="&amp;$A$121&amp;","&amp;$B$1&amp;"="&amp;$B$121&amp;","&amp;$C$1&amp;"="&amp;$C$121&amp;","&amp;$D$1&amp;"="&amp;$D$121&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=120,DegreePlanID=15,TermID=1,RequirementID=542},</v>
       </c>
     </row>
     <row r="122" spans="1:7" ht="15.75" customHeight="1">
@@ -7571,8 +8069,8 @@
         <v>95</v>
       </c>
       <c r="G122" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E122&amp;$A$1&amp;"="&amp;$A$122&amp;","&amp;$B$1&amp;"="&amp;$B$122&amp;","&amp;$C$1&amp;"="&amp;$C$122&amp;","&amp;$D$1&amp;"="&amp;$D$122&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=121,DegreePlanID=15,TermID=1,RequirementID=563},</v>
       </c>
     </row>
     <row r="123" spans="1:7" ht="15.75" customHeight="1">
@@ -7595,8 +8093,8 @@
         <v>95</v>
       </c>
       <c r="G123" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E123&amp;$A$1&amp;"="&amp;$A$123&amp;","&amp;$B$1&amp;"="&amp;$B$123&amp;","&amp;$C$1&amp;"="&amp;$C$123&amp;","&amp;$D$1&amp;"="&amp;$D$123&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=122,DegreePlanID=15,TermID=3,RequirementID=560},</v>
       </c>
     </row>
     <row r="124" spans="1:7" ht="15.75" customHeight="1">
@@ -7619,8 +8117,8 @@
         <v>95</v>
       </c>
       <c r="G124" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E124&amp;$A$1&amp;"="&amp;$A$124&amp;","&amp;$B$1&amp;"="&amp;$B$124&amp;","&amp;$C$1&amp;"="&amp;$C$124&amp;","&amp;$D$1&amp;"="&amp;$D$124&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=123,DegreePlanID=15,TermID=3,RequirementID=555},</v>
       </c>
     </row>
     <row r="125" spans="1:7" ht="15.75" customHeight="1">
@@ -7643,8 +8141,8 @@
         <v>95</v>
       </c>
       <c r="G125" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E125&amp;$A$1&amp;"="&amp;$A$125&amp;","&amp;$B$1&amp;"="&amp;$B$125&amp;","&amp;$C$1&amp;"="&amp;$C$125&amp;","&amp;$D$1&amp;"="&amp;$D$125&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=124,DegreePlanID=15,TermID=3,RequirementID=618},</v>
       </c>
     </row>
     <row r="126" spans="1:7" ht="15.75" customHeight="1">
@@ -7667,8 +8165,8 @@
         <v>95</v>
       </c>
       <c r="G126" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E126&amp;$A$1&amp;"="&amp;$A$126&amp;","&amp;$B$1&amp;"="&amp;$B$126&amp;","&amp;$C$1&amp;"="&amp;$C$126&amp;","&amp;$D$1&amp;"="&amp;$D$126&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=125,DegreePlanID=15,TermID=4,RequirementID=1},</v>
       </c>
     </row>
     <row r="127" spans="1:7" ht="15.75" customHeight="1">
@@ -7691,8 +8189,8 @@
         <v>95</v>
       </c>
       <c r="G127" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E127&amp;$A$1&amp;"="&amp;$A$127&amp;","&amp;$B$1&amp;"="&amp;$B$127&amp;","&amp;$C$1&amp;"="&amp;$C$127&amp;","&amp;$D$1&amp;"="&amp;$D$127&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=126,DegreePlanID=15,TermID=4,RequirementID=664},</v>
       </c>
     </row>
     <row r="128" spans="1:7" ht="15.75" customHeight="1">
@@ -7715,8 +8213,8 @@
         <v>95</v>
       </c>
       <c r="G128" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E128&amp;$A$1&amp;"="&amp;$A$128&amp;","&amp;$B$1&amp;"="&amp;$B$128&amp;","&amp;$C$1&amp;"="&amp;$C$128&amp;","&amp;$D$1&amp;"="&amp;$D$128&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=127,DegreePlanID=15,TermID=4,RequirementID=691},</v>
       </c>
     </row>
     <row r="129" spans="1:7" ht="15.75" customHeight="1">
@@ -7739,8 +8237,8 @@
         <v>95</v>
       </c>
       <c r="G129" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E129&amp;$A$1&amp;"="&amp;$A$129&amp;","&amp;$B$1&amp;"="&amp;$B$129&amp;","&amp;$C$1&amp;"="&amp;$C$129&amp;","&amp;$D$1&amp;"="&amp;$D$129&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=128,DegreePlanID=15,TermID=5,RequirementID=10},</v>
       </c>
     </row>
     <row r="130" spans="1:7" ht="15.75" customHeight="1">
@@ -7763,8 +8261,8 @@
         <v>95</v>
       </c>
       <c r="G130" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E130&amp;$A$1&amp;"="&amp;$A$130&amp;","&amp;$B$1&amp;"="&amp;$B$130&amp;","&amp;$C$1&amp;"="&amp;$C$130&amp;","&amp;$D$1&amp;"="&amp;$D$130&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=129,DegreePlanID=15,TermID=5,RequirementID=20},</v>
       </c>
     </row>
     <row r="131" spans="1:7" ht="15.75" customHeight="1">
@@ -7787,8 +8285,8 @@
         <v>95</v>
       </c>
       <c r="G131" t="str">
-        <f t="shared" si="1"/>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <f>E131&amp;$A$1&amp;"="&amp;$A$131&amp;","&amp;$B$1&amp;"="&amp;$B$131&amp;","&amp;$C$1&amp;"="&amp;$C$131&amp;","&amp;$D$1&amp;"="&amp;$D$131&amp;$F$2</f>
+        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=130,DegreePlanID=15,TermID=5,RequirementID=692},</v>
       </c>
     </row>
     <row r="132" spans="1:7" ht="15.75" customHeight="1"/>
@@ -8663,25 +9161,32 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
+  <ignoredErrors>
+    <ignoredError sqref="G70" formula="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:E998"/>
+  <dimension ref="A1:H998"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1"/>
-    <col min="2" max="3" width="24.42578125" customWidth="1"/>
-    <col min="4" max="4" width="37.85546875" customWidth="1"/>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
     <col min="5" max="5" width="20.5703125" customWidth="1"/>
-    <col min="6" max="26" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" customWidth="1"/>
+    <col min="7" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>37</v>
       </c>
@@ -8697,8 +9202,17 @@
       <c r="E1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>12</v>
       </c>
@@ -8714,8 +9228,18 @@
       <c r="E2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" t="s">
+        <v>107</v>
+      </c>
+      <c r="G2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H2" t="str">
+        <f>F2&amp;$A$1&amp;"="&amp;A2&amp;","&amp;$B$1&amp;"="&amp;B2&amp;","&amp;$C$1&amp;"="&amp;C2&amp;","&amp;$D$1&amp;"="&amp;D2&amp;""&amp;$E$1&amp;"="""&amp;E2&amp;G2</f>
+        <v>new Models.DegreePlan{DegreePlanId=12,DegreeID=1,StudentId=S531494,DegreePlanAbbrev(u,8)=NSODegreePlanName(u,20)="No summer off},</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>13</v>
       </c>
@@ -8731,8 +9255,18 @@
       <c r="E3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" t="s">
+        <v>107</v>
+      </c>
+      <c r="G3" t="s">
+        <v>95</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H11" si="0">F3&amp;$A$1&amp;"="&amp;A3&amp;","&amp;$B$1&amp;"="&amp;B3&amp;","&amp;$C$1&amp;"="&amp;C3&amp;","&amp;$D$1&amp;"="&amp;D3&amp;""&amp;$E$1&amp;"="""&amp;E3&amp;G3</f>
+        <v>new Models.DegreePlan{DegreePlanId=13,DegreeID=1,StudentId=S531494,DegreePlanAbbrev(u,8)=SODegreePlanName(u,20)="summer off},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="2">
         <v>14</v>
       </c>
@@ -8748,8 +9282,18 @@
       <c r="E4" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" t="s">
+        <v>107</v>
+      </c>
+      <c r="G4" t="s">
+        <v>95</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreePlan{DegreePlanId=14,DegreeID=1,StudentId=s531507,DegreePlanAbbrev(u,8)=SODegreePlanName(u,20)="summer off},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="2">
         <v>15</v>
       </c>
@@ -8765,8 +9309,18 @@
       <c r="E5" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5" t="s">
+        <v>107</v>
+      </c>
+      <c r="G5" t="s">
+        <v>95</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreePlan{DegreePlanId=15,DegreeID=1,StudentId=s531507,DegreePlanAbbrev(u,8)=NSODegreePlanName(u,20)="No summer off},</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="2">
         <v>16</v>
       </c>
@@ -8782,8 +9336,18 @@
       <c r="E6" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6" t="s">
+        <v>107</v>
+      </c>
+      <c r="G6" t="s">
+        <v>95</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreePlan{DegreePlanId=16,DegreeID=1,StudentId=s533707,DegreePlanAbbrev(u,8)=SODegreePlanName(u,20)="summer off},</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="2">
         <v>17</v>
       </c>
@@ -8799,8 +9363,18 @@
       <c r="E7" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7" t="s">
+        <v>107</v>
+      </c>
+      <c r="G7" t="s">
+        <v>95</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreePlan{DegreePlanId=17,DegreeID=1,StudentId=s533707,DegreePlanAbbrev(u,8)=NSODegreePlanName(u,20)="No summer off},</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="2">
         <v>18</v>
       </c>
@@ -8816,8 +9390,18 @@
       <c r="E8" s="3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8" t="s">
+        <v>107</v>
+      </c>
+      <c r="G8" t="s">
+        <v>95</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreePlan{DegreePlanId=18,DegreeID=1,StudentId=s531384,DegreePlanAbbrev(u,8)=NSODegreePlanName(u,20)="No summer off},</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="2">
         <v>19</v>
       </c>
@@ -8833,8 +9417,18 @@
       <c r="E9" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G9" t="s">
+        <v>95</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreePlan{DegreePlanId=19,DegreeID=1,StudentId=s531384,DegreePlanAbbrev(u,8)=SODegreePlanName(u,20)="summer off},</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="2">
         <v>20</v>
       </c>
@@ -8850,8 +9444,18 @@
       <c r="E10" s="3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="F10" t="s">
+        <v>107</v>
+      </c>
+      <c r="G10" t="s">
+        <v>95</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreePlan{DegreePlanId=20,DegreeID=1,StudentId=S531503,DegreePlanAbbrev(u,8)=NSODegreePlanName(u,20)="No summer off},</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="2">
         <v>21</v>
       </c>
@@ -8866,6 +9470,16 @@
       </c>
       <c r="E11" s="3" t="s">
         <v>56</v>
+      </c>
+      <c r="F11" t="s">
+        <v>107</v>
+      </c>
+      <c r="G11" t="s">
+        <v>95</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreePlan{DegreePlanId=21,DegreeID=1,StudentId=s531503,DegreePlanAbbrev(u,8)=SODegreePlanName(u,20)="summer off},</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -9858,8 +10472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -9920,8 +10534,8 @@
         <v>95</v>
       </c>
       <c r="H2" t="str">
-        <f>$F$2&amp;$A$1&amp;"="&amp;$A$2&amp;","&amp;$B$1&amp;"="&amp;$B$2&amp;$C$1&amp;"="&amp;$C$2&amp;","&amp;$D$1&amp;"="&amp;$D$2&amp;","&amp;$E$1&amp;"="&amp;$E$2&amp;$G$2</f>
-        <v>new Student{StudentId=531494,FirstName=ShivaniLastName=Busireddy,Snumber=S531494,NineOneNineNumber=919564348},</v>
+        <f>$F$2&amp;$A$1&amp;"="&amp;$A$2&amp;","&amp;$B$1&amp;"="&amp;$B$2&amp;","&amp;$C$1&amp;"="&amp;$C$2&amp;","&amp;$D$1&amp;"="&amp;$D$2&amp;","&amp;$E$1&amp;"="&amp;$E$2&amp;$G$2</f>
+        <v>new Student{StudentId=531494,FirstName=Shivani,LastName=Busireddy,Snumber=S531494,NineOneNineNumber=919564348},</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -9941,8 +10555,8 @@
         <v>919561527</v>
       </c>
       <c r="H3" t="str">
-        <f>$F$2&amp;$A$1&amp;"="&amp;$A$2&amp;","&amp;$B$1&amp;"="&amp;$B$2&amp;$C$1&amp;"="&amp;$C$2&amp;","&amp;$D$1&amp;"="&amp;$D$2&amp;","&amp;$E$1&amp;"="&amp;$E$2&amp;$G$2</f>
-        <v>new Student{StudentId=531494,FirstName=ShivaniLastName=Busireddy,Snumber=S531494,NineOneNineNumber=919564348},</v>
+        <f>$F$2&amp;$A$1&amp;"="&amp;$A$3&amp;","&amp;$B$1&amp;"="&amp;$B$3&amp;","&amp;$C$1&amp;"="&amp;$C$3&amp;","&amp;$D$1&amp;"="&amp;$D$3&amp;","&amp;$E$1&amp;"="&amp;$E$3&amp;$G$2</f>
+        <v>new Student{StudentId=531503,FirstName=Santosh ,LastName=Muchkur,Snumber=S531503,NineOneNineNumber=919561527},</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -9962,8 +10576,8 @@
         <v>919561950</v>
       </c>
       <c r="H4" t="str">
-        <f t="shared" ref="H3:H6" si="0">$F$2&amp;$A$1&amp;"="&amp;$A$2&amp;","&amp;$B$1&amp;"="&amp;$B$2&amp;$C$1&amp;"="&amp;$C$2&amp;","&amp;$D$1&amp;"="&amp;$D$2&amp;","&amp;$E$1&amp;"="&amp;$E$2&amp;$G$2</f>
-        <v>new Student{StudentId=531494,FirstName=ShivaniLastName=Busireddy,Snumber=S531494,NineOneNineNumber=919564348},</v>
+        <f>$F$2&amp;$A$1&amp;"="&amp;$A$4&amp;","&amp;$B$1&amp;"="&amp;$B$4&amp;","&amp;$C$1&amp;"="&amp;$C$4&amp;","&amp;$D$1&amp;"="&amp;$D$4&amp;","&amp;$E$1&amp;"="&amp;$E$4&amp;$G$2</f>
+        <v>new Student{StudentId=531384,FirstName=Srimai Reddy ,LastName=Yanala,Snumber=s531384,NineOneNineNumber=919561950},</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -9983,8 +10597,8 @@
         <v>919571235</v>
       </c>
       <c r="H5" t="str">
-        <f t="shared" si="0"/>
-        <v>new Student{StudentId=531494,FirstName=ShivaniLastName=Busireddy,Snumber=S531494,NineOneNineNumber=919564348},</v>
+        <f>$F$2&amp;$A$1&amp;"="&amp;$A$5&amp;","&amp;$B$1&amp;"="&amp;$B$5&amp;","&amp;$C$1&amp;"="&amp;$C$5&amp;","&amp;$D$1&amp;"="&amp;$D$5&amp;","&amp;$E$1&amp;"="&amp;$E$5&amp;$G$2</f>
+        <v>new Student{StudentId=533707,FirstName=Lakshmi Seshu,LastName=Kalvakuri,Snumber=s533707,NineOneNineNumber=919571235},</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -10004,8 +10618,8 @@
         <v>919564693</v>
       </c>
       <c r="H6" t="str">
-        <f t="shared" si="0"/>
-        <v>new Student{StudentId=531494,FirstName=ShivaniLastName=Busireddy,Snumber=S531494,NineOneNineNumber=919564348},</v>
+        <f>$F$2&amp;$A$1&amp;"="&amp;$A$6&amp;","&amp;$B$1&amp;"="&amp;$B$6&amp;","&amp;$C$1&amp;"="&amp;$C$6&amp;","&amp;$D$1&amp;"="&amp;$D$6&amp;","&amp;$E$1&amp;"="&amp;$E$6&amp;$G$2</f>
+        <v>new Student{StudentId=531507,FirstName=Vijay,LastName=Thupakala,Snumber=S531507,NineOneNineNumber=919564693},</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -10998,7 +11612,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E995"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Created seed data for student term and degree plan
</commit_message>
<xml_diff>
--- a/Docs/Project05.xlsx
+++ b/Docs/Project05.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S531384\Documents\Masters\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D0E8DF5-29F6-4B99-955C-7D2C002EDFA8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9116FC9-3958-4890-8B82-E63141719FE0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Degree" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="110">
   <si>
     <t>RequirementID</t>
   </si>
@@ -317,9 +317,6 @@
     <t>str</t>
   </si>
   <si>
-    <t>new Degree {</t>
-  </si>
-  <si>
     <t>},</t>
   </si>
   <si>
@@ -344,19 +341,28 @@
     <t>TermID</t>
   </si>
   <si>
-    <t>new Requirement {</t>
-  </si>
-  <si>
-    <t>new DegreePlanTermRequirement {</t>
-  </si>
-  <si>
-    <t>new Student{</t>
-  </si>
-  <si>
     <t>new Models.DegreeRequirement {</t>
   </si>
   <si>
     <t>new Models.DegreePlan{</t>
+  </si>
+  <si>
+    <t xml:space="preserve">opening </t>
+  </si>
+  <si>
+    <t>new Models.StudentTerm{</t>
+  </si>
+  <si>
+    <t>new Models.Student{</t>
+  </si>
+  <si>
+    <t>new Models.DegreePlanTermRequirement {</t>
+  </si>
+  <si>
+    <t>new Models.Requirement {</t>
+  </si>
+  <si>
+    <t>new Models.Degree {</t>
   </si>
 </sst>
 </file>
@@ -703,8 +709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -767,14 +773,14 @@
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="E2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F2" t="str">
         <f>D2&amp;$A$1&amp;"="&amp;A2&amp;", "&amp;$B$1&amp;"="&amp;$B$2&amp;", "&amp;$C$1&amp;" ="&amp;C2&amp;E2</f>
-        <v>new Degree {DegreeID=1, DegreeAbrrev(unique,max 6 characters)=ACS+2, DegreeName(unique, max 20 characters) =MS ACS +2 },</v>
+        <v>new Models.Degree {DegreeID=1, DegreeAbrrev(unique,max 6 characters)=ACS+2, DegreeName(unique, max 20 characters) =MS ACS +2 },</v>
       </c>
     </row>
     <row r="3" spans="1:26">
@@ -788,14 +794,14 @@
         <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="E3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F3" t="str">
         <f>D3&amp;$A$1&amp;"="&amp;A3&amp;", "&amp;$B$1&amp;"="&amp;$B$3&amp;", "&amp;$C$1&amp;" ="&amp;C3&amp;E3</f>
-        <v>new Degree {DegreeID=2, DegreeAbrrev(unique,max 6 characters)=ACS+DB, DegreeName(unique, max 20 characters) =MS ACS +DB},</v>
+        <v>new Models.Degree {DegreeID=2, DegreeAbrrev(unique,max 6 characters)=ACS+DB, DegreeName(unique, max 20 characters) =MS ACS +DB},</v>
       </c>
     </row>
     <row r="4" spans="1:26">
@@ -809,14 +815,14 @@
         <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="E4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F4" t="str">
         <f>D4&amp;$A$1&amp;"="&amp;A4&amp;", "&amp;$B$1&amp;"="&amp;$B$4&amp;", "&amp;$C$1&amp;" ="&amp;C4&amp;E4</f>
-        <v>new Degree {DegreeID=3, DegreeAbrrev(unique,max 6 characters)=ACS+NF, DegreeName(unique, max 20 characters) =MS ACS+NF},</v>
+        <v>new Models.Degree {DegreeID=3, DegreeAbrrev(unique,max 6 characters)=ACS+NF, DegreeName(unique, max 20 characters) =MS ACS+NF},</v>
       </c>
     </row>
     <row r="5" spans="1:26">
@@ -830,14 +836,14 @@
         <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="E5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F5" t="str">
         <f>D5&amp;$A$1&amp;"="&amp;A5&amp;", "&amp;$B$1&amp;"="&amp;$B$5&amp;", "&amp;$C$1&amp;" ="&amp;C5&amp;E5</f>
-        <v>new Degree {DegreeID=4, DegreeAbrrev(unique,max 6 characters)=ACS, DegreeName(unique, max 20 characters) =MS ACS},</v>
+        <v>new Models.Degree {DegreeID=4, DegreeAbrrev(unique,max 6 characters)=ACS, DegreeName(unique, max 20 characters) =MS ACS},</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -1831,7 +1837,7 @@
   <dimension ref="A1:F1000"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1876,14 +1882,14 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="E2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F2" t="str">
         <f>Student!H:H</f>
-        <v>new Student{StudentId=531494,FirstName=Shivani,LastName=Busireddy,Snumber=S531494,NineOneNineNumber=919564348},</v>
+        <v>new Models.Student{StudentId=531494,FirstName=Shivani,LastName=Busireddy,Snumber=S531494,NineOneNineNumber=919564348},</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1897,14 +1903,14 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="E3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F3" t="str">
         <f>D3&amp;$A$1&amp;"="&amp;$A$3&amp;","&amp;$B$1&amp;"="&amp;$B$3&amp;","&amp;$C$1&amp;"="&amp;$C$3&amp;$E$2</f>
-        <v>new Requirement {RequirementID=356,RequirementAbbrev(unique,max 6)=NF,RequirementName(unique, max 20)=44-356 Network Fundamemtals},</v>
+        <v>new Models.Requirement {RequirementID=356,RequirementAbbrev(unique,max 6)=NF,RequirementName(unique, max 20)=44-356 Network Fundamemtals},</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1918,14 +1924,14 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="E4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F4" t="str">
         <f>D4&amp;$A$1&amp;"="&amp;$A$4&amp;","&amp;$B$1&amp;"="&amp;$B$4&amp;","&amp;$C$1&amp;"="&amp;$C$4&amp;$E$2</f>
-        <v>new Requirement {RequirementID=542,RequirementAbbrev(unique,max 6)=OOP,RequirementName(unique, max 20)=44-542 OOP with Java},</v>
+        <v>new Models.Requirement {RequirementID=542,RequirementAbbrev(unique,max 6)=OOP,RequirementName(unique, max 20)=44-542 OOP with Java},</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1939,14 +1945,14 @@
         <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="E5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F5" t="str">
         <f>D5&amp;$A$1&amp;"="&amp;$A$5&amp;","&amp;$B$1&amp;"="&amp;$B$5&amp;","&amp;$C$1&amp;"="&amp;$C$5&amp;$E$2</f>
-        <v>new Requirement {RequirementID=563,RequirementAbbrev(unique,max 6)=Web apps,RequirementName(unique, max 20)=44-563 Web apps},</v>
+        <v>new Models.Requirement {RequirementID=563,RequirementAbbrev(unique,max 6)=Web apps,RequirementName(unique, max 20)=44-563 Web apps},</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1960,14 +1966,14 @@
         <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="E6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F6" t="str">
         <f>D6&amp;$A$1&amp;"="&amp;$A$6&amp;","&amp;$B$1&amp;"="&amp;$B$6&amp;","&amp;$C$1&amp;"="&amp;$C$6&amp;$E$2</f>
-        <v>new Requirement {RequirementID=560,RequirementAbbrev(unique,max 6)=ADB,RequirementName(unique, max 20)=44-560 ADB},</v>
+        <v>new Models.Requirement {RequirementID=560,RequirementAbbrev(unique,max 6)=ADB,RequirementName(unique, max 20)=44-560 ADB},</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1981,14 +1987,14 @@
         <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="E7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F7" t="str">
         <f>D7&amp;$A$1&amp;"="&amp;$A$7&amp;","&amp;$B$1&amp;"="&amp;$B$7&amp;","&amp;$C$1&amp;"="&amp;$C$7&amp;$E$2</f>
-        <v>new Requirement {RequirementID=555,RequirementAbbrev(unique,max 6)=NS,RequirementName(unique, max 20)=44-555 Network Security},</v>
+        <v>new Models.Requirement {RequirementID=555,RequirementAbbrev(unique,max 6)=NS,RequirementName(unique, max 20)=44-555 Network Security},</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2002,14 +2008,14 @@
         <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="E8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F8" t="str">
         <f>D8&amp;$A$1&amp;"="&amp;$A$8&amp;","&amp;$B$1&amp;"="&amp;$B$8&amp;","&amp;$C$1&amp;"="&amp;$C$8&amp;$E$2</f>
-        <v>new Requirement {RequirementID=618,RequirementAbbrev(unique,max 6)=PM,RequirementName(unique, max 20)=44-618 PM},</v>
+        <v>new Models.Requirement {RequirementID=618,RequirementAbbrev(unique,max 6)=PM,RequirementName(unique, max 20)=44-618 PM},</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2023,14 +2029,14 @@
         <v>28</v>
       </c>
       <c r="D9" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="E9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F9" t="str">
         <f>D9&amp;$A$1&amp;"="&amp;$A$9&amp;","&amp;$B$1&amp;"="&amp;$B$9&amp;","&amp;$C$1&amp;"="&amp;$C$9&amp;$E$2</f>
-        <v>new Requirement {RequirementID=1,RequirementAbbrev(unique,max 6)=Mobile,RequirementName(unique, max 20)=44-643 or 44-644},</v>
+        <v>new Models.Requirement {RequirementID=1,RequirementAbbrev(unique,max 6)=Mobile,RequirementName(unique, max 20)=44-643 or 44-644},</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2044,14 +2050,14 @@
         <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="E10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F10" t="str">
         <f>D10&amp;$A$1&amp;"="&amp;$A$10&amp;","&amp;$B$1&amp;"="&amp;$B$10&amp;","&amp;$C$1&amp;"="&amp;$C$10&amp;$E$2</f>
-        <v>new Requirement {RequirementID=664,RequirementAbbrev(unique,max 6)=UX,RequirementName(unique, max 20)=44-664 UX},</v>
+        <v>new Models.Requirement {RequirementID=664,RequirementAbbrev(unique,max 6)=UX,RequirementName(unique, max 20)=44-664 UX},</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2065,14 +2071,14 @@
         <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="E11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F11" t="str">
         <f>D11&amp;$A$1&amp;"="&amp;$A$11&amp;","&amp;$B$1&amp;"="&amp;$B$11&amp;","&amp;$C$1&amp;"="&amp;$C$11&amp;$E$2</f>
-        <v>new Requirement {RequirementID=10,RequirementAbbrev(unique,max 6)=E1,RequirementName(unique, max 20)=Elective 1},</v>
+        <v>new Models.Requirement {RequirementID=10,RequirementAbbrev(unique,max 6)=E1,RequirementName(unique, max 20)=Elective 1},</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2086,14 +2092,14 @@
         <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="E12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F12" t="str">
         <f>D12&amp;$A$1&amp;"="&amp;$A$12&amp;","&amp;$B$1&amp;"="&amp;$B$12&amp;","&amp;$C$1&amp;"="&amp;$C$12&amp;$E$2</f>
-        <v>new Requirement {RequirementID=20,RequirementAbbrev(unique,max 6)=E2,RequirementName(unique, max 20)=Elective 2},</v>
+        <v>new Models.Requirement {RequirementID=20,RequirementAbbrev(unique,max 6)=E2,RequirementName(unique, max 20)=Elective 2},</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2107,14 +2113,14 @@
         <v>35</v>
       </c>
       <c r="D13" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="E13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F13" t="str">
         <f>D13&amp;$A$1&amp;"="&amp;$A$13&amp;","&amp;$B$1&amp;"="&amp;$B$13&amp;","&amp;$C$1&amp;"="&amp;$C$13&amp;$E$2</f>
-        <v>new Requirement {RequirementID=691,RequirementAbbrev(unique,max 6)=GDP1,RequirementName(unique, max 20)=GDP1},</v>
+        <v>new Models.Requirement {RequirementID=691,RequirementAbbrev(unique,max 6)=GDP1,RequirementName(unique, max 20)=GDP1},</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2128,14 +2134,14 @@
         <v>36</v>
       </c>
       <c r="D14" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="E14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F14" t="str">
         <f>D14&amp;$A$1&amp;"="&amp;$A$14&amp;","&amp;$B$1&amp;"="&amp;$B$14&amp;","&amp;$C$1&amp;"="&amp;$C$14&amp;$E$2</f>
-        <v>new Requirement {RequirementID=692,RequirementAbbrev(unique,max 6)=GDP2,RequirementName(unique, max 20)=GDP2},</v>
+        <v>new Models.Requirement {RequirementID=692,RequirementAbbrev(unique,max 6)=GDP2,RequirementName(unique, max 20)=GDP2},</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -3128,7 +3134,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView topLeftCell="B40" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
@@ -3143,7 +3149,7 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B1" t="s">
         <v>38</v>
@@ -3172,10 +3178,10 @@
         <v>460</v>
       </c>
       <c r="D2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F2" t="str">
         <f>D2&amp;$A$1&amp;"="&amp;A2&amp;","&amp;$B$1&amp;"="&amp;B2&amp;","&amp;$C$1&amp;"="&amp;C2&amp;E3</f>
@@ -3193,13 +3199,13 @@
         <v>356</v>
       </c>
       <c r="D3" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3:F49" si="0">D3&amp;$A$1&amp;"="&amp;A3&amp;","&amp;$B$1&amp;"="&amp;B3&amp;","&amp;$C$1&amp;"="&amp;C3&amp;E4</f>
+        <f t="shared" ref="F3:F48" si="0">D3&amp;$A$1&amp;"="&amp;A3&amp;","&amp;$B$1&amp;"="&amp;B3&amp;","&amp;$C$1&amp;"="&amp;C3&amp;E4</f>
         <v>new Models.DegreeRequirement {DegreeRequirementID=2,DegreeID=1,RequirementID=356},</v>
       </c>
     </row>
@@ -3214,10 +3220,10 @@
         <v>542</v>
       </c>
       <c r="D4" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="0"/>
@@ -3235,10 +3241,10 @@
         <v>563</v>
       </c>
       <c r="D5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="0"/>
@@ -3256,10 +3262,10 @@
         <v>560</v>
       </c>
       <c r="D6" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="0"/>
@@ -3277,10 +3283,10 @@
         <v>555</v>
       </c>
       <c r="D7" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="0"/>
@@ -3298,10 +3304,10 @@
         <v>618</v>
       </c>
       <c r="D8" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="0"/>
@@ -3319,10 +3325,10 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="0"/>
@@ -3340,10 +3346,10 @@
         <v>664</v>
       </c>
       <c r="D10" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="0"/>
@@ -3361,10 +3367,10 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="0"/>
@@ -3382,10 +3388,10 @@
         <v>20</v>
       </c>
       <c r="D12" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="0"/>
@@ -3403,10 +3409,10 @@
         <v>691</v>
       </c>
       <c r="D13" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="0"/>
@@ -3424,10 +3430,10 @@
         <v>692</v>
       </c>
       <c r="D14" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="0"/>
@@ -3445,10 +3451,10 @@
         <v>460</v>
       </c>
       <c r="D15" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="0"/>
@@ -3466,10 +3472,10 @@
         <v>542</v>
       </c>
       <c r="D16" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="0"/>
@@ -3487,10 +3493,10 @@
         <v>563</v>
       </c>
       <c r="D17" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" si="0"/>
@@ -3508,10 +3514,10 @@
         <v>560</v>
       </c>
       <c r="D18" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" si="0"/>
@@ -3529,10 +3535,10 @@
         <v>555</v>
       </c>
       <c r="D19" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" si="0"/>
@@ -3550,10 +3556,10 @@
         <v>618</v>
       </c>
       <c r="D20" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F20" t="str">
         <f t="shared" si="0"/>
@@ -3571,10 +3577,10 @@
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" si="0"/>
@@ -3592,10 +3598,10 @@
         <v>664</v>
       </c>
       <c r="D22" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F22" t="str">
         <f t="shared" si="0"/>
@@ -3613,10 +3619,10 @@
         <v>10</v>
       </c>
       <c r="D23" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F23" t="str">
         <f t="shared" si="0"/>
@@ -3634,10 +3640,10 @@
         <v>20</v>
       </c>
       <c r="D24" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F24" t="str">
         <f t="shared" si="0"/>
@@ -3655,10 +3661,10 @@
         <v>691</v>
       </c>
       <c r="D25" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F25" t="str">
         <f t="shared" si="0"/>
@@ -3676,10 +3682,10 @@
         <v>692</v>
       </c>
       <c r="D26" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" si="0"/>
@@ -3697,10 +3703,10 @@
         <v>356</v>
       </c>
       <c r="D27" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F27" t="str">
         <f t="shared" si="0"/>
@@ -3718,10 +3724,10 @@
         <v>542</v>
       </c>
       <c r="D28" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F28" t="str">
         <f t="shared" si="0"/>
@@ -3739,10 +3745,10 @@
         <v>563</v>
       </c>
       <c r="D29" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F29" t="str">
         <f t="shared" si="0"/>
@@ -3760,10 +3766,10 @@
         <v>560</v>
       </c>
       <c r="D30" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F30" t="str">
         <f t="shared" si="0"/>
@@ -3781,10 +3787,10 @@
         <v>555</v>
       </c>
       <c r="D31" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F31" t="str">
         <f t="shared" si="0"/>
@@ -3802,10 +3808,10 @@
         <v>618</v>
       </c>
       <c r="D32" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E32" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F32" t="str">
         <f t="shared" si="0"/>
@@ -3823,10 +3829,10 @@
         <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F33" t="str">
         <f t="shared" si="0"/>
@@ -3844,10 +3850,10 @@
         <v>664</v>
       </c>
       <c r="D34" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E34" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F34" t="str">
         <f t="shared" si="0"/>
@@ -3865,10 +3871,10 @@
         <v>10</v>
       </c>
       <c r="D35" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E35" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F35" t="str">
         <f t="shared" si="0"/>
@@ -3886,10 +3892,10 @@
         <v>20</v>
       </c>
       <c r="D36" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E36" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F36" t="str">
         <f t="shared" si="0"/>
@@ -3907,10 +3913,10 @@
         <v>691</v>
       </c>
       <c r="D37" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E37" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F37" t="str">
         <f t="shared" si="0"/>
@@ -3928,10 +3934,10 @@
         <v>692</v>
       </c>
       <c r="D38" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E38" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F38" t="str">
         <f t="shared" si="0"/>
@@ -3949,10 +3955,10 @@
         <v>542</v>
       </c>
       <c r="D39" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E39" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F39" t="str">
         <f t="shared" si="0"/>
@@ -3970,10 +3976,10 @@
         <v>563</v>
       </c>
       <c r="D40" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E40" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F40" t="str">
         <f t="shared" si="0"/>
@@ -3991,10 +3997,10 @@
         <v>560</v>
       </c>
       <c r="D41" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E41" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F41" t="str">
         <f t="shared" si="0"/>
@@ -4012,10 +4018,10 @@
         <v>555</v>
       </c>
       <c r="D42" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E42" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F42" t="str">
         <f t="shared" si="0"/>
@@ -4033,10 +4039,10 @@
         <v>618</v>
       </c>
       <c r="D43" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E43" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F43" t="str">
         <f t="shared" si="0"/>
@@ -4054,10 +4060,10 @@
         <v>1</v>
       </c>
       <c r="D44" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E44" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F44" t="str">
         <f t="shared" si="0"/>
@@ -4075,10 +4081,10 @@
         <v>664</v>
       </c>
       <c r="D45" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E45" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F45" t="str">
         <f t="shared" si="0"/>
@@ -4096,10 +4102,10 @@
         <v>10</v>
       </c>
       <c r="D46" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F46" t="str">
         <f t="shared" si="0"/>
@@ -4117,10 +4123,10 @@
         <v>20</v>
       </c>
       <c r="D47" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E47" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F47" t="str">
         <f t="shared" si="0"/>
@@ -4138,10 +4144,10 @@
         <v>691</v>
       </c>
       <c r="D48" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E48" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F48" t="str">
         <f t="shared" si="0"/>
@@ -4159,10 +4165,10 @@
         <v>692</v>
       </c>
       <c r="D49" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E49" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F49" t="str">
         <f>D49&amp;$A$1&amp;"="&amp;A49&amp;","&amp;$B$1&amp;"="&amp;B49&amp;","&amp;$C$1&amp;"="&amp;C49&amp;E50</f>
@@ -5130,8 +5136,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView topLeftCell="C121" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -5154,7 +5160,7 @@
         <v>43</v>
       </c>
       <c r="C1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -5183,14 +5189,14 @@
         <v>460</v>
       </c>
       <c r="E2" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G2" t="str">
         <f>E2&amp;$A$1&amp;"="&amp;$A$2&amp;","&amp;$B$1&amp;"="&amp;$B$2&amp;","&amp;$C$1&amp;"="&amp;$C$2&amp;","&amp;$D$1&amp;"="&amp;$D$2&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=1,DegreePlanID=20,TermID=1,RequirementID=460},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=1,DegreePlanID=20,TermID=1,RequirementID=460},</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -5207,14 +5213,14 @@
         <v>356</v>
       </c>
       <c r="E3" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G3" t="str">
         <f>E3&amp;$A$1&amp;"="&amp;$A$3&amp;","&amp;$B$1&amp;"="&amp;$B$3&amp;","&amp;$C$1&amp;"="&amp;$C$3&amp;","&amp;$D$1&amp;"="&amp;$D$3&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -5231,14 +5237,14 @@
         <v>542</v>
       </c>
       <c r="E4" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G4" t="str">
         <f>E4&amp;$A$1&amp;"="&amp;$A$4&amp;","&amp;$B$1&amp;"="&amp;$B$4&amp;","&amp;$C$1&amp;"="&amp;$C$4&amp;","&amp;$D$1&amp;"="&amp;$D$4&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=3,DegreePlanID=20,TermID=1,RequirementID=542},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=3,DegreePlanID=20,TermID=1,RequirementID=542},</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -5255,14 +5261,14 @@
         <v>563</v>
       </c>
       <c r="E5" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G5" t="str">
         <f>E5&amp;$A$1&amp;"="&amp;$A$5&amp;","&amp;$B$1&amp;"="&amp;$B$5&amp;","&amp;$C$1&amp;"="&amp;$C$5&amp;","&amp;$D$1&amp;"="&amp;$D$5&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=4,DegreePlanID=20,TermID=1,RequirementID=563},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=4,DegreePlanID=20,TermID=1,RequirementID=563},</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -5279,14 +5285,14 @@
         <v>560</v>
       </c>
       <c r="E6" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G6" t="str">
         <f>E6&amp;$A$1&amp;"="&amp;$A$6&amp;","&amp;$B$1&amp;"="&amp;$B$6&amp;","&amp;$C$1&amp;"="&amp;$C$6&amp;","&amp;$D$1&amp;"="&amp;$D$6&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=5,DegreePlanID=20,TermID=2,RequirementID=560},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=5,DegreePlanID=20,TermID=2,RequirementID=560},</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -5303,14 +5309,14 @@
         <v>555</v>
       </c>
       <c r="E7" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G7" t="str">
         <f>E7&amp;$A$1&amp;"="&amp;$A$7&amp;","&amp;$B$1&amp;"="&amp;$B$7&amp;","&amp;$C$1&amp;"="&amp;$C$7&amp;","&amp;$D$1&amp;"="&amp;$D$7&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=6,DegreePlanID=20,TermID=2,RequirementID=555},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=6,DegreePlanID=20,TermID=2,RequirementID=555},</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -5327,14 +5333,14 @@
         <v>618</v>
       </c>
       <c r="E8" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G8" t="str">
         <f>E8&amp;$A$1&amp;"="&amp;$A$8&amp;","&amp;$B$1&amp;"="&amp;$B$8&amp;","&amp;$C$1&amp;"="&amp;$C$8&amp;","&amp;$D$1&amp;"="&amp;$D$8&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=7,DegreePlanID=20,TermID=2,RequirementID=618},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=7,DegreePlanID=20,TermID=2,RequirementID=618},</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -5351,14 +5357,14 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G9" t="str">
         <f>E9&amp;$A$1&amp;"="&amp;$A$9&amp;","&amp;$B$1&amp;"="&amp;$B$9&amp;","&amp;$C$1&amp;"="&amp;$C$9&amp;","&amp;$D$1&amp;"="&amp;$D$9&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=8,DegreePlanID=20,TermID=3,RequirementID=1},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=8,DegreePlanID=20,TermID=3,RequirementID=1},</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -5375,14 +5381,14 @@
         <v>664</v>
       </c>
       <c r="E10" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G10" t="str">
         <f>E10&amp;$A$1&amp;"="&amp;$A$10&amp;","&amp;$B$1&amp;"="&amp;$B$10&amp;","&amp;$C$1&amp;"="&amp;$C$10&amp;","&amp;$D$1&amp;"="&amp;$D$10&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=9,DegreePlanID=20,TermID=3,RequirementID=664},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=9,DegreePlanID=20,TermID=3,RequirementID=664},</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -5399,14 +5405,14 @@
         <v>691</v>
       </c>
       <c r="E11" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G11" t="str">
         <f>E11&amp;$A$1&amp;"="&amp;$A$11&amp;","&amp;$B$1&amp;"="&amp;$B$11&amp;","&amp;$C$1&amp;"="&amp;$C$11&amp;","&amp;$D$1&amp;"="&amp;$D$11&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=10,DegreePlanID=20,TermID=3,RequirementID=691},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=10,DegreePlanID=20,TermID=3,RequirementID=691},</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -5423,14 +5429,14 @@
         <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G12" t="str">
         <f>E12&amp;$A$1&amp;"="&amp;$A$12&amp;","&amp;$B$1&amp;"="&amp;$B$12&amp;","&amp;$C$1&amp;"="&amp;$C$12&amp;","&amp;$D$1&amp;"="&amp;$D$12&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=11,DegreePlanID=20,TermID=4,RequirementID=10},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=11,DegreePlanID=20,TermID=4,RequirementID=10},</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -5447,14 +5453,14 @@
         <v>20</v>
       </c>
       <c r="E13" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G13" t="str">
         <f>E13&amp;$A$1&amp;"="&amp;$A$13&amp;","&amp;$B$1&amp;"="&amp;$B$13&amp;","&amp;$C$1&amp;"="&amp;$C$13&amp;","&amp;$D$1&amp;"="&amp;$D$13&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=12,DegreePlanID=20,TermID=4,RequirementID=20},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=12,DegreePlanID=20,TermID=4,RequirementID=20},</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -5471,14 +5477,14 @@
         <v>692</v>
       </c>
       <c r="E14" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G14" t="str">
         <f>E14&amp;$A$1&amp;"="&amp;$A$14&amp;","&amp;$B$1&amp;"="&amp;$B$14&amp;","&amp;$C$1&amp;"="&amp;$C$14&amp;","&amp;$D$1&amp;"="&amp;$D$14&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=13,DegreePlanID=20,TermID=5,RequirementID=692},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=13,DegreePlanID=20,TermID=5,RequirementID=692},</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -5495,14 +5501,14 @@
         <v>460</v>
       </c>
       <c r="E15" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G15" t="str">
         <f>E15&amp;$A$1&amp;"="&amp;$A$15&amp;","&amp;$B$1&amp;"="&amp;$B$15&amp;","&amp;$C$1&amp;"="&amp;$C$15&amp;","&amp;$D$1&amp;"="&amp;$D$15&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=14,DegreePlanID=21,TermID=1,RequirementID=460},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=14,DegreePlanID=21,TermID=1,RequirementID=460},</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -5519,14 +5525,14 @@
         <v>356</v>
       </c>
       <c r="E16" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G16" t="str">
         <f>E16&amp;$A$1&amp;"="&amp;$A$16&amp;","&amp;$B$1&amp;"="&amp;$B$16&amp;","&amp;$C$1&amp;"="&amp;$C$16&amp;","&amp;$D$1&amp;"="&amp;$D$16&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=15,DegreePlanID=21,TermID=1,RequirementID=356},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=15,DegreePlanID=21,TermID=1,RequirementID=356},</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -5543,14 +5549,14 @@
         <v>542</v>
       </c>
       <c r="E17" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G17" t="str">
         <f>E17&amp;$A$1&amp;"="&amp;$A$17&amp;","&amp;$B$1&amp;"="&amp;$B$17&amp;","&amp;$C$1&amp;"="&amp;$C$17&amp;","&amp;$D$1&amp;"="&amp;$D$17&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=16,DegreePlanID=21,TermID=1,RequirementID=542},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=16,DegreePlanID=21,TermID=1,RequirementID=542},</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -5567,14 +5573,14 @@
         <v>563</v>
       </c>
       <c r="E18" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G18" t="str">
         <f>E18&amp;$A$1&amp;"="&amp;$A$18&amp;","&amp;$B$1&amp;"="&amp;$B$18&amp;","&amp;$C$1&amp;"="&amp;$C$18&amp;","&amp;$D$1&amp;"="&amp;$D$18&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=17,DegreePlanID=21,TermID=1,RequirementID=563},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=17,DegreePlanID=21,TermID=1,RequirementID=563},</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -5591,14 +5597,14 @@
         <v>560</v>
       </c>
       <c r="E19" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G19" t="str">
         <f>E19&amp;$A$1&amp;"="&amp;$A$19&amp;","&amp;$B$1&amp;"="&amp;$B$19&amp;","&amp;$C$1&amp;"="&amp;$C$19&amp;","&amp;$D$1&amp;"="&amp;$D$19&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=18,DegreePlanID=21,TermID=2,RequirementID=560},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=18,DegreePlanID=21,TermID=2,RequirementID=560},</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -5615,14 +5621,14 @@
         <v>555</v>
       </c>
       <c r="E20" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G20" t="str">
         <f>E20&amp;$A$1&amp;"="&amp;$A$20&amp;","&amp;$B$1&amp;"="&amp;$B$20&amp;","&amp;$C$1&amp;"="&amp;$C$20&amp;","&amp;$D$1&amp;"="&amp;$D$20&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=19,DegreePlanID=21,TermID=2,RequirementID=555},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=19,DegreePlanID=21,TermID=2,RequirementID=555},</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1">
@@ -5639,14 +5645,14 @@
         <v>618</v>
       </c>
       <c r="E21" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G21" t="str">
         <f>E21&amp;$A$1&amp;"="&amp;$A$21&amp;","&amp;$B$1&amp;"="&amp;$B$21&amp;","&amp;$C$1&amp;"="&amp;$C$21&amp;","&amp;$D$1&amp;"="&amp;$D$21&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=20,DegreePlanID=21,TermID=2,RequirementID=618},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=20,DegreePlanID=21,TermID=2,RequirementID=618},</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1">
@@ -5663,14 +5669,14 @@
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G22" t="str">
         <f>E22&amp;$A$1&amp;"="&amp;$A$22&amp;","&amp;$B$1&amp;"="&amp;$B$22&amp;","&amp;$C$1&amp;"="&amp;$C$22&amp;","&amp;$D$1&amp;"="&amp;$D$22&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=21,DegreePlanID=21,TermID=4,RequirementID=1},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=21,DegreePlanID=21,TermID=4,RequirementID=1},</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1">
@@ -5687,14 +5693,14 @@
         <v>664</v>
       </c>
       <c r="E23" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G23" t="str">
         <f>E23&amp;$A$1&amp;"="&amp;$A$23&amp;","&amp;$B$1&amp;"="&amp;$B$23&amp;","&amp;$C$1&amp;"="&amp;$C$23&amp;","&amp;$D$1&amp;"="&amp;$D$23&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=22,DegreePlanID=21,TermID=4,RequirementID=664},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=22,DegreePlanID=21,TermID=4,RequirementID=664},</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1">
@@ -5711,14 +5717,14 @@
         <v>691</v>
       </c>
       <c r="E24" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G24" t="str">
         <f>E24&amp;$A$1&amp;"="&amp;$A$24&amp;","&amp;$B$1&amp;"="&amp;$B$24&amp;","&amp;$C$1&amp;"="&amp;$C$24&amp;","&amp;$D$1&amp;"="&amp;$D$24&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=23,DegreePlanID=21,TermID=4,RequirementID=691},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=23,DegreePlanID=21,TermID=4,RequirementID=691},</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1">
@@ -5735,14 +5741,14 @@
         <v>10</v>
       </c>
       <c r="E25" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G25" t="str">
         <f>E25&amp;$A$1&amp;"="&amp;$A$25&amp;","&amp;$B$1&amp;"="&amp;$B$25&amp;","&amp;$C$1&amp;"="&amp;$C$25&amp;","&amp;$D$1&amp;"="&amp;$D$25&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=24,DegreePlanID=21,TermID=5,RequirementID=10},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=24,DegreePlanID=21,TermID=5,RequirementID=10},</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1">
@@ -5759,14 +5765,14 @@
         <v>20</v>
       </c>
       <c r="E26" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G26" t="str">
         <f>E26&amp;$A$1&amp;"="&amp;$A$26&amp;","&amp;$B$1&amp;"="&amp;$B$26&amp;","&amp;$C$1&amp;"="&amp;$C$26&amp;","&amp;$D$1&amp;"="&amp;$D$26&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=25,DegreePlanID=21,TermID=5,RequirementID=20},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=25,DegreePlanID=21,TermID=5,RequirementID=20},</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1">
@@ -5783,14 +5789,14 @@
         <v>692</v>
       </c>
       <c r="E27" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G27" t="str">
         <f>E27&amp;$A$1&amp;"="&amp;$A$27&amp;","&amp;$B$1&amp;"="&amp;$B$27&amp;","&amp;$C$1&amp;"="&amp;$C$27&amp;","&amp;$D$1&amp;"="&amp;$D$27&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=26,DegreePlanID=21,TermID=5,RequirementID=692},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=26,DegreePlanID=21,TermID=5,RequirementID=692},</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1">
@@ -5807,14 +5813,14 @@
         <v>460</v>
       </c>
       <c r="E28" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G28" t="str">
         <f>E28&amp;$A$1&amp;"="&amp;$A$28&amp;","&amp;$B$1&amp;"="&amp;$B$28&amp;","&amp;$C$1&amp;"="&amp;$C$28&amp;","&amp;$D$1&amp;"="&amp;$D$28&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=27,DegreePlanID=12,TermID=1,RequirementID=460},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=27,DegreePlanID=12,TermID=1,RequirementID=460},</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1">
@@ -5831,14 +5837,14 @@
         <v>356</v>
       </c>
       <c r="E29" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G29" t="str">
         <f>E29&amp;$A$1&amp;"="&amp;$A$29&amp;","&amp;$B$1&amp;"="&amp;$B$29&amp;","&amp;$C$1&amp;"="&amp;$C$29&amp;","&amp;$D$1&amp;"="&amp;$D$29&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=28,DegreePlanID=12,TermID=1,RequirementID=356},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=28,DegreePlanID=12,TermID=1,RequirementID=356},</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1">
@@ -5855,14 +5861,14 @@
         <v>542</v>
       </c>
       <c r="E30" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G30" t="str">
         <f>E30&amp;$A$1&amp;"="&amp;$A$30&amp;","&amp;$B$1&amp;"="&amp;$B$30&amp;","&amp;$C$1&amp;"="&amp;$C$30&amp;","&amp;$D$1&amp;"="&amp;$D$30&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=29,DegreePlanID=12,TermID=1,RequirementID=542},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=29,DegreePlanID=12,TermID=1,RequirementID=542},</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1">
@@ -5879,14 +5885,14 @@
         <v>563</v>
       </c>
       <c r="E31" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G31" t="str">
         <f>E31&amp;$A$1&amp;"="&amp;$A$31&amp;","&amp;$B$1&amp;"="&amp;$B$31&amp;","&amp;$C$1&amp;"="&amp;$C$31&amp;","&amp;$D$1&amp;"="&amp;$D$31&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=30,DegreePlanID=12,TermID=1,RequirementID=563},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=30,DegreePlanID=12,TermID=1,RequirementID=563},</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="15.75" customHeight="1">
@@ -5903,14 +5909,14 @@
         <v>560</v>
       </c>
       <c r="E32" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F32" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G32" t="str">
         <f>E32&amp;$A$1&amp;"="&amp;$A$32&amp;","&amp;$B$1&amp;"="&amp;$B$32&amp;","&amp;$C$1&amp;"="&amp;$C$32&amp;","&amp;$D$1&amp;"="&amp;$D$32&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=31,DegreePlanID=12,TermID=2,RequirementID=560},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=31,DegreePlanID=12,TermID=2,RequirementID=560},</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="15.75" customHeight="1">
@@ -5927,14 +5933,14 @@
         <v>555</v>
       </c>
       <c r="E33" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G33" t="str">
         <f>E33&amp;$A$1&amp;"="&amp;$A$33&amp;","&amp;$B$1&amp;"="&amp;$B$33&amp;","&amp;$C$1&amp;"="&amp;$C$33&amp;","&amp;$D$1&amp;"="&amp;$D$33&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=32,DegreePlanID=12,TermID=2,RequirementID=555},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=32,DegreePlanID=12,TermID=2,RequirementID=555},</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="15.75" customHeight="1">
@@ -5951,14 +5957,14 @@
         <v>618</v>
       </c>
       <c r="E34" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F34" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G34" t="str">
         <f>E34&amp;$A$1&amp;"="&amp;$A$34&amp;","&amp;$B$1&amp;"="&amp;$B$34&amp;","&amp;$C$1&amp;"="&amp;$C$34&amp;","&amp;$D$1&amp;"="&amp;$D$34&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=33,DegreePlanID=12,TermID=2,RequirementID=618},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=33,DegreePlanID=12,TermID=2,RequirementID=618},</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="15.75" customHeight="1">
@@ -5975,14 +5981,14 @@
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F35" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G35" t="str">
         <f>E35&amp;$A$1&amp;"="&amp;$A$35&amp;","&amp;$B$1&amp;"="&amp;$B$35&amp;","&amp;$C$1&amp;"="&amp;$C$35&amp;","&amp;$D$1&amp;"="&amp;$D$35&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=34,DegreePlanID=12,TermID=3,RequirementID=1},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=34,DegreePlanID=12,TermID=3,RequirementID=1},</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="15.75" customHeight="1">
@@ -5999,14 +6005,14 @@
         <v>664</v>
       </c>
       <c r="E36" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F36" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G36" t="str">
         <f>E36&amp;$A$1&amp;"="&amp;$A$36&amp;","&amp;$B$1&amp;"="&amp;$B$36&amp;","&amp;$C$1&amp;"="&amp;$C$36&amp;","&amp;$D$1&amp;"="&amp;$D$36&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=35,DegreePlanID=12,TermID=3,RequirementID=664},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=35,DegreePlanID=12,TermID=3,RequirementID=664},</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="15.75" customHeight="1">
@@ -6023,14 +6029,14 @@
         <v>691</v>
       </c>
       <c r="E37" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F37" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G37" t="str">
         <f>E37&amp;$A$1&amp;"="&amp;$A$37&amp;","&amp;$B$1&amp;"="&amp;$B$37&amp;","&amp;$C$1&amp;"="&amp;$C$37&amp;","&amp;$D$1&amp;"="&amp;$D$37&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=36,DegreePlanID=12,TermID=4,RequirementID=691},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=36,DegreePlanID=12,TermID=4,RequirementID=691},</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="15.75" customHeight="1">
@@ -6047,14 +6053,14 @@
         <v>10</v>
       </c>
       <c r="E38" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F38" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G38" t="str">
         <f>E38&amp;$A$1&amp;"="&amp;$A$38&amp;","&amp;$B$1&amp;"="&amp;$B$38&amp;","&amp;$C$1&amp;"="&amp;$C$38&amp;","&amp;$D$1&amp;"="&amp;$D$38&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=37,DegreePlanID=12,TermID=4,RequirementID=10},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=37,DegreePlanID=12,TermID=4,RequirementID=10},</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="15.75" customHeight="1">
@@ -6071,14 +6077,14 @@
         <v>20</v>
       </c>
       <c r="E39" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F39" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G39" t="str">
         <f>E39&amp;$A$1&amp;"="&amp;$A$39&amp;","&amp;$B$1&amp;"="&amp;$B$39&amp;","&amp;$C$1&amp;"="&amp;$C$39&amp;","&amp;$D$1&amp;"="&amp;$D$39&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=38,DegreePlanID=12,TermID=4,RequirementID=20},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=38,DegreePlanID=12,TermID=4,RequirementID=20},</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="15.75" customHeight="1">
@@ -6095,14 +6101,14 @@
         <v>692</v>
       </c>
       <c r="E40" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F40" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G40" t="str">
         <f>E40&amp;$A$1&amp;"="&amp;$A$40&amp;","&amp;$B$1&amp;"="&amp;$B$40&amp;","&amp;$C$1&amp;"="&amp;$C$40&amp;","&amp;$D$1&amp;"="&amp;$D$40&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=39,DegreePlanID=12,TermID=5,RequirementID=692},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=39,DegreePlanID=12,TermID=5,RequirementID=692},</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="15.75" customHeight="1">
@@ -6119,14 +6125,14 @@
         <v>460</v>
       </c>
       <c r="E41" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F41" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G41" t="str">
         <f>E41&amp;$A$1&amp;"="&amp;$A$41&amp;","&amp;$B$1&amp;"="&amp;$B$41&amp;","&amp;$C$1&amp;"="&amp;$C$41&amp;","&amp;$D$1&amp;"="&amp;$D$41&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=40,DegreePlanID=13,TermID=1,RequirementID=460},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=40,DegreePlanID=13,TermID=1,RequirementID=460},</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="15.75" customHeight="1">
@@ -6143,14 +6149,14 @@
         <v>356</v>
       </c>
       <c r="E42" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F42" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G42" t="str">
         <f>E42&amp;$A$1&amp;"="&amp;$A$42&amp;","&amp;$B$1&amp;"="&amp;$B$42&amp;","&amp;$C$1&amp;"="&amp;$C$42&amp;","&amp;$D$1&amp;"="&amp;$D$42&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=41,DegreePlanID=13,TermID=1,RequirementID=356},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=41,DegreePlanID=13,TermID=1,RequirementID=356},</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="15.75" customHeight="1">
@@ -6167,14 +6173,14 @@
         <v>542</v>
       </c>
       <c r="E43" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F43" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G43" t="str">
         <f>E43&amp;$A$1&amp;"="&amp;$A$43&amp;","&amp;$B$1&amp;"="&amp;$B$43&amp;","&amp;$C$1&amp;"="&amp;$C$43&amp;","&amp;$D$1&amp;"="&amp;$D$43&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=42,DegreePlanID=13,TermID=1,RequirementID=542},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=42,DegreePlanID=13,TermID=1,RequirementID=542},</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="15.75" customHeight="1">
@@ -6191,14 +6197,14 @@
         <v>563</v>
       </c>
       <c r="E44" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F44" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G44" t="str">
         <f>E44&amp;$A$1&amp;"="&amp;$A$44&amp;","&amp;$B$1&amp;"="&amp;$B$44&amp;","&amp;$C$1&amp;"="&amp;$C$44&amp;","&amp;$D$1&amp;"="&amp;$D$44&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=43,DegreePlanID=13,TermID=1,RequirementID=563},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=43,DegreePlanID=13,TermID=1,RequirementID=563},</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="15.75" customHeight="1">
@@ -6215,14 +6221,14 @@
         <v>560</v>
       </c>
       <c r="E45" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F45" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G45" t="str">
         <f>E45&amp;$A$1&amp;"="&amp;$A$45&amp;","&amp;$B$1&amp;"="&amp;$B$45&amp;","&amp;$C$1&amp;"="&amp;$C$45&amp;","&amp;$D$1&amp;"="&amp;$D$45&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=44,DegreePlanID=13,TermID=3,RequirementID=560},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=44,DegreePlanID=13,TermID=3,RequirementID=560},</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="15.75" customHeight="1">
@@ -6239,14 +6245,14 @@
         <v>555</v>
       </c>
       <c r="E46" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G46" t="str">
         <f>E46&amp;$A$1&amp;"="&amp;$A$46&amp;","&amp;$B$1&amp;"="&amp;$B$46&amp;","&amp;$C$1&amp;"="&amp;$C$46&amp;","&amp;$D$1&amp;"="&amp;$D$46&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=45,DegreePlanID=13,TermID=3,RequirementID=555},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=45,DegreePlanID=13,TermID=3,RequirementID=555},</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="15.75" customHeight="1">
@@ -6263,14 +6269,14 @@
         <v>618</v>
       </c>
       <c r="E47" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F47" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G47" t="str">
         <f>E47&amp;$A$1&amp;"="&amp;$A$47&amp;","&amp;$B$1&amp;"="&amp;$B$47&amp;","&amp;$C$1&amp;"="&amp;$C$47&amp;","&amp;$D$1&amp;"="&amp;$D$47&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=46,DegreePlanID=13,TermID=3,RequirementID=618},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=46,DegreePlanID=13,TermID=3,RequirementID=618},</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="15.75" customHeight="1">
@@ -6287,14 +6293,14 @@
         <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F48" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G48" t="str">
         <f>E48&amp;$A$1&amp;"="&amp;$A$48&amp;","&amp;$B$1&amp;"="&amp;$B$48&amp;","&amp;$C$1&amp;"="&amp;$C$48&amp;","&amp;$D$1&amp;"="&amp;$D$48&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=47,DegreePlanID=13,TermID=4,RequirementID=1},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=47,DegreePlanID=13,TermID=4,RequirementID=1},</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="15.75" customHeight="1">
@@ -6311,14 +6317,14 @@
         <v>664</v>
       </c>
       <c r="E49" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F49" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G49" t="str">
         <f>E49&amp;$A$1&amp;"="&amp;$A$49&amp;","&amp;$B$1&amp;"="&amp;$B$49&amp;","&amp;$C$1&amp;"="&amp;$C$49&amp;","&amp;$D$1&amp;"="&amp;$D$49&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=48,DegreePlanID=13,TermID=4,RequirementID=664},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=48,DegreePlanID=13,TermID=4,RequirementID=664},</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="15.75" customHeight="1">
@@ -6335,14 +6341,14 @@
         <v>691</v>
       </c>
       <c r="E50" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F50" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G50" t="str">
         <f>E50&amp;$A$1&amp;"="&amp;$A$50&amp;","&amp;$B$1&amp;"="&amp;$B$50&amp;","&amp;$C$1&amp;"="&amp;$C$50&amp;","&amp;$D$1&amp;"="&amp;$D$50&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=49,DegreePlanID=13,TermID=4,RequirementID=691},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=49,DegreePlanID=13,TermID=4,RequirementID=691},</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="15.75" customHeight="1">
@@ -6359,14 +6365,14 @@
         <v>10</v>
       </c>
       <c r="E51" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F51" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G51" t="str">
         <f>E51&amp;$A$1&amp;"="&amp;$A$51&amp;","&amp;$B$1&amp;"="&amp;$B$51&amp;","&amp;$C$1&amp;"="&amp;$C$51&amp;","&amp;$D$1&amp;"="&amp;$D$51&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=50,DegreePlanID=13,TermID=5,RequirementID=10},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=50,DegreePlanID=13,TermID=5,RequirementID=10},</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="15.75" customHeight="1">
@@ -6383,14 +6389,14 @@
         <v>20</v>
       </c>
       <c r="E52" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F52" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G52" t="str">
         <f>E52&amp;$A$1&amp;"="&amp;$A$52&amp;","&amp;$B$1&amp;"="&amp;$B$52&amp;","&amp;$C$1&amp; "="&amp;$C$52&amp;","&amp;$D$1&amp;"="&amp;$D$52&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=51,DegreePlanID=13,TermID=5,RequirementID=20},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=51,DegreePlanID=13,TermID=5,RequirementID=20},</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="15.75" customHeight="1">
@@ -6407,14 +6413,14 @@
         <v>692</v>
       </c>
       <c r="E53" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F53" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G53" t="str">
         <f>E53&amp;$A$1&amp;"="&amp;$A$53&amp;","&amp;$B$1&amp;"="&amp;$B$53&amp;","&amp;$C$1&amp;"="&amp;$C$53&amp;","&amp;$D$1&amp;"="&amp;$D$53&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=52,DegreePlanID=13,TermID=5,RequirementID=692},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=52,DegreePlanID=13,TermID=5,RequirementID=692},</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="15.75" customHeight="1">
@@ -6431,14 +6437,14 @@
         <v>460</v>
       </c>
       <c r="E54" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F54" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G54" t="str">
         <f>E54&amp;$A$1&amp;"="&amp;$A$54&amp;","&amp;$B$1&amp;"="&amp;$B$54&amp;","&amp;$C$1&amp;"="&amp;$C$54&amp;","&amp;$D$1&amp;"="&amp;$D$54&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=53,DegreePlanID=18,TermID=1,RequirementID=460},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=53,DegreePlanID=18,TermID=1,RequirementID=460},</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="15.75" customHeight="1">
@@ -6455,14 +6461,14 @@
         <v>356</v>
       </c>
       <c r="E55" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F55" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G55" t="str">
         <f>E55&amp;$A$1&amp;"="&amp;$A$55&amp;","&amp;$B$1&amp;"="&amp;$B$55&amp;","&amp;$C$1&amp;"="&amp;$C$55&amp;","&amp;$D$1&amp;"="&amp;$D$55&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=54,DegreePlanID=18,TermID=1,RequirementID=356},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=54,DegreePlanID=18,TermID=1,RequirementID=356},</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="15.75" customHeight="1">
@@ -6479,14 +6485,14 @@
         <v>542</v>
       </c>
       <c r="E56" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F56" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G56" t="str">
         <f>E56&amp;$A$1&amp;"="&amp;$A$56&amp;","&amp;$B$1&amp;"="&amp;$B$56&amp;","&amp;$C$1&amp;"="&amp;$C$56&amp;","&amp;$D$1&amp;"="&amp;$D$56&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=55,DegreePlanID=18,TermID=1,RequirementID=542},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=55,DegreePlanID=18,TermID=1,RequirementID=542},</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="15.75" customHeight="1">
@@ -6503,14 +6509,14 @@
         <v>563</v>
       </c>
       <c r="E57" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F57" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G57" t="str">
         <f>E57&amp;$A$1&amp;"="&amp;$A$57&amp;","&amp;$B$1&amp;"="&amp;$B$57&amp;","&amp;$C$1&amp;"="&amp;$C$57&amp;","&amp;$D$1&amp;"="&amp;$D$57&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=56,DegreePlanID=18,TermID=1,RequirementID=563},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=56,DegreePlanID=18,TermID=1,RequirementID=563},</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="15.75" customHeight="1">
@@ -6527,14 +6533,14 @@
         <v>560</v>
       </c>
       <c r="E58" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F58" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G58" t="str">
         <f>E58&amp;$A$1&amp;"="&amp;$A$58&amp;","&amp;$B$1&amp;"="&amp;$B$58&amp;","&amp;$C$1&amp;"="&amp;$C$58&amp;","&amp;$D$1&amp;"="&amp;$D$58&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=57,DegreePlanID=18,TermID=2,RequirementID=560},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=57,DegreePlanID=18,TermID=2,RequirementID=560},</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="15.75" customHeight="1">
@@ -6551,14 +6557,14 @@
         <v>555</v>
       </c>
       <c r="E59" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F59" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G59" t="str">
         <f>E59&amp;$A$1&amp;"="&amp;$A$59&amp;","&amp;$B$1&amp;"="&amp;$B$59&amp;","&amp;$C$1&amp;"="&amp;$C$59&amp;","&amp;$D$1&amp;"="&amp;$D$59&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=58,DegreePlanID=18,TermID=2,RequirementID=555},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=58,DegreePlanID=18,TermID=2,RequirementID=555},</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="15.75" customHeight="1">
@@ -6575,14 +6581,14 @@
         <v>618</v>
       </c>
       <c r="E60" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F60" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G60" t="str">
         <f>E60&amp;$A$1&amp;"="&amp;$A$60&amp;","&amp;$B$1&amp;"="&amp;$B$60&amp;","&amp;$C$1&amp;"="&amp;$C$60&amp;","&amp;$D$1&amp;"="&amp;$D$60&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=59,DegreePlanID=18,TermID=2,RequirementID=618},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=59,DegreePlanID=18,TermID=2,RequirementID=618},</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="15.75" customHeight="1">
@@ -6599,14 +6605,14 @@
         <v>1</v>
       </c>
       <c r="E61" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F61" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G61" t="str">
         <f>E61&amp;$A$1&amp;"="&amp;$A$61&amp;","&amp;$B$1&amp;"="&amp;$B$61&amp;","&amp;$C$1&amp;"="&amp;$C$61&amp;","&amp;$D$1&amp;"="&amp;$D$61&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=60,DegreePlanID=18,TermID=3,RequirementID=1},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=60,DegreePlanID=18,TermID=3,RequirementID=1},</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="15.75" customHeight="1">
@@ -6623,14 +6629,14 @@
         <v>664</v>
       </c>
       <c r="E62" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F62" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G62" t="str">
         <f>E62&amp;$A$1&amp;"="&amp;$A$62&amp;","&amp;$B$1&amp;"="&amp;$B$62&amp;","&amp;$C$1&amp;"="&amp;$C$62&amp;","&amp;$D$1&amp;"="&amp;$D$62&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=61,DegreePlanID=18,TermID=3,RequirementID=664},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=61,DegreePlanID=18,TermID=3,RequirementID=664},</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="15.75" customHeight="1">
@@ -6647,14 +6653,14 @@
         <v>691</v>
       </c>
       <c r="E63" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F63" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G63" t="str">
         <f>E63&amp;$A$1&amp;"="&amp;$A$63&amp;","&amp;$B$1&amp;"="&amp;$B$63&amp;","&amp;$C$1&amp;"="&amp;$C$63&amp;","&amp;$D$1&amp;"="&amp;$D$63&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=62,DegreePlanID=18,TermID=4,RequirementID=691},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=62,DegreePlanID=18,TermID=4,RequirementID=691},</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="15.75" customHeight="1">
@@ -6671,14 +6677,14 @@
         <v>10</v>
       </c>
       <c r="E64" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F64" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G64" t="str">
         <f>E64&amp;$A$1&amp;"="&amp;$A$64&amp;","&amp;$B$1&amp;"="&amp;$B$64&amp;","&amp;$C$1&amp;"="&amp;$C$64&amp;","&amp;$D$1&amp;"="&amp;$D$64&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=63,DegreePlanID=18,TermID=4,RequirementID=10},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=63,DegreePlanID=18,TermID=4,RequirementID=10},</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="15.75" customHeight="1">
@@ -6695,14 +6701,14 @@
         <v>20</v>
       </c>
       <c r="E65" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F65" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G65" t="str">
         <f>E65&amp;$A$1&amp;"="&amp;$A$65&amp;","&amp;$B$1&amp;"="&amp;$B$65&amp;","&amp;$C$1&amp;"="&amp;$C$65&amp;","&amp;$D$1&amp;"="&amp;$D$65&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=64,DegreePlanID=18,TermID=4,RequirementID=20},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=64,DegreePlanID=18,TermID=4,RequirementID=20},</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="15.75" customHeight="1">
@@ -6719,14 +6725,14 @@
         <v>692</v>
       </c>
       <c r="E66" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F66" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G66" t="str">
         <f>E66&amp;$A$1&amp;"="&amp;$A$66&amp;","&amp;$B$1&amp;"="&amp;$B$66&amp;","&amp;$C$1&amp;"="&amp;$C$66&amp;","&amp;$D$1&amp;"="&amp;$D$66&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=65,DegreePlanID=18,TermID=5,RequirementID=692},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=65,DegreePlanID=18,TermID=5,RequirementID=692},</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="15.75" customHeight="1">
@@ -6743,14 +6749,14 @@
         <v>460</v>
       </c>
       <c r="E67" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F67" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G67" t="str">
         <f>E67&amp;$A$1&amp;"="&amp;$A$67&amp;","&amp;$B$1&amp;"="&amp;$B$67&amp;","&amp;$C$1&amp;"="&amp;$C$67&amp;","&amp;$D$1&amp;"="&amp;$D$67&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=66,DegreePlanID=19,TermID=1,RequirementID=460},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=66,DegreePlanID=19,TermID=1,RequirementID=460},</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="15.75" customHeight="1">
@@ -6767,14 +6773,14 @@
         <v>356</v>
       </c>
       <c r="E68" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F68" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G68" t="str">
         <f>E68&amp;$A$1&amp;"="&amp;$A$68&amp;","&amp;$B$1&amp;"="&amp;$B$68&amp;","&amp;$C$1&amp;"="&amp;$C$68&amp;","&amp;$D$1&amp;"="&amp;$D$68&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=67,DegreePlanID=19,TermID=1,RequirementID=356},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=67,DegreePlanID=19,TermID=1,RequirementID=356},</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="15.75" customHeight="1">
@@ -6791,14 +6797,14 @@
         <v>542</v>
       </c>
       <c r="E69" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F69" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G69" t="str">
         <f>E69&amp;$A$1&amp;"="&amp;$A$69&amp;","&amp;$B$1&amp;"="&amp;$B$69&amp;","&amp;$C$1&amp;"="&amp;$C$69&amp;","&amp;$D$1&amp;"="&amp;$D$69&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=68,DegreePlanID=19,TermID=1,RequirementID=542},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=68,DegreePlanID=19,TermID=1,RequirementID=542},</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="15.75" customHeight="1">
@@ -6815,14 +6821,14 @@
         <v>563</v>
       </c>
       <c r="E70" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F70" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G70" t="str">
         <f>E70&amp;$A$1&amp;"="&amp;$A$70&amp;","&amp;$B$1&amp;"="&amp;$B$70&amp;","&amp;$C$1&amp;"="&amp;$C$70&amp;","&amp;$D$1&amp;"="&amp;$D$70&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=69,DegreePlanID=19,TermID=1,RequirementID=563},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=69,DegreePlanID=19,TermID=1,RequirementID=563},</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="15.75" customHeight="1">
@@ -6839,14 +6845,14 @@
         <v>560</v>
       </c>
       <c r="E71" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F71" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G71" t="str">
         <f>E71&amp;$A$1&amp;"="&amp;$A$71&amp;","&amp;$B$1&amp;"="&amp;$B$71&amp;","&amp;$C$1&amp;"="&amp;$C$71&amp;","&amp;$D$1&amp;"="&amp;$D$71&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=70,DegreePlanID=19,TermID=3,RequirementID=560},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=70,DegreePlanID=19,TermID=3,RequirementID=560},</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="15.75" customHeight="1">
@@ -6863,14 +6869,14 @@
         <v>555</v>
       </c>
       <c r="E72" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F72" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G72" t="str">
         <f>E72&amp;$A$1&amp;"="&amp;$A$72&amp;","&amp;$B$1&amp;"="&amp;$B$72&amp;","&amp;$C$1&amp;"="&amp;$C$72&amp;","&amp;$D$1&amp;"="&amp;$D$72&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=71,DegreePlanID=19,TermID=3,RequirementID=555},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=71,DegreePlanID=19,TermID=3,RequirementID=555},</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="15.75" customHeight="1">
@@ -6887,14 +6893,14 @@
         <v>618</v>
       </c>
       <c r="E73" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F73" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G73" t="str">
         <f>E73&amp;$A$1&amp;"="&amp;$A$73&amp;","&amp;$B$1&amp;"="&amp;$B$73&amp;","&amp;$C$1&amp;"="&amp;$C$73&amp;","&amp;$D$1&amp;"="&amp;$D$73&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=72,DegreePlanID=19,TermID=3,RequirementID=618},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=72,DegreePlanID=19,TermID=3,RequirementID=618},</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="15.75" customHeight="1">
@@ -6911,14 +6917,14 @@
         <v>1</v>
       </c>
       <c r="E74" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F74" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G74" t="str">
         <f>E74&amp;$A$1&amp;"="&amp;$A$74&amp;","&amp;$B$1&amp;"="&amp;$B$74&amp;","&amp;$C$1&amp;"="&amp;$C$74&amp;","&amp;$D$1&amp;"="&amp;$D$74&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=73,DegreePlanID=19,TermID=4,RequirementID=1},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=73,DegreePlanID=19,TermID=4,RequirementID=1},</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="15.75" customHeight="1">
@@ -6935,14 +6941,14 @@
         <v>664</v>
       </c>
       <c r="E75" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F75" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G75" t="str">
         <f>E75&amp;$A$1&amp;"="&amp;$A$75&amp;","&amp;$B$1&amp;"="&amp;$B$75&amp;","&amp;$C$1&amp;"="&amp;$C$75&amp;","&amp;$D$1&amp;"="&amp;$D$75&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=74,DegreePlanID=19,TermID=4,RequirementID=664},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=74,DegreePlanID=19,TermID=4,RequirementID=664},</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="15.75" customHeight="1">
@@ -6959,14 +6965,14 @@
         <v>691</v>
       </c>
       <c r="E76" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F76" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G76" t="str">
         <f>E76&amp;$A$1&amp;"="&amp;$A$76&amp;","&amp;$B$1&amp;"="&amp;$B$76&amp;","&amp;$C$1&amp;"="&amp;$C$76&amp;","&amp;$D$1&amp;"="&amp;$D$76&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=75,DegreePlanID=19,TermID=4,RequirementID=691},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=75,DegreePlanID=19,TermID=4,RequirementID=691},</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="15.75" customHeight="1">
@@ -6983,14 +6989,14 @@
         <v>10</v>
       </c>
       <c r="E77" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F77" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G77" t="str">
         <f>E77&amp;$A$1&amp;"="&amp;$A$77&amp;","&amp;$B$1&amp;"="&amp;$B$77&amp;","&amp;$C$1&amp;"="&amp;$C$77&amp;","&amp;$D$1&amp;"="&amp;$D$77&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=76,DegreePlanID=19,TermID=5,RequirementID=10},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=76,DegreePlanID=19,TermID=5,RequirementID=10},</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="15.75" customHeight="1">
@@ -7007,14 +7013,14 @@
         <v>20</v>
       </c>
       <c r="E78" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F78" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G78" t="str">
         <f>E78&amp;$A$1&amp;"="&amp;$A$78&amp;","&amp;$B$1&amp;"="&amp;$B$78&amp;","&amp;$C$1&amp;"="&amp;$C$78&amp;","&amp;$D$1&amp;"="&amp;$D$78&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=77,DegreePlanID=19,TermID=5,RequirementID=20},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=77,DegreePlanID=19,TermID=5,RequirementID=20},</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="15.75" customHeight="1">
@@ -7031,14 +7037,14 @@
         <v>692</v>
       </c>
       <c r="E79" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F79" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G79" t="str">
         <f>E79&amp;$A$1&amp;"="&amp;$A$79&amp;","&amp;$B$1&amp;"="&amp;$B$79&amp;","&amp;$C$1&amp;"="&amp;$C$79&amp;","&amp;$D$1&amp;"="&amp;$D$79&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=78,DegreePlanID=19,TermID=5,RequirementID=692},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=78,DegreePlanID=19,TermID=5,RequirementID=692},</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="15.75" customHeight="1">
@@ -7055,14 +7061,14 @@
         <v>460</v>
       </c>
       <c r="E80" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F80" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G80" t="str">
         <f>E80&amp;$A$1&amp;"="&amp;$A$80&amp;","&amp;$B$1&amp;"="&amp;$B$80&amp;","&amp;$C$1&amp;"="&amp;$C$80&amp;","&amp;$D$1&amp;"="&amp;$D$80&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=79,DegreePlanID=16,TermID=1,RequirementID=460},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=79,DegreePlanID=16,TermID=1,RequirementID=460},</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="15.75" customHeight="1">
@@ -7079,14 +7085,14 @@
         <v>356</v>
       </c>
       <c r="E81" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F81" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G81" t="str">
         <f>E81&amp;$A$1&amp;"="&amp;$A$81&amp;","&amp;$B$1&amp;"="&amp;$B$81&amp;","&amp;$C$1&amp;"="&amp;$C$81&amp;","&amp;$D$1&amp;"="&amp;$D$81&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=80,DegreePlanID=16,TermID=1,RequirementID=356},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=80,DegreePlanID=16,TermID=1,RequirementID=356},</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="15.75" customHeight="1">
@@ -7103,14 +7109,14 @@
         <v>542</v>
       </c>
       <c r="E82" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F82" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G82" t="str">
         <f>E82&amp;$A$1&amp;"="&amp;$A$82&amp;","&amp;$B$1&amp;"="&amp;$B$82&amp;","&amp;$C$1&amp;"="&amp;$C$82&amp;","&amp;$D$1&amp;"="&amp;$D$82&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=81,DegreePlanID=16,TermID=1,RequirementID=542},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=81,DegreePlanID=16,TermID=1,RequirementID=542},</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="15.75" customHeight="1">
@@ -7127,14 +7133,14 @@
         <v>563</v>
       </c>
       <c r="E83" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F83" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G83" t="str">
         <f>E83&amp;$A$1&amp;"="&amp;$A$83&amp;","&amp;$B$1&amp;"="&amp;$B$83&amp;","&amp;$C$1&amp;"="&amp;$C$83&amp;","&amp;$D$1&amp;"="&amp;$D$83&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=82,DegreePlanID=16,TermID=1,RequirementID=563},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=82,DegreePlanID=16,TermID=1,RequirementID=563},</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="15.75" customHeight="1">
@@ -7151,14 +7157,14 @@
         <v>560</v>
       </c>
       <c r="E84" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F84" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G84" t="str">
         <f>E84&amp;$A$1&amp;"="&amp;$A$84&amp;","&amp;$B$1&amp;"="&amp;$B$84&amp;","&amp;$C$1&amp;"="&amp;$C$84&amp;","&amp;$D$1&amp;"="&amp;$D$84&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=83,DegreePlanID=16,TermID=2,RequirementID=560},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=83,DegreePlanID=16,TermID=2,RequirementID=560},</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="15.75" customHeight="1">
@@ -7175,14 +7181,14 @@
         <v>555</v>
       </c>
       <c r="E85" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F85" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G85" t="str">
         <f>E85&amp;$A$1&amp;"="&amp;$A$85&amp;","&amp;$B$1&amp;"="&amp;$B$85&amp;","&amp;$C$1&amp;"="&amp;$C$85&amp;","&amp;$D$1&amp;"="&amp;$D$85&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=84,DegreePlanID=16,TermID=2,RequirementID=555},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=84,DegreePlanID=16,TermID=2,RequirementID=555},</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="15.75" customHeight="1">
@@ -7199,14 +7205,14 @@
         <v>618</v>
       </c>
       <c r="E86" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F86" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G86" t="str">
         <f>E86&amp;$A$1&amp;"="&amp;$A$86&amp;","&amp;$B$1&amp;"="&amp;$B$86&amp;","&amp;$C$1&amp;"="&amp;$C$86&amp;","&amp;$D$1&amp;"="&amp;$D$86&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=85,DegreePlanID=16,TermID=2,RequirementID=618},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=85,DegreePlanID=16,TermID=2,RequirementID=618},</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="15.75" customHeight="1">
@@ -7223,14 +7229,14 @@
         <v>1</v>
       </c>
       <c r="E87" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F87" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G87" t="str">
         <f>E87&amp;$A$1&amp;"="&amp;$A$87&amp;","&amp;$B$1&amp;"="&amp;$B$87&amp;","&amp;$C$1&amp;"="&amp;$C$87&amp;","&amp;$D$1&amp;"="&amp;$D$87&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=86,DegreePlanID=16,TermID=3,RequirementID=1},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=86,DegreePlanID=16,TermID=3,RequirementID=1},</v>
       </c>
     </row>
     <row r="88" spans="1:7" ht="15.75" customHeight="1">
@@ -7247,14 +7253,14 @@
         <v>664</v>
       </c>
       <c r="E88" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F88" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G88" t="str">
         <f>E88&amp;$A$1&amp;"="&amp;$A$88&amp;","&amp;$B$1&amp;"="&amp;$B$88&amp;","&amp;$C$1&amp;"="&amp;$C$88&amp;","&amp;$D$1&amp;"="&amp;$D$88&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=87,DegreePlanID=16,TermID=3,RequirementID=664},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=87,DegreePlanID=16,TermID=3,RequirementID=664},</v>
       </c>
     </row>
     <row r="89" spans="1:7" ht="15.75" customHeight="1">
@@ -7271,14 +7277,14 @@
         <v>691</v>
       </c>
       <c r="E89" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F89" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G89" t="str">
         <f>E89&amp;$A$1&amp;"="&amp;$A$89&amp;","&amp;$B$1&amp;"="&amp;$B$89&amp;","&amp;$C$1&amp;"="&amp;$C$89&amp;","&amp;$D$1&amp;"="&amp;$D$89&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=88,DegreePlanID=16,TermID=3,RequirementID=691},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=88,DegreePlanID=16,TermID=3,RequirementID=691},</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="15.75" customHeight="1">
@@ -7295,14 +7301,14 @@
         <v>10</v>
       </c>
       <c r="E90" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F90" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G90" t="str">
         <f>E90&amp;$A$1&amp;"="&amp;$A$90&amp;","&amp;$B$1&amp;"="&amp;$B$90&amp;","&amp;$C$1&amp;"="&amp;$C$90&amp;","&amp;$D$1&amp;"="&amp;$D$90&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=89,DegreePlanID=16,TermID=4,RequirementID=10},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=89,DegreePlanID=16,TermID=4,RequirementID=10},</v>
       </c>
     </row>
     <row r="91" spans="1:7" ht="15.75" customHeight="1">
@@ -7319,14 +7325,14 @@
         <v>20</v>
       </c>
       <c r="E91" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F91" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G91" t="str">
         <f>E91&amp;$A$1&amp;"="&amp;$A$91&amp;","&amp;$B$1&amp;"="&amp;$B$91&amp;","&amp;$C$1&amp;"="&amp;$C$91&amp;","&amp;$D$1&amp;"="&amp;$D$91&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=90,DegreePlanID=16,TermID=4,RequirementID=20},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=90,DegreePlanID=16,TermID=4,RequirementID=20},</v>
       </c>
     </row>
     <row r="92" spans="1:7" ht="15.75" customHeight="1">
@@ -7343,14 +7349,14 @@
         <v>692</v>
       </c>
       <c r="E92" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F92" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G92" t="str">
         <f>E92&amp;$A$1&amp;"="&amp;$A$92&amp;","&amp;$B$1&amp;"="&amp;$B$92&amp;","&amp;$C$1&amp;"="&amp;$C$92&amp;","&amp;$D$1&amp;"="&amp;$D$92&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=91,DegreePlanID=16,TermID=5,RequirementID=692},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=91,DegreePlanID=16,TermID=5,RequirementID=692},</v>
       </c>
     </row>
     <row r="93" spans="1:7" ht="15.75" customHeight="1">
@@ -7367,14 +7373,14 @@
         <v>460</v>
       </c>
       <c r="E93" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F93" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G93" t="str">
         <f>E93&amp;$A$1&amp;"="&amp;$A$93&amp;","&amp;$B$1&amp;"="&amp;$B$93&amp;","&amp;$C$1&amp;"="&amp;$C$93&amp;","&amp;$D$1&amp;"="&amp;$D$93&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=92,DegreePlanID=17,TermID=1,RequirementID=460},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=92,DegreePlanID=17,TermID=1,RequirementID=460},</v>
       </c>
     </row>
     <row r="94" spans="1:7" ht="15.75" customHeight="1">
@@ -7391,14 +7397,14 @@
         <v>356</v>
       </c>
       <c r="E94" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F94" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G94" t="str">
         <f>E94&amp;$A$1&amp;"="&amp;$A$94&amp;","&amp;$B$1&amp;"="&amp;$B$94&amp;","&amp;$C$1&amp;"="&amp;$C$94&amp;","&amp;$D$1&amp;"="&amp;$D$94&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=93,DegreePlanID=17,TermID=1,RequirementID=356},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=93,DegreePlanID=17,TermID=1,RequirementID=356},</v>
       </c>
     </row>
     <row r="95" spans="1:7" ht="15.75" customHeight="1">
@@ -7415,14 +7421,14 @@
         <v>542</v>
       </c>
       <c r="E95" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F95" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G95" t="str">
         <f>E95&amp;$A$1&amp;"="&amp;$A$95&amp;","&amp;$B$1&amp;"="&amp;$B$95&amp;","&amp;$C$1&amp;"="&amp;$C$95&amp;","&amp;$D$1&amp;"="&amp;$D$95&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=94,DegreePlanID=17,TermID=1,RequirementID=542},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=94,DegreePlanID=17,TermID=1,RequirementID=542},</v>
       </c>
     </row>
     <row r="96" spans="1:7" ht="15.75" customHeight="1">
@@ -7439,14 +7445,14 @@
         <v>563</v>
       </c>
       <c r="E96" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F96" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G96" t="str">
         <f>E96&amp;$A$1&amp;"="&amp;$A$96&amp;","&amp;$B$1&amp;"="&amp;$B$96&amp;","&amp;$C$1&amp;"="&amp;$C$96&amp;","&amp;$D$1&amp;"="&amp;$D$96&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=95,DegreePlanID=17,TermID=1,RequirementID=563},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=95,DegreePlanID=17,TermID=1,RequirementID=563},</v>
       </c>
     </row>
     <row r="97" spans="1:7" ht="15.75" customHeight="1">
@@ -7463,14 +7469,14 @@
         <v>560</v>
       </c>
       <c r="E97" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F97" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G97" t="str">
         <f>E97&amp;$A$1&amp;"="&amp;$A$97&amp;","&amp;$B$1&amp;"="&amp;$B$97&amp;","&amp;$C$1&amp;"="&amp;$C$97&amp;","&amp;$D$1&amp;"="&amp;$D$97&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=96,DegreePlanID=17,TermID=2,RequirementID=560},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=96,DegreePlanID=17,TermID=2,RequirementID=560},</v>
       </c>
     </row>
     <row r="98" spans="1:7" ht="15.75" customHeight="1">
@@ -7487,14 +7493,14 @@
         <v>555</v>
       </c>
       <c r="E98" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F98" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G98" t="str">
         <f>E98&amp;$A$1&amp;"="&amp;$A$98&amp;","&amp;$B$1&amp;"="&amp;$B$98&amp;","&amp;$C$1&amp;"="&amp;$C$98&amp;","&amp;$D$1&amp;"="&amp;$D$98&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=97,DegreePlanID=17,TermID=2,RequirementID=555},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=97,DegreePlanID=17,TermID=2,RequirementID=555},</v>
       </c>
     </row>
     <row r="99" spans="1:7" ht="15.75" customHeight="1">
@@ -7511,14 +7517,14 @@
         <v>618</v>
       </c>
       <c r="E99" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F99" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G99" t="str">
         <f>E99&amp;$A$1&amp;"="&amp;$A$99&amp;","&amp;$B$1&amp;"="&amp;$B$99&amp;","&amp;$C$1&amp;"="&amp;$C$99&amp;","&amp;$D$1&amp;"="&amp;$D$99&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=98,DegreePlanID=17,TermID=2,RequirementID=618},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=98,DegreePlanID=17,TermID=2,RequirementID=618},</v>
       </c>
     </row>
     <row r="100" spans="1:7" ht="15.75" customHeight="1">
@@ -7535,14 +7541,14 @@
         <v>1</v>
       </c>
       <c r="E100" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F100" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G100" t="str">
         <f>E100&amp;$A$1&amp;"="&amp;$A$100&amp;","&amp;$B$1&amp;"="&amp;$B$100&amp;","&amp;$C$1&amp;"="&amp;$C$100&amp;","&amp;$D$1&amp;"="&amp;$D$100&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=99,DegreePlanID=17,TermID=4,RequirementID=1},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=99,DegreePlanID=17,TermID=4,RequirementID=1},</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="15.75" customHeight="1">
@@ -7559,14 +7565,14 @@
         <v>664</v>
       </c>
       <c r="E101" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F101" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G101" t="str">
         <f>E101&amp;$A$1&amp;"="&amp;$A$101&amp;","&amp;$B$1&amp;"="&amp;$B$101&amp;","&amp;$C$1&amp;"="&amp;$C$101&amp;","&amp;$D$1&amp;"="&amp;$D$101&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=100,DegreePlanID=17,TermID=4,RequirementID=664},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=100,DegreePlanID=17,TermID=4,RequirementID=664},</v>
       </c>
     </row>
     <row r="102" spans="1:7" ht="15.75" customHeight="1">
@@ -7583,14 +7589,14 @@
         <v>691</v>
       </c>
       <c r="E102" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F102" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G102" t="str">
         <f>E102&amp;$A$1&amp;"="&amp;$A$102&amp;","&amp;$B$1&amp;"="&amp;$B$102&amp;","&amp;$C$1&amp;"="&amp;$C$102&amp;","&amp;$D$1&amp;"="&amp;$D$102&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=101,DegreePlanID=17,TermID=4,RequirementID=691},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=101,DegreePlanID=17,TermID=4,RequirementID=691},</v>
       </c>
     </row>
     <row r="103" spans="1:7" ht="15.75" customHeight="1">
@@ -7607,14 +7613,14 @@
         <v>10</v>
       </c>
       <c r="E103" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F103" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G103" t="str">
         <f>E103&amp;$A$1&amp;"="&amp;$A$103&amp;","&amp;$B$1&amp;"="&amp;$B$103&amp;","&amp;$C$1&amp;"="&amp;$C$103&amp;","&amp;$D$1&amp;"="&amp;$D$103&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=102,DegreePlanID=17,TermID=5,RequirementID=10},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=102,DegreePlanID=17,TermID=5,RequirementID=10},</v>
       </c>
     </row>
     <row r="104" spans="1:7" ht="15.75" customHeight="1">
@@ -7631,14 +7637,14 @@
         <v>20</v>
       </c>
       <c r="E104" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F104" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G104" t="str">
         <f>E104&amp;$A$1&amp;"="&amp;$A$104&amp;","&amp;$B$1&amp;"="&amp;$B$104&amp;","&amp;$C$1&amp;"="&amp;$C$104&amp;","&amp;$D$1&amp;"="&amp;$D$104&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=103,DegreePlanID=17,TermID=5,RequirementID=20},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=103,DegreePlanID=17,TermID=5,RequirementID=20},</v>
       </c>
     </row>
     <row r="105" spans="1:7" ht="15.75" customHeight="1">
@@ -7655,14 +7661,14 @@
         <v>692</v>
       </c>
       <c r="E105" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F105" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G105" t="str">
         <f>E105&amp;$A$1&amp;"="&amp;$A$105&amp;","&amp;$B$1&amp;"="&amp;$B$105&amp;","&amp;$C$1&amp;"="&amp;$C$105&amp;","&amp;$D$1&amp;"="&amp;$D$105&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=104,DegreePlanID=17,TermID=5,RequirementID=692},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=104,DegreePlanID=17,TermID=5,RequirementID=692},</v>
       </c>
     </row>
     <row r="106" spans="1:7" ht="15.75" customHeight="1">
@@ -7679,14 +7685,14 @@
         <v>460</v>
       </c>
       <c r="E106" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F106" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G106" t="str">
         <f>E106&amp;$A$1&amp;"="&amp;$A$106&amp;","&amp;$B$1&amp;"="&amp;$B$106&amp;","&amp;$C$1&amp;"="&amp;$C$106&amp;","&amp;$D$1&amp;"="&amp;$D$106&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=105,DegreePlanID=14,TermID=1,RequirementID=460},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=105,DegreePlanID=14,TermID=1,RequirementID=460},</v>
       </c>
     </row>
     <row r="107" spans="1:7" ht="15.75" customHeight="1">
@@ -7703,14 +7709,14 @@
         <v>356</v>
       </c>
       <c r="E107" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F107" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G107" t="str">
         <f>E107&amp;$A$1&amp;"="&amp;$A$107&amp;","&amp;$B$1&amp;"="&amp;$B$107&amp;","&amp;$C$1&amp;"="&amp;$C$107&amp;","&amp;$D$1&amp;"="&amp;$D$107&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=106,DegreePlanID=14,TermID=1,RequirementID=356},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=106,DegreePlanID=14,TermID=1,RequirementID=356},</v>
       </c>
     </row>
     <row r="108" spans="1:7" ht="15.75" customHeight="1">
@@ -7727,14 +7733,14 @@
         <v>542</v>
       </c>
       <c r="E108" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F108" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G108" t="str">
         <f>E108&amp;$A$1&amp;"="&amp;$A$108&amp;","&amp;$B$1&amp;"="&amp;$B$108&amp;","&amp;$C$1&amp;"="&amp;$C$108&amp;","&amp;$D$1&amp;"="&amp;$D$108&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=107,DegreePlanID=15,TermID=1,RequirementID=542},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=107,DegreePlanID=15,TermID=1,RequirementID=542},</v>
       </c>
     </row>
     <row r="109" spans="1:7" ht="15.75" customHeight="1">
@@ -7751,14 +7757,14 @@
         <v>563</v>
       </c>
       <c r="E109" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F109" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G109" t="str">
         <f>E109&amp;$A$1&amp;"="&amp;$A$109&amp;","&amp;$B$1&amp;"="&amp;$B$109&amp;","&amp;$C$1&amp;"="&amp;$C$109&amp;","&amp;$D$1&amp;"="&amp;$D$109&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=108,DegreePlanID=15,TermID=1,RequirementID=563},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=108,DegreePlanID=15,TermID=1,RequirementID=563},</v>
       </c>
     </row>
     <row r="110" spans="1:7" ht="15.75" customHeight="1">
@@ -7775,14 +7781,14 @@
         <v>560</v>
       </c>
       <c r="E110" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F110" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G110" t="str">
         <f>E110&amp;$A$1&amp;"="&amp;$A$110&amp;","&amp;$B$1&amp;"="&amp;$B$110&amp;","&amp;$C$1&amp;"="&amp;$C$110&amp;","&amp;$D$1&amp;"="&amp;$D$110&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=109,DegreePlanID=15,TermID=2,RequirementID=560},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=109,DegreePlanID=15,TermID=2,RequirementID=560},</v>
       </c>
     </row>
     <row r="111" spans="1:7" ht="15.75" customHeight="1">
@@ -7799,14 +7805,14 @@
         <v>555</v>
       </c>
       <c r="E111" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F111" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G111" t="str">
         <f>E111&amp;$A$1&amp;"="&amp;$A$111&amp;","&amp;$B$1&amp;"="&amp;$B$111&amp;","&amp;$C$1&amp;"="&amp;$C$111&amp;","&amp;$D$1&amp;"="&amp;$D$111&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=110,DegreePlanID=15,TermID=2,RequirementID=555},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=110,DegreePlanID=15,TermID=2,RequirementID=555},</v>
       </c>
     </row>
     <row r="112" spans="1:7" ht="15.75" customHeight="1">
@@ -7823,14 +7829,14 @@
         <v>618</v>
       </c>
       <c r="E112" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F112" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G112" t="str">
         <f>E112&amp;$A$1&amp;"="&amp;$A$112&amp;","&amp;$B$1&amp;"="&amp;$B$112&amp;","&amp;$C$1&amp;"="&amp;$C$112&amp;","&amp;$D$1&amp;"="&amp;$D$112&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=111,DegreePlanID=15,TermID=2,RequirementID=618},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=111,DegreePlanID=15,TermID=2,RequirementID=618},</v>
       </c>
     </row>
     <row r="113" spans="1:7" ht="15.75" customHeight="1">
@@ -7847,14 +7853,14 @@
         <v>1</v>
       </c>
       <c r="E113" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F113" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G113" t="str">
         <f>E113&amp;$A$1&amp;"="&amp;$A$113&amp;","&amp;$B$1&amp;"="&amp;$B$113&amp;","&amp;$C$1&amp;"="&amp;$C$113&amp;","&amp;$D$1&amp;"="&amp;$D$113&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=112,DegreePlanID=15,TermID=3,RequirementID=1},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=112,DegreePlanID=15,TermID=3,RequirementID=1},</v>
       </c>
     </row>
     <row r="114" spans="1:7" ht="15.75" customHeight="1">
@@ -7871,14 +7877,14 @@
         <v>664</v>
       </c>
       <c r="E114" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F114" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G114" t="str">
         <f>E114&amp;$A$1&amp;"="&amp;$A$114&amp;","&amp;$B$1&amp;"="&amp;$B$114&amp;","&amp;$C$1&amp;"="&amp;$C$114&amp;","&amp;$D$1&amp;"="&amp;$D$114&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=113,DegreePlanID=15,TermID=3,RequirementID=664},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=113,DegreePlanID=15,TermID=3,RequirementID=664},</v>
       </c>
     </row>
     <row r="115" spans="1:7" ht="15.75" customHeight="1">
@@ -7895,14 +7901,14 @@
         <v>691</v>
       </c>
       <c r="E115" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F115" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G115" t="str">
         <f>E115&amp;$A$1&amp;"="&amp;$A$115&amp;","&amp;$B$1&amp;"="&amp;$B$115&amp;","&amp;$C$1&amp;"="&amp;$C$115&amp;","&amp;$D$1&amp;"="&amp;$D$115&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=114,DegreePlanID=15,TermID=4,RequirementID=691},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=114,DegreePlanID=15,TermID=4,RequirementID=691},</v>
       </c>
     </row>
     <row r="116" spans="1:7" ht="15.75" customHeight="1">
@@ -7919,14 +7925,14 @@
         <v>10</v>
       </c>
       <c r="E116" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F116" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G116" t="str">
         <f>E116&amp;$A$1&amp;"="&amp;$A$116&amp;","&amp;$B$1&amp;"="&amp;$B$116&amp;","&amp;$C$1&amp;"="&amp;$C$116&amp;","&amp;$D$1&amp;"="&amp;$D$116&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=115,DegreePlanID=15,TermID=4,RequirementID=10},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=115,DegreePlanID=15,TermID=4,RequirementID=10},</v>
       </c>
     </row>
     <row r="117" spans="1:7" ht="15.75" customHeight="1">
@@ -7943,14 +7949,14 @@
         <v>20</v>
       </c>
       <c r="E117" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F117" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G117" t="str">
         <f>E117&amp;$A$1&amp;"="&amp;$A$117&amp;","&amp;$B$1&amp;"="&amp;$B$117&amp;","&amp;$C$1&amp;"="&amp;$C$117&amp;","&amp;$D$1&amp;"="&amp;$D$117&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=116,DegreePlanID=15,TermID=4,RequirementID=20},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=116,DegreePlanID=15,TermID=4,RequirementID=20},</v>
       </c>
     </row>
     <row r="118" spans="1:7" ht="15.75" customHeight="1">
@@ -7967,14 +7973,14 @@
         <v>692</v>
       </c>
       <c r="E118" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F118" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G118" t="str">
         <f>E118&amp;$A$1&amp;"="&amp;$A$118&amp;","&amp;$B$1&amp;"="&amp;$B$118&amp;","&amp;$C$1&amp;"="&amp;$C$118&amp;","&amp;$D$1&amp;"="&amp;$D$118&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=117,DegreePlanID=15,TermID=5,RequirementID=692},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=117,DegreePlanID=15,TermID=5,RequirementID=692},</v>
       </c>
     </row>
     <row r="119" spans="1:7" ht="15.75" customHeight="1">
@@ -7991,14 +7997,14 @@
         <v>460</v>
       </c>
       <c r="E119" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F119" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G119" t="str">
         <f>E119&amp;$A$1&amp;"="&amp;$A$119&amp;","&amp;$B$1&amp;"="&amp;$B$119&amp;","&amp;$C$1&amp;"="&amp;$C$119&amp;","&amp;$D$1&amp;"="&amp;$D$119&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=118,DegreePlanID=15,TermID=1,RequirementID=460},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=118,DegreePlanID=15,TermID=1,RequirementID=460},</v>
       </c>
     </row>
     <row r="120" spans="1:7" ht="15.75" customHeight="1">
@@ -8015,14 +8021,14 @@
         <v>356</v>
       </c>
       <c r="E120" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F120" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G120" t="str">
         <f>E120&amp;$A$1&amp;"="&amp;$A$120&amp;","&amp;$B$1&amp;"="&amp;$B$120&amp;","&amp;$C$1&amp;"="&amp;$C$120&amp;","&amp;$D$1&amp;"="&amp;$D$120&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=119,DegreePlanID=15,TermID=1,RequirementID=356},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=119,DegreePlanID=15,TermID=1,RequirementID=356},</v>
       </c>
     </row>
     <row r="121" spans="1:7" ht="15.75" customHeight="1">
@@ -8039,14 +8045,14 @@
         <v>542</v>
       </c>
       <c r="E121" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F121" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G121" t="str">
         <f>E121&amp;$A$1&amp;"="&amp;$A$121&amp;","&amp;$B$1&amp;"="&amp;$B$121&amp;","&amp;$C$1&amp;"="&amp;$C$121&amp;","&amp;$D$1&amp;"="&amp;$D$121&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=120,DegreePlanID=15,TermID=1,RequirementID=542},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=120,DegreePlanID=15,TermID=1,RequirementID=542},</v>
       </c>
     </row>
     <row r="122" spans="1:7" ht="15.75" customHeight="1">
@@ -8063,14 +8069,14 @@
         <v>563</v>
       </c>
       <c r="E122" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F122" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G122" t="str">
         <f>E122&amp;$A$1&amp;"="&amp;$A$122&amp;","&amp;$B$1&amp;"="&amp;$B$122&amp;","&amp;$C$1&amp;"="&amp;$C$122&amp;","&amp;$D$1&amp;"="&amp;$D$122&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=121,DegreePlanID=15,TermID=1,RequirementID=563},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=121,DegreePlanID=15,TermID=1,RequirementID=563},</v>
       </c>
     </row>
     <row r="123" spans="1:7" ht="15.75" customHeight="1">
@@ -8087,14 +8093,14 @@
         <v>560</v>
       </c>
       <c r="E123" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F123" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G123" t="str">
         <f>E123&amp;$A$1&amp;"="&amp;$A$123&amp;","&amp;$B$1&amp;"="&amp;$B$123&amp;","&amp;$C$1&amp;"="&amp;$C$123&amp;","&amp;$D$1&amp;"="&amp;$D$123&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=122,DegreePlanID=15,TermID=3,RequirementID=560},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=122,DegreePlanID=15,TermID=3,RequirementID=560},</v>
       </c>
     </row>
     <row r="124" spans="1:7" ht="15.75" customHeight="1">
@@ -8111,14 +8117,14 @@
         <v>555</v>
       </c>
       <c r="E124" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F124" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G124" t="str">
         <f>E124&amp;$A$1&amp;"="&amp;$A$124&amp;","&amp;$B$1&amp;"="&amp;$B$124&amp;","&amp;$C$1&amp;"="&amp;$C$124&amp;","&amp;$D$1&amp;"="&amp;$D$124&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=123,DegreePlanID=15,TermID=3,RequirementID=555},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=123,DegreePlanID=15,TermID=3,RequirementID=555},</v>
       </c>
     </row>
     <row r="125" spans="1:7" ht="15.75" customHeight="1">
@@ -8135,14 +8141,14 @@
         <v>618</v>
       </c>
       <c r="E125" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F125" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G125" t="str">
         <f>E125&amp;$A$1&amp;"="&amp;$A$125&amp;","&amp;$B$1&amp;"="&amp;$B$125&amp;","&amp;$C$1&amp;"="&amp;$C$125&amp;","&amp;$D$1&amp;"="&amp;$D$125&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=124,DegreePlanID=15,TermID=3,RequirementID=618},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=124,DegreePlanID=15,TermID=3,RequirementID=618},</v>
       </c>
     </row>
     <row r="126" spans="1:7" ht="15.75" customHeight="1">
@@ -8159,14 +8165,14 @@
         <v>1</v>
       </c>
       <c r="E126" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F126" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G126" t="str">
         <f>E126&amp;$A$1&amp;"="&amp;$A$126&amp;","&amp;$B$1&amp;"="&amp;$B$126&amp;","&amp;$C$1&amp;"="&amp;$C$126&amp;","&amp;$D$1&amp;"="&amp;$D$126&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=125,DegreePlanID=15,TermID=4,RequirementID=1},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=125,DegreePlanID=15,TermID=4,RequirementID=1},</v>
       </c>
     </row>
     <row r="127" spans="1:7" ht="15.75" customHeight="1">
@@ -8183,14 +8189,14 @@
         <v>664</v>
       </c>
       <c r="E127" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F127" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G127" t="str">
         <f>E127&amp;$A$1&amp;"="&amp;$A$127&amp;","&amp;$B$1&amp;"="&amp;$B$127&amp;","&amp;$C$1&amp;"="&amp;$C$127&amp;","&amp;$D$1&amp;"="&amp;$D$127&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=126,DegreePlanID=15,TermID=4,RequirementID=664},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=126,DegreePlanID=15,TermID=4,RequirementID=664},</v>
       </c>
     </row>
     <row r="128" spans="1:7" ht="15.75" customHeight="1">
@@ -8207,14 +8213,14 @@
         <v>691</v>
       </c>
       <c r="E128" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F128" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G128" t="str">
         <f>E128&amp;$A$1&amp;"="&amp;$A$128&amp;","&amp;$B$1&amp;"="&amp;$B$128&amp;","&amp;$C$1&amp;"="&amp;$C$128&amp;","&amp;$D$1&amp;"="&amp;$D$128&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=127,DegreePlanID=15,TermID=4,RequirementID=691},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=127,DegreePlanID=15,TermID=4,RequirementID=691},</v>
       </c>
     </row>
     <row r="129" spans="1:7" ht="15.75" customHeight="1">
@@ -8231,14 +8237,14 @@
         <v>10</v>
       </c>
       <c r="E129" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F129" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G129" t="str">
         <f>E129&amp;$A$1&amp;"="&amp;$A$129&amp;","&amp;$B$1&amp;"="&amp;$B$129&amp;","&amp;$C$1&amp;"="&amp;$C$129&amp;","&amp;$D$1&amp;"="&amp;$D$129&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=128,DegreePlanID=15,TermID=5,RequirementID=10},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=128,DegreePlanID=15,TermID=5,RequirementID=10},</v>
       </c>
     </row>
     <row r="130" spans="1:7" ht="15.75" customHeight="1">
@@ -8255,14 +8261,14 @@
         <v>20</v>
       </c>
       <c r="E130" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F130" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G130" t="str">
         <f>E130&amp;$A$1&amp;"="&amp;$A$130&amp;","&amp;$B$1&amp;"="&amp;$B$130&amp;","&amp;$C$1&amp;"="&amp;$C$130&amp;","&amp;$D$1&amp;"="&amp;$D$130&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=129,DegreePlanID=15,TermID=5,RequirementID=20},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=129,DegreePlanID=15,TermID=5,RequirementID=20},</v>
       </c>
     </row>
     <row r="131" spans="1:7" ht="15.75" customHeight="1">
@@ -8279,14 +8285,14 @@
         <v>692</v>
       </c>
       <c r="E131" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F131" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G131" t="str">
         <f>E131&amp;$A$1&amp;"="&amp;$A$131&amp;","&amp;$B$1&amp;"="&amp;$B$131&amp;","&amp;$C$1&amp;"="&amp;$C$131&amp;","&amp;$D$1&amp;"="&amp;$D$131&amp;$F$2</f>
-        <v>new DegreePlanTermRequirement {DegreePlanTermRequirementId=130,DegreePlanID=15,TermID=5,RequirementID=692},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=130,DegreePlanID=15,TermID=5,RequirementID=692},</v>
       </c>
     </row>
     <row r="132" spans="1:7" ht="15.75" customHeight="1"/>
@@ -9171,8 +9177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -9229,10 +9235,10 @@
         <v>52</v>
       </c>
       <c r="F2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H2" t="str">
         <f>F2&amp;$A$1&amp;"="&amp;A2&amp;","&amp;$B$1&amp;"="&amp;B2&amp;","&amp;$C$1&amp;"="&amp;C2&amp;","&amp;$D$1&amp;"="&amp;D2&amp;""&amp;$E$1&amp;"="""&amp;E2&amp;G2</f>
@@ -9256,10 +9262,10 @@
         <v>56</v>
       </c>
       <c r="F3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H3" t="str">
         <f t="shared" ref="H3:H11" si="0">F3&amp;$A$1&amp;"="&amp;A3&amp;","&amp;$B$1&amp;"="&amp;B3&amp;","&amp;$C$1&amp;"="&amp;C3&amp;","&amp;$D$1&amp;"="&amp;D3&amp;""&amp;$E$1&amp;"="""&amp;E3&amp;G3</f>
@@ -9283,10 +9289,10 @@
         <v>56</v>
       </c>
       <c r="F4" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" si="0"/>
@@ -9310,10 +9316,10 @@
         <v>52</v>
       </c>
       <c r="F5" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H5" t="str">
         <f t="shared" si="0"/>
@@ -9337,10 +9343,10 @@
         <v>56</v>
       </c>
       <c r="F6" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" si="0"/>
@@ -9364,10 +9370,10 @@
         <v>52</v>
       </c>
       <c r="F7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="0"/>
@@ -9391,10 +9397,10 @@
         <v>52</v>
       </c>
       <c r="F8" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
@@ -9418,10 +9424,10 @@
         <v>56</v>
       </c>
       <c r="F9" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
@@ -9445,10 +9451,10 @@
         <v>52</v>
       </c>
       <c r="F10" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="0"/>
@@ -9472,10 +9478,10 @@
         <v>56</v>
       </c>
       <c r="F11" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="0"/>
@@ -10473,7 +10479,7 @@
   <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -10490,16 +10496,16 @@
         <v>39</v>
       </c>
       <c r="B1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" t="s">
         <v>99</v>
-      </c>
-      <c r="C1" t="s">
-        <v>100</v>
       </c>
       <c r="D1" t="s">
         <v>44</v>
       </c>
       <c r="E1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F1" t="s">
         <v>91</v>
@@ -10528,14 +10534,14 @@
         <v>919564348</v>
       </c>
       <c r="F2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H2" t="str">
         <f>$F$2&amp;$A$1&amp;"="&amp;$A$2&amp;","&amp;$B$1&amp;"="&amp;$B$2&amp;","&amp;$C$1&amp;"="&amp;$C$2&amp;","&amp;$D$1&amp;"="&amp;$D$2&amp;","&amp;$E$1&amp;"="&amp;$E$2&amp;$G$2</f>
-        <v>new Student{StudentId=531494,FirstName=Shivani,LastName=Busireddy,Snumber=S531494,NineOneNineNumber=919564348},</v>
+        <v>new Models.Student{StudentId=531494,FirstName=Shivani,LastName=Busireddy,Snumber=S531494,NineOneNineNumber=919564348},</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -10554,9 +10560,15 @@
       <c r="E3" s="2">
         <v>919561527</v>
       </c>
+      <c r="F3" t="s">
+        <v>106</v>
+      </c>
+      <c r="G3" t="s">
+        <v>94</v>
+      </c>
       <c r="H3" t="str">
         <f>$F$2&amp;$A$1&amp;"="&amp;$A$3&amp;","&amp;$B$1&amp;"="&amp;$B$3&amp;","&amp;$C$1&amp;"="&amp;$C$3&amp;","&amp;$D$1&amp;"="&amp;$D$3&amp;","&amp;$E$1&amp;"="&amp;$E$3&amp;$G$2</f>
-        <v>new Student{StudentId=531503,FirstName=Santosh ,LastName=Muchkur,Snumber=S531503,NineOneNineNumber=919561527},</v>
+        <v>new Models.Student{StudentId=531503,FirstName=Santosh ,LastName=Muchkur,Snumber=S531503,NineOneNineNumber=919561527},</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -10575,9 +10587,15 @@
       <c r="E4" s="2">
         <v>919561950</v>
       </c>
+      <c r="F4" t="s">
+        <v>106</v>
+      </c>
+      <c r="G4" t="s">
+        <v>94</v>
+      </c>
       <c r="H4" t="str">
         <f>$F$2&amp;$A$1&amp;"="&amp;$A$4&amp;","&amp;$B$1&amp;"="&amp;$B$4&amp;","&amp;$C$1&amp;"="&amp;$C$4&amp;","&amp;$D$1&amp;"="&amp;$D$4&amp;","&amp;$E$1&amp;"="&amp;$E$4&amp;$G$2</f>
-        <v>new Student{StudentId=531384,FirstName=Srimai Reddy ,LastName=Yanala,Snumber=s531384,NineOneNineNumber=919561950},</v>
+        <v>new Models.Student{StudentId=531384,FirstName=Srimai Reddy ,LastName=Yanala,Snumber=s531384,NineOneNineNumber=919561950},</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -10596,9 +10614,15 @@
       <c r="E5" s="2">
         <v>919571235</v>
       </c>
+      <c r="F5" t="s">
+        <v>106</v>
+      </c>
+      <c r="G5" t="s">
+        <v>94</v>
+      </c>
       <c r="H5" t="str">
         <f>$F$2&amp;$A$1&amp;"="&amp;$A$5&amp;","&amp;$B$1&amp;"="&amp;$B$5&amp;","&amp;$C$1&amp;"="&amp;$C$5&amp;","&amp;$D$1&amp;"="&amp;$D$5&amp;","&amp;$E$1&amp;"="&amp;$E$5&amp;$G$2</f>
-        <v>new Student{StudentId=533707,FirstName=Lakshmi Seshu,LastName=Kalvakuri,Snumber=s533707,NineOneNineNumber=919571235},</v>
+        <v>new Models.Student{StudentId=533707,FirstName=Lakshmi Seshu,LastName=Kalvakuri,Snumber=s533707,NineOneNineNumber=919571235},</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -10617,9 +10641,15 @@
       <c r="E6" s="2">
         <v>919564693</v>
       </c>
+      <c r="F6" t="s">
+        <v>106</v>
+      </c>
+      <c r="G6" t="s">
+        <v>94</v>
+      </c>
       <c r="H6" t="str">
         <f>$F$2&amp;$A$1&amp;"="&amp;$A$6&amp;","&amp;$B$1&amp;"="&amp;$B$6&amp;","&amp;$C$1&amp;"="&amp;$C$6&amp;","&amp;$D$1&amp;"="&amp;$D$6&amp;","&amp;$E$1&amp;"="&amp;$E$6&amp;$G$2</f>
-        <v>new Student{StudentId=531507,FirstName=Vijay,LastName=Thupakala,Snumber=S531507,NineOneNineNumber=919564693},</v>
+        <v>new Models.Student{StudentId=531507,FirstName=Vijay,LastName=Thupakala,Snumber=S531507,NineOneNineNumber=919564693},</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -11610,10 +11640,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:E995"/>
+  <dimension ref="A1:H995"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -11621,10 +11651,11 @@
     <col min="1" max="1" width="26.140625" customWidth="1"/>
     <col min="2" max="4" width="8.7109375" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" customWidth="1"/>
-    <col min="6" max="27" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" customWidth="1"/>
+    <col min="7" max="27" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>66</v>
       </c>
@@ -11632,16 +11663,25 @@
         <v>67</v>
       </c>
       <c r="C1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1" t="s">
         <v>97</v>
       </c>
-      <c r="E1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -11657,8 +11697,18 @@
       <c r="E2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G2" t="s">
+        <v>94</v>
+      </c>
+      <c r="H2" t="str">
+        <f>F2&amp;$A$1&amp;"="&amp;$A2&amp;","&amp;$B$1&amp;"="&amp;B2&amp;","&amp;$C$1&amp;"="&amp;C2&amp;","&amp;$D$1&amp;"="&amp;D2&amp;","&amp;$E$1&amp;"="&amp;E2&amp;$G$2</f>
+        <v>new Models.StudentTerm{StudentTermId=1,StudentID=531494,TermID=1,TermAbbrev=S18,TermLabel=Spring 2018},</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -11674,8 +11724,18 @@
       <c r="E3" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" t="s">
+        <v>105</v>
+      </c>
+      <c r="G3" t="s">
+        <v>94</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H26" si="0">F3&amp;$A$1&amp;"="&amp;$A3&amp;","&amp;$B$1&amp;"="&amp;B3&amp;","&amp;$C$1&amp;"="&amp;C3&amp;","&amp;$D$1&amp;"="&amp;D3&amp;","&amp;$E$1&amp;"="&amp;E3&amp;$G$2</f>
+        <v>new Models.StudentTerm{StudentTermId=2,StudentID=531494,TermID=2,TermAbbrev=Su18,TermLabel=Summer 2018},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -11691,8 +11751,18 @@
       <c r="E4" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" t="s">
+        <v>105</v>
+      </c>
+      <c r="G4" t="s">
+        <v>94</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.StudentTerm{StudentTermId=3,StudentID=531494,TermID=3,TermAbbrev=F18,TermLabel=Fall 2018},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -11708,8 +11778,18 @@
       <c r="E5" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5" t="s">
+        <v>105</v>
+      </c>
+      <c r="G5" t="s">
+        <v>94</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.StudentTerm{StudentTermId=4,StudentID=531494,TermID=4,TermAbbrev=S19,TermLabel=Spring 2019},</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -11725,8 +11805,18 @@
       <c r="E6" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6" t="s">
+        <v>105</v>
+      </c>
+      <c r="G6" t="s">
+        <v>94</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.StudentTerm{StudentTermId=5,StudentID=531494,TermID=5,TermAbbrev=Su19,TermLabel=Summer2019},</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -11742,8 +11832,18 @@
       <c r="E7" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G7" t="s">
+        <v>94</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.StudentTerm{StudentTermId=6,StudentID=531503,TermID=1,TermAbbrev=F17,TermLabel=Fall 2017},</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -11759,8 +11859,18 @@
       <c r="E8" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8" t="s">
+        <v>105</v>
+      </c>
+      <c r="G8" t="s">
+        <v>94</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.StudentTerm{StudentTermId=7,StudentID=531503,TermID=2,TermAbbrev=S18,TermLabel=Spring 2018},</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -11776,8 +11886,18 @@
       <c r="E9" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9" t="s">
+        <v>105</v>
+      </c>
+      <c r="G9" t="s">
+        <v>94</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.StudentTerm{StudentTermId=8,StudentID=531503,TermID=3,TermAbbrev=Su18,TermLabel=Summer 2018},</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -11793,8 +11913,18 @@
       <c r="E10" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="F10" t="s">
+        <v>105</v>
+      </c>
+      <c r="G10" t="s">
+        <v>94</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.StudentTerm{StudentTermId=9,StudentID=531503,TermID=4,TermAbbrev=F18,TermLabel=Fall 2018},</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -11810,8 +11940,18 @@
       <c r="E11" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11" t="s">
+        <v>105</v>
+      </c>
+      <c r="G11" t="s">
+        <v>94</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.StudentTerm{StudentTermId=10,StudentID=531503,TermID=5,TermAbbrev=S19,TermLabel=Spring 2019},</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -11827,8 +11967,18 @@
       <c r="E12" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="F12" t="s">
+        <v>105</v>
+      </c>
+      <c r="G12" t="s">
+        <v>94</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.StudentTerm{StudentTermId=11,StudentID=531384,TermID=1,TermAbbrev=S18,TermLabel=Fall 2019},</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -11844,8 +11994,18 @@
       <c r="E13" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="F13" t="s">
+        <v>105</v>
+      </c>
+      <c r="G13" t="s">
+        <v>94</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.StudentTerm{StudentTermId=12,StudentID=531384,TermID=2,TermAbbrev=Su18,TermLabel=Spring 2020},</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -11861,8 +12021,18 @@
       <c r="E14" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="F14" t="s">
+        <v>105</v>
+      </c>
+      <c r="G14" t="s">
+        <v>94</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.StudentTerm{StudentTermId=13,StudentID=531384,TermID=3,TermAbbrev=F18,TermLabel=Summer 2020},</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -11878,8 +12048,18 @@
       <c r="E15" s="2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F15" t="s">
+        <v>105</v>
+      </c>
+      <c r="G15" t="s">
+        <v>94</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.StudentTerm{StudentTermId=14,StudentID=531384,TermID=4,TermAbbrev=S19,TermLabel=Fall 2020},</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" customHeight="1">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -11895,8 +12075,18 @@
       <c r="E16" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F16" t="s">
+        <v>105</v>
+      </c>
+      <c r="G16" t="s">
+        <v>94</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.StudentTerm{StudentTermId=15,StudentID=531384,TermID=5,TermAbbrev=Su19,TermLabel=Spring 2021},</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" customHeight="1">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -11912,8 +12102,18 @@
       <c r="E17" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F17" t="s">
+        <v>105</v>
+      </c>
+      <c r="G17" t="s">
+        <v>94</v>
+      </c>
+      <c r="H17" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.StudentTerm{StudentTermId=16,StudentID=533707,TermID=1,TermAbbrev=F18,TermLabel=Fall 2018},</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" customHeight="1">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -11929,8 +12129,18 @@
       <c r="E18" s="2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F18" t="s">
+        <v>105</v>
+      </c>
+      <c r="G18" t="s">
+        <v>94</v>
+      </c>
+      <c r="H18" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.StudentTerm{StudentTermId=17,StudentID=533707,TermID=2,TermAbbrev=S19,TermLabel=spring 2019},</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" customHeight="1">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -11946,8 +12156,18 @@
       <c r="E19" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F19" t="s">
+        <v>105</v>
+      </c>
+      <c r="G19" t="s">
+        <v>94</v>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.StudentTerm{StudentTermId=18,StudentID=533707,TermID=3,TermAbbrev=Su19,TermLabel=summer 2019},</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" customHeight="1">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -11963,8 +12183,18 @@
       <c r="E20" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F20" t="s">
+        <v>105</v>
+      </c>
+      <c r="G20" t="s">
+        <v>94</v>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.StudentTerm{StudentTermId=19,StudentID=533707,TermID=4,TermAbbrev=F19,TermLabel=Fall 2019},</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" customHeight="1">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -11980,8 +12210,18 @@
       <c r="E21" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F21" t="s">
+        <v>105</v>
+      </c>
+      <c r="G21" t="s">
+        <v>94</v>
+      </c>
+      <c r="H21" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.StudentTerm{StudentTermId=20,StudentID=533707,TermID=5,TermAbbrev=S20,TermLabel=Spring 2020},</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15.75" customHeight="1">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -11997,8 +12237,18 @@
       <c r="E22" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F22" t="s">
+        <v>105</v>
+      </c>
+      <c r="G22" t="s">
+        <v>94</v>
+      </c>
+      <c r="H22" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.StudentTerm{StudentTermId=21,StudentID=531507,TermID=1,TermAbbrev=S19,TermLabel=Spring 2019},</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" customHeight="1">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -12014,8 +12264,18 @@
       <c r="E23" s="2" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F23" t="s">
+        <v>105</v>
+      </c>
+      <c r="G23" t="s">
+        <v>94</v>
+      </c>
+      <c r="H23" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.StudentTerm{StudentTermId=22,StudentID=531507,TermID=2,TermAbbrev=Su19,TermLabel=Summer 2019},</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" customHeight="1">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -12031,8 +12291,18 @@
       <c r="E24" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F24" t="s">
+        <v>105</v>
+      </c>
+      <c r="G24" t="s">
+        <v>94</v>
+      </c>
+      <c r="H24" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.StudentTerm{StudentTermId=23,StudentID=531507,TermID=3,TermAbbrev=F19,TermLabel=Fall 2019},</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15.75" customHeight="1">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -12048,8 +12318,18 @@
       <c r="E25" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F25" t="s">
+        <v>105</v>
+      </c>
+      <c r="G25" t="s">
+        <v>94</v>
+      </c>
+      <c r="H25" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.StudentTerm{StudentTermId=24,StudentID=531507,TermID=4,TermAbbrev=S20,TermLabel=Spring 2020},</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15.75" customHeight="1">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -12065,13 +12345,23 @@
       <c r="E26" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1"/>
+      <c r="F26" t="s">
+        <v>105</v>
+      </c>
+      <c r="G26" t="s">
+        <v>94</v>
+      </c>
+      <c r="H26" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.StudentTerm{StudentTermId=25,StudentID=531507,TermID=5,TermAbbrev=Su20,TermLabel=Summer 2020},</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="28" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="29" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="30" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="31" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="32" spans="1:8" ht="15.75" customHeight="1"/>
     <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Fixed errors in Program.cs
</commit_message>
<xml_diff>
--- a/Docs/Project05.xlsx
+++ b/Docs/Project05.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S531384\Documents\Masters\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S531494\Documents\44663\Project\Masters\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9116FC9-3958-4890-8B82-E63141719FE0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Degree" sheetId="1" r:id="rId1"/>
@@ -21,7 +20,7 @@
     <sheet name="Student" sheetId="6" r:id="rId6"/>
     <sheet name="StudentTerm" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="109">
   <si>
     <t>RequirementID</t>
   </si>
@@ -146,9 +145,6 @@
     <t>GDP2</t>
   </si>
   <si>
-    <t>DegreePlanId</t>
-  </si>
-  <si>
     <t>DegreeID</t>
   </si>
   <si>
@@ -159,9 +155,6 @@
   </si>
   <si>
     <t>DegreePlanName(u,20)</t>
-  </si>
-  <si>
-    <t>DegreePlanTermRequirementId</t>
   </si>
   <si>
     <t>DegreePlanID</t>
@@ -231,9 +224,6 @@
   </si>
   <si>
     <t>s531503</t>
-  </si>
-  <si>
-    <t>StudentTermId</t>
   </si>
   <si>
     <t>StudentID</t>
@@ -364,11 +354,17 @@
   <si>
     <t>new Models.Degree {</t>
   </si>
+  <si>
+    <t>DegreePlanTermRequirementID</t>
+  </si>
+  <si>
+    <t>StudentTermID</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -706,10 +702,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -724,7 +720,7 @@
   <sheetData>
     <row r="1" spans="1:26">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
@@ -733,13 +729,13 @@
         <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -773,10 +769,10 @@
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F2" t="str">
         <f>D2&amp;$A$1&amp;"="&amp;A2&amp;", "&amp;$B$1&amp;"="&amp;$B$2&amp;", "&amp;$C$1&amp;" ="&amp;C2&amp;E2</f>
@@ -794,10 +790,10 @@
         <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F3" t="str">
         <f>D3&amp;$A$1&amp;"="&amp;A3&amp;", "&amp;$B$1&amp;"="&amp;$B$3&amp;", "&amp;$C$1&amp;" ="&amp;C3&amp;E3</f>
@@ -815,10 +811,10 @@
         <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F4" t="str">
         <f>D4&amp;$A$1&amp;"="&amp;A4&amp;", "&amp;$B$1&amp;"="&amp;$B$4&amp;", "&amp;$C$1&amp;" ="&amp;C4&amp;E4</f>
@@ -836,10 +832,10 @@
         <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F5" t="str">
         <f>D5&amp;$A$1&amp;"="&amp;A5&amp;", "&amp;$B$1&amp;"="&amp;$B$5&amp;", "&amp;$C$1&amp;" ="&amp;C5&amp;E5</f>
@@ -1833,10 +1829,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -1862,13 +1858,13 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1882,14 +1878,14 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F2" t="str">
         <f>Student!H:H</f>
-        <v>new Models.Student{StudentId=531494,FirstName=Shivani,LastName=Busireddy,Snumber=S531494,NineOneNineNumber=919564348},</v>
+        <v>new Models.Student{StudentID=531494,FirstName=Shivani,LastName=Busireddy,Snumber=S531494,NineOneNineNumber=919564348},</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1903,10 +1899,10 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F3" t="str">
         <f>D3&amp;$A$1&amp;"="&amp;$A$3&amp;","&amp;$B$1&amp;"="&amp;$B$3&amp;","&amp;$C$1&amp;"="&amp;$C$3&amp;$E$2</f>
@@ -1924,10 +1920,10 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F4" t="str">
         <f>D4&amp;$A$1&amp;"="&amp;$A$4&amp;","&amp;$B$1&amp;"="&amp;$B$4&amp;","&amp;$C$1&amp;"="&amp;$C$4&amp;$E$2</f>
@@ -1945,10 +1941,10 @@
         <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F5" t="str">
         <f>D5&amp;$A$1&amp;"="&amp;$A$5&amp;","&amp;$B$1&amp;"="&amp;$B$5&amp;","&amp;$C$1&amp;"="&amp;$C$5&amp;$E$2</f>
@@ -1966,10 +1962,10 @@
         <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E6" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F6" t="str">
         <f>D6&amp;$A$1&amp;"="&amp;$A$6&amp;","&amp;$B$1&amp;"="&amp;$B$6&amp;","&amp;$C$1&amp;"="&amp;$C$6&amp;$E$2</f>
@@ -1987,10 +1983,10 @@
         <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E7" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F7" t="str">
         <f>D7&amp;$A$1&amp;"="&amp;$A$7&amp;","&amp;$B$1&amp;"="&amp;$B$7&amp;","&amp;$C$1&amp;"="&amp;$C$7&amp;$E$2</f>
@@ -2008,10 +2004,10 @@
         <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E8" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F8" t="str">
         <f>D8&amp;$A$1&amp;"="&amp;$A$8&amp;","&amp;$B$1&amp;"="&amp;$B$8&amp;","&amp;$C$1&amp;"="&amp;$C$8&amp;$E$2</f>
@@ -2029,10 +2025,10 @@
         <v>28</v>
       </c>
       <c r="D9" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E9" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F9" t="str">
         <f>D9&amp;$A$1&amp;"="&amp;$A$9&amp;","&amp;$B$1&amp;"="&amp;$B$9&amp;","&amp;$C$1&amp;"="&amp;$C$9&amp;$E$2</f>
@@ -2050,10 +2046,10 @@
         <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E10" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F10" t="str">
         <f>D10&amp;$A$1&amp;"="&amp;$A$10&amp;","&amp;$B$1&amp;"="&amp;$B$10&amp;","&amp;$C$1&amp;"="&amp;$C$10&amp;$E$2</f>
@@ -2071,10 +2067,10 @@
         <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E11" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F11" t="str">
         <f>D11&amp;$A$1&amp;"="&amp;$A$11&amp;","&amp;$B$1&amp;"="&amp;$B$11&amp;","&amp;$C$1&amp;"="&amp;$C$11&amp;$E$2</f>
@@ -2092,10 +2088,10 @@
         <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E12" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F12" t="str">
         <f>D12&amp;$A$1&amp;"="&amp;$A$12&amp;","&amp;$B$1&amp;"="&amp;$B$12&amp;","&amp;$C$1&amp;"="&amp;$C$12&amp;$E$2</f>
@@ -2113,10 +2109,10 @@
         <v>35</v>
       </c>
       <c r="D13" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E13" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F13" t="str">
         <f>D13&amp;$A$1&amp;"="&amp;$A$13&amp;","&amp;$B$1&amp;"="&amp;$B$13&amp;","&amp;$C$1&amp;"="&amp;$C$13&amp;$E$2</f>
@@ -2134,10 +2130,10 @@
         <v>36</v>
       </c>
       <c r="D14" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E14" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F14" t="str">
         <f>D14&amp;$A$1&amp;"="&amp;$A$14&amp;","&amp;$B$1&amp;"="&amp;$B$14&amp;","&amp;$C$1&amp;"="&amp;$C$14&amp;$E$2</f>
@@ -3131,10 +3127,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
@@ -3149,22 +3145,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -3178,10 +3174,10 @@
         <v>460</v>
       </c>
       <c r="D2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F2" t="str">
         <f>D2&amp;$A$1&amp;"="&amp;A2&amp;","&amp;$B$1&amp;"="&amp;B2&amp;","&amp;$C$1&amp;"="&amp;C2&amp;E3</f>
@@ -3199,10 +3195,10 @@
         <v>356</v>
       </c>
       <c r="D3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" ref="F3:F48" si="0">D3&amp;$A$1&amp;"="&amp;A3&amp;","&amp;$B$1&amp;"="&amp;B3&amp;","&amp;$C$1&amp;"="&amp;C3&amp;E4</f>
@@ -3220,10 +3216,10 @@
         <v>542</v>
       </c>
       <c r="D4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="0"/>
@@ -3241,10 +3237,10 @@
         <v>563</v>
       </c>
       <c r="D5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="0"/>
@@ -3262,10 +3258,10 @@
         <v>560</v>
       </c>
       <c r="D6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E6" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="0"/>
@@ -3283,10 +3279,10 @@
         <v>555</v>
       </c>
       <c r="D7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E7" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="0"/>
@@ -3304,10 +3300,10 @@
         <v>618</v>
       </c>
       <c r="D8" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E8" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="0"/>
@@ -3325,10 +3321,10 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E9" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="0"/>
@@ -3346,10 +3342,10 @@
         <v>664</v>
       </c>
       <c r="D10" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E10" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="0"/>
@@ -3367,10 +3363,10 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E11" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="0"/>
@@ -3388,10 +3384,10 @@
         <v>20</v>
       </c>
       <c r="D12" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E12" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="0"/>
@@ -3409,10 +3405,10 @@
         <v>691</v>
       </c>
       <c r="D13" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E13" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="0"/>
@@ -3430,10 +3426,10 @@
         <v>692</v>
       </c>
       <c r="D14" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E14" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="0"/>
@@ -3451,10 +3447,10 @@
         <v>460</v>
       </c>
       <c r="D15" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E15" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="0"/>
@@ -3472,10 +3468,10 @@
         <v>542</v>
       </c>
       <c r="D16" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E16" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="0"/>
@@ -3493,10 +3489,10 @@
         <v>563</v>
       </c>
       <c r="D17" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E17" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" si="0"/>
@@ -3514,10 +3510,10 @@
         <v>560</v>
       </c>
       <c r="D18" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" si="0"/>
@@ -3535,10 +3531,10 @@
         <v>555</v>
       </c>
       <c r="D19" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E19" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" si="0"/>
@@ -3556,10 +3552,10 @@
         <v>618</v>
       </c>
       <c r="D20" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E20" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F20" t="str">
         <f t="shared" si="0"/>
@@ -3577,10 +3573,10 @@
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E21" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" si="0"/>
@@ -3598,10 +3594,10 @@
         <v>664</v>
       </c>
       <c r="D22" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E22" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F22" t="str">
         <f t="shared" si="0"/>
@@ -3619,10 +3615,10 @@
         <v>10</v>
       </c>
       <c r="D23" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E23" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F23" t="str">
         <f t="shared" si="0"/>
@@ -3640,10 +3636,10 @@
         <v>20</v>
       </c>
       <c r="D24" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E24" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F24" t="str">
         <f t="shared" si="0"/>
@@ -3661,10 +3657,10 @@
         <v>691</v>
       </c>
       <c r="D25" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E25" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F25" t="str">
         <f t="shared" si="0"/>
@@ -3682,10 +3678,10 @@
         <v>692</v>
       </c>
       <c r="D26" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E26" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" si="0"/>
@@ -3703,10 +3699,10 @@
         <v>356</v>
       </c>
       <c r="D27" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E27" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F27" t="str">
         <f t="shared" si="0"/>
@@ -3724,10 +3720,10 @@
         <v>542</v>
       </c>
       <c r="D28" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E28" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F28" t="str">
         <f t="shared" si="0"/>
@@ -3745,10 +3741,10 @@
         <v>563</v>
       </c>
       <c r="D29" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E29" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F29" t="str">
         <f t="shared" si="0"/>
@@ -3766,10 +3762,10 @@
         <v>560</v>
       </c>
       <c r="D30" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E30" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F30" t="str">
         <f t="shared" si="0"/>
@@ -3787,10 +3783,10 @@
         <v>555</v>
       </c>
       <c r="D31" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E31" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F31" t="str">
         <f t="shared" si="0"/>
@@ -3808,10 +3804,10 @@
         <v>618</v>
       </c>
       <c r="D32" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E32" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F32" t="str">
         <f t="shared" si="0"/>
@@ -3829,10 +3825,10 @@
         <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E33" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F33" t="str">
         <f t="shared" si="0"/>
@@ -3850,10 +3846,10 @@
         <v>664</v>
       </c>
       <c r="D34" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E34" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F34" t="str">
         <f t="shared" si="0"/>
@@ -3871,10 +3867,10 @@
         <v>10</v>
       </c>
       <c r="D35" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E35" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F35" t="str">
         <f t="shared" si="0"/>
@@ -3892,10 +3888,10 @@
         <v>20</v>
       </c>
       <c r="D36" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E36" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F36" t="str">
         <f t="shared" si="0"/>
@@ -3913,10 +3909,10 @@
         <v>691</v>
       </c>
       <c r="D37" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E37" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F37" t="str">
         <f t="shared" si="0"/>
@@ -3934,10 +3930,10 @@
         <v>692</v>
       </c>
       <c r="D38" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E38" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F38" t="str">
         <f t="shared" si="0"/>
@@ -3955,10 +3951,10 @@
         <v>542</v>
       </c>
       <c r="D39" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E39" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F39" t="str">
         <f t="shared" si="0"/>
@@ -3976,10 +3972,10 @@
         <v>563</v>
       </c>
       <c r="D40" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E40" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F40" t="str">
         <f t="shared" si="0"/>
@@ -3997,10 +3993,10 @@
         <v>560</v>
       </c>
       <c r="D41" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E41" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F41" t="str">
         <f t="shared" si="0"/>
@@ -4018,10 +4014,10 @@
         <v>555</v>
       </c>
       <c r="D42" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E42" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F42" t="str">
         <f t="shared" si="0"/>
@@ -4039,10 +4035,10 @@
         <v>618</v>
       </c>
       <c r="D43" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E43" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F43" t="str">
         <f t="shared" si="0"/>
@@ -4060,10 +4056,10 @@
         <v>1</v>
       </c>
       <c r="D44" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E44" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F44" t="str">
         <f t="shared" si="0"/>
@@ -4081,10 +4077,10 @@
         <v>664</v>
       </c>
       <c r="D45" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E45" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F45" t="str">
         <f t="shared" si="0"/>
@@ -4102,10 +4098,10 @@
         <v>10</v>
       </c>
       <c r="D46" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E46" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F46" t="str">
         <f t="shared" si="0"/>
@@ -4123,10 +4119,10 @@
         <v>20</v>
       </c>
       <c r="D47" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E47" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F47" t="str">
         <f t="shared" si="0"/>
@@ -4144,10 +4140,10 @@
         <v>691</v>
       </c>
       <c r="D48" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E48" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F48" t="str">
         <f t="shared" si="0"/>
@@ -4165,10 +4161,10 @@
         <v>692</v>
       </c>
       <c r="D49" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E49" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F49" t="str">
         <f>D49&amp;$A$1&amp;"="&amp;A49&amp;","&amp;$B$1&amp;"="&amp;B49&amp;","&amp;$C$1&amp;"="&amp;C49&amp;E50</f>
@@ -5133,12 +5129,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -5154,25 +5148,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>107</v>
       </c>
       <c r="B1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -5189,14 +5183,14 @@
         <v>460</v>
       </c>
       <c r="E2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G2" t="str">
         <f>E2&amp;$A$1&amp;"="&amp;$A$2&amp;","&amp;$B$1&amp;"="&amp;$B$2&amp;","&amp;$C$1&amp;"="&amp;$C$2&amp;","&amp;$D$1&amp;"="&amp;$D$2&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=1,DegreePlanID=20,TermID=1,RequirementID=460},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=1,DegreePlanID=20,TermID=1,RequirementID=460},</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -5213,14 +5207,14 @@
         <v>356</v>
       </c>
       <c r="E3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G3" t="str">
         <f>E3&amp;$A$1&amp;"="&amp;$A$3&amp;","&amp;$B$1&amp;"="&amp;$B$3&amp;","&amp;$C$1&amp;"="&amp;$C$3&amp;","&amp;$D$1&amp;"="&amp;$D$3&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=2,DegreePlanID=20,TermID=1,RequirementID=356},</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -5237,14 +5231,14 @@
         <v>542</v>
       </c>
       <c r="E4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G4" t="str">
         <f>E4&amp;$A$1&amp;"="&amp;$A$4&amp;","&amp;$B$1&amp;"="&amp;$B$4&amp;","&amp;$C$1&amp;"="&amp;$C$4&amp;","&amp;$D$1&amp;"="&amp;$D$4&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=3,DegreePlanID=20,TermID=1,RequirementID=542},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=3,DegreePlanID=20,TermID=1,RequirementID=542},</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -5261,14 +5255,14 @@
         <v>563</v>
       </c>
       <c r="E5" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G5" t="str">
         <f>E5&amp;$A$1&amp;"="&amp;$A$5&amp;","&amp;$B$1&amp;"="&amp;$B$5&amp;","&amp;$C$1&amp;"="&amp;$C$5&amp;","&amp;$D$1&amp;"="&amp;$D$5&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=4,DegreePlanID=20,TermID=1,RequirementID=563},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=4,DegreePlanID=20,TermID=1,RequirementID=563},</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -5285,14 +5279,14 @@
         <v>560</v>
       </c>
       <c r="E6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F6" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G6" t="str">
         <f>E6&amp;$A$1&amp;"="&amp;$A$6&amp;","&amp;$B$1&amp;"="&amp;$B$6&amp;","&amp;$C$1&amp;"="&amp;$C$6&amp;","&amp;$D$1&amp;"="&amp;$D$6&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=5,DegreePlanID=20,TermID=2,RequirementID=560},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=5,DegreePlanID=20,TermID=2,RequirementID=560},</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -5309,14 +5303,14 @@
         <v>555</v>
       </c>
       <c r="E7" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F7" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G7" t="str">
         <f>E7&amp;$A$1&amp;"="&amp;$A$7&amp;","&amp;$B$1&amp;"="&amp;$B$7&amp;","&amp;$C$1&amp;"="&amp;$C$7&amp;","&amp;$D$1&amp;"="&amp;$D$7&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=6,DegreePlanID=20,TermID=2,RequirementID=555},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=6,DegreePlanID=20,TermID=2,RequirementID=555},</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -5333,14 +5327,14 @@
         <v>618</v>
       </c>
       <c r="E8" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F8" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G8" t="str">
         <f>E8&amp;$A$1&amp;"="&amp;$A$8&amp;","&amp;$B$1&amp;"="&amp;$B$8&amp;","&amp;$C$1&amp;"="&amp;$C$8&amp;","&amp;$D$1&amp;"="&amp;$D$8&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=7,DegreePlanID=20,TermID=2,RequirementID=618},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=7,DegreePlanID=20,TermID=2,RequirementID=618},</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -5357,14 +5351,14 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F9" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G9" t="str">
         <f>E9&amp;$A$1&amp;"="&amp;$A$9&amp;","&amp;$B$1&amp;"="&amp;$B$9&amp;","&amp;$C$1&amp;"="&amp;$C$9&amp;","&amp;$D$1&amp;"="&amp;$D$9&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=8,DegreePlanID=20,TermID=3,RequirementID=1},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=8,DegreePlanID=20,TermID=3,RequirementID=1},</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -5381,14 +5375,14 @@
         <v>664</v>
       </c>
       <c r="E10" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F10" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G10" t="str">
         <f>E10&amp;$A$1&amp;"="&amp;$A$10&amp;","&amp;$B$1&amp;"="&amp;$B$10&amp;","&amp;$C$1&amp;"="&amp;$C$10&amp;","&amp;$D$1&amp;"="&amp;$D$10&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=9,DegreePlanID=20,TermID=3,RequirementID=664},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=9,DegreePlanID=20,TermID=3,RequirementID=664},</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -5405,14 +5399,14 @@
         <v>691</v>
       </c>
       <c r="E11" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F11" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G11" t="str">
         <f>E11&amp;$A$1&amp;"="&amp;$A$11&amp;","&amp;$B$1&amp;"="&amp;$B$11&amp;","&amp;$C$1&amp;"="&amp;$C$11&amp;","&amp;$D$1&amp;"="&amp;$D$11&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=10,DegreePlanID=20,TermID=3,RequirementID=691},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=10,DegreePlanID=20,TermID=3,RequirementID=691},</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -5429,14 +5423,14 @@
         <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F12" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G12" t="str">
         <f>E12&amp;$A$1&amp;"="&amp;$A$12&amp;","&amp;$B$1&amp;"="&amp;$B$12&amp;","&amp;$C$1&amp;"="&amp;$C$12&amp;","&amp;$D$1&amp;"="&amp;$D$12&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=11,DegreePlanID=20,TermID=4,RequirementID=10},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=11,DegreePlanID=20,TermID=4,RequirementID=10},</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -5453,14 +5447,14 @@
         <v>20</v>
       </c>
       <c r="E13" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F13" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G13" t="str">
         <f>E13&amp;$A$1&amp;"="&amp;$A$13&amp;","&amp;$B$1&amp;"="&amp;$B$13&amp;","&amp;$C$1&amp;"="&amp;$C$13&amp;","&amp;$D$1&amp;"="&amp;$D$13&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=12,DegreePlanID=20,TermID=4,RequirementID=20},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=12,DegreePlanID=20,TermID=4,RequirementID=20},</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -5477,14 +5471,14 @@
         <v>692</v>
       </c>
       <c r="E14" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F14" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G14" t="str">
         <f>E14&amp;$A$1&amp;"="&amp;$A$14&amp;","&amp;$B$1&amp;"="&amp;$B$14&amp;","&amp;$C$1&amp;"="&amp;$C$14&amp;","&amp;$D$1&amp;"="&amp;$D$14&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=13,DegreePlanID=20,TermID=5,RequirementID=692},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=13,DegreePlanID=20,TermID=5,RequirementID=692},</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -5501,14 +5495,14 @@
         <v>460</v>
       </c>
       <c r="E15" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F15" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G15" t="str">
         <f>E15&amp;$A$1&amp;"="&amp;$A$15&amp;","&amp;$B$1&amp;"="&amp;$B$15&amp;","&amp;$C$1&amp;"="&amp;$C$15&amp;","&amp;$D$1&amp;"="&amp;$D$15&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=14,DegreePlanID=21,TermID=1,RequirementID=460},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=14,DegreePlanID=21,TermID=1,RequirementID=460},</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -5525,14 +5519,14 @@
         <v>356</v>
       </c>
       <c r="E16" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F16" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G16" t="str">
         <f>E16&amp;$A$1&amp;"="&amp;$A$16&amp;","&amp;$B$1&amp;"="&amp;$B$16&amp;","&amp;$C$1&amp;"="&amp;$C$16&amp;","&amp;$D$1&amp;"="&amp;$D$16&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=15,DegreePlanID=21,TermID=1,RequirementID=356},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=15,DegreePlanID=21,TermID=1,RequirementID=356},</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -5549,14 +5543,14 @@
         <v>542</v>
       </c>
       <c r="E17" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F17" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G17" t="str">
         <f>E17&amp;$A$1&amp;"="&amp;$A$17&amp;","&amp;$B$1&amp;"="&amp;$B$17&amp;","&amp;$C$1&amp;"="&amp;$C$17&amp;","&amp;$D$1&amp;"="&amp;$D$17&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=16,DegreePlanID=21,TermID=1,RequirementID=542},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=16,DegreePlanID=21,TermID=1,RequirementID=542},</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -5573,14 +5567,14 @@
         <v>563</v>
       </c>
       <c r="E18" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G18" t="str">
         <f>E18&amp;$A$1&amp;"="&amp;$A$18&amp;","&amp;$B$1&amp;"="&amp;$B$18&amp;","&amp;$C$1&amp;"="&amp;$C$18&amp;","&amp;$D$1&amp;"="&amp;$D$18&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=17,DegreePlanID=21,TermID=1,RequirementID=563},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=17,DegreePlanID=21,TermID=1,RequirementID=563},</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -5597,14 +5591,14 @@
         <v>560</v>
       </c>
       <c r="E19" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F19" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G19" t="str">
         <f>E19&amp;$A$1&amp;"="&amp;$A$19&amp;","&amp;$B$1&amp;"="&amp;$B$19&amp;","&amp;$C$1&amp;"="&amp;$C$19&amp;","&amp;$D$1&amp;"="&amp;$D$19&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=18,DegreePlanID=21,TermID=2,RequirementID=560},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=18,DegreePlanID=21,TermID=2,RequirementID=560},</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -5621,14 +5615,14 @@
         <v>555</v>
       </c>
       <c r="E20" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F20" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G20" t="str">
         <f>E20&amp;$A$1&amp;"="&amp;$A$20&amp;","&amp;$B$1&amp;"="&amp;$B$20&amp;","&amp;$C$1&amp;"="&amp;$C$20&amp;","&amp;$D$1&amp;"="&amp;$D$20&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=19,DegreePlanID=21,TermID=2,RequirementID=555},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=19,DegreePlanID=21,TermID=2,RequirementID=555},</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1">
@@ -5645,14 +5639,14 @@
         <v>618</v>
       </c>
       <c r="E21" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F21" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G21" t="str">
         <f>E21&amp;$A$1&amp;"="&amp;$A$21&amp;","&amp;$B$1&amp;"="&amp;$B$21&amp;","&amp;$C$1&amp;"="&amp;$C$21&amp;","&amp;$D$1&amp;"="&amp;$D$21&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=20,DegreePlanID=21,TermID=2,RequirementID=618},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=20,DegreePlanID=21,TermID=2,RequirementID=618},</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1">
@@ -5669,14 +5663,14 @@
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F22" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G22" t="str">
         <f>E22&amp;$A$1&amp;"="&amp;$A$22&amp;","&amp;$B$1&amp;"="&amp;$B$22&amp;","&amp;$C$1&amp;"="&amp;$C$22&amp;","&amp;$D$1&amp;"="&amp;$D$22&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=21,DegreePlanID=21,TermID=4,RequirementID=1},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=21,DegreePlanID=21,TermID=4,RequirementID=1},</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1">
@@ -5693,14 +5687,14 @@
         <v>664</v>
       </c>
       <c r="E23" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F23" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G23" t="str">
         <f>E23&amp;$A$1&amp;"="&amp;$A$23&amp;","&amp;$B$1&amp;"="&amp;$B$23&amp;","&amp;$C$1&amp;"="&amp;$C$23&amp;","&amp;$D$1&amp;"="&amp;$D$23&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=22,DegreePlanID=21,TermID=4,RequirementID=664},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=22,DegreePlanID=21,TermID=4,RequirementID=664},</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1">
@@ -5717,14 +5711,14 @@
         <v>691</v>
       </c>
       <c r="E24" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F24" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G24" t="str">
         <f>E24&amp;$A$1&amp;"="&amp;$A$24&amp;","&amp;$B$1&amp;"="&amp;$B$24&amp;","&amp;$C$1&amp;"="&amp;$C$24&amp;","&amp;$D$1&amp;"="&amp;$D$24&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=23,DegreePlanID=21,TermID=4,RequirementID=691},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=23,DegreePlanID=21,TermID=4,RequirementID=691},</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1">
@@ -5741,14 +5735,14 @@
         <v>10</v>
       </c>
       <c r="E25" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F25" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G25" t="str">
         <f>E25&amp;$A$1&amp;"="&amp;$A$25&amp;","&amp;$B$1&amp;"="&amp;$B$25&amp;","&amp;$C$1&amp;"="&amp;$C$25&amp;","&amp;$D$1&amp;"="&amp;$D$25&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=24,DegreePlanID=21,TermID=5,RequirementID=10},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=24,DegreePlanID=21,TermID=5,RequirementID=10},</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1">
@@ -5765,14 +5759,14 @@
         <v>20</v>
       </c>
       <c r="E26" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F26" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G26" t="str">
         <f>E26&amp;$A$1&amp;"="&amp;$A$26&amp;","&amp;$B$1&amp;"="&amp;$B$26&amp;","&amp;$C$1&amp;"="&amp;$C$26&amp;","&amp;$D$1&amp;"="&amp;$D$26&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=25,DegreePlanID=21,TermID=5,RequirementID=20},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=25,DegreePlanID=21,TermID=5,RequirementID=20},</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1">
@@ -5789,14 +5783,14 @@
         <v>692</v>
       </c>
       <c r="E27" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F27" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G27" t="str">
         <f>E27&amp;$A$1&amp;"="&amp;$A$27&amp;","&amp;$B$1&amp;"="&amp;$B$27&amp;","&amp;$C$1&amp;"="&amp;$C$27&amp;","&amp;$D$1&amp;"="&amp;$D$27&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=26,DegreePlanID=21,TermID=5,RequirementID=692},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=26,DegreePlanID=21,TermID=5,RequirementID=692},</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1">
@@ -5813,14 +5807,14 @@
         <v>460</v>
       </c>
       <c r="E28" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F28" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G28" t="str">
         <f>E28&amp;$A$1&amp;"="&amp;$A$28&amp;","&amp;$B$1&amp;"="&amp;$B$28&amp;","&amp;$C$1&amp;"="&amp;$C$28&amp;","&amp;$D$1&amp;"="&amp;$D$28&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=27,DegreePlanID=12,TermID=1,RequirementID=460},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=27,DegreePlanID=12,TermID=1,RequirementID=460},</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1">
@@ -5837,14 +5831,14 @@
         <v>356</v>
       </c>
       <c r="E29" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F29" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G29" t="str">
         <f>E29&amp;$A$1&amp;"="&amp;$A$29&amp;","&amp;$B$1&amp;"="&amp;$B$29&amp;","&amp;$C$1&amp;"="&amp;$C$29&amp;","&amp;$D$1&amp;"="&amp;$D$29&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=28,DegreePlanID=12,TermID=1,RequirementID=356},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=28,DegreePlanID=12,TermID=1,RequirementID=356},</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1">
@@ -5861,14 +5855,14 @@
         <v>542</v>
       </c>
       <c r="E30" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F30" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G30" t="str">
         <f>E30&amp;$A$1&amp;"="&amp;$A$30&amp;","&amp;$B$1&amp;"="&amp;$B$30&amp;","&amp;$C$1&amp;"="&amp;$C$30&amp;","&amp;$D$1&amp;"="&amp;$D$30&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=29,DegreePlanID=12,TermID=1,RequirementID=542},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=29,DegreePlanID=12,TermID=1,RequirementID=542},</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1">
@@ -5885,14 +5879,14 @@
         <v>563</v>
       </c>
       <c r="E31" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F31" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G31" t="str">
         <f>E31&amp;$A$1&amp;"="&amp;$A$31&amp;","&amp;$B$1&amp;"="&amp;$B$31&amp;","&amp;$C$1&amp;"="&amp;$C$31&amp;","&amp;$D$1&amp;"="&amp;$D$31&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=30,DegreePlanID=12,TermID=1,RequirementID=563},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=30,DegreePlanID=12,TermID=1,RequirementID=563},</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="15.75" customHeight="1">
@@ -5909,14 +5903,14 @@
         <v>560</v>
       </c>
       <c r="E32" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F32" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G32" t="str">
         <f>E32&amp;$A$1&amp;"="&amp;$A$32&amp;","&amp;$B$1&amp;"="&amp;$B$32&amp;","&amp;$C$1&amp;"="&amp;$C$32&amp;","&amp;$D$1&amp;"="&amp;$D$32&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=31,DegreePlanID=12,TermID=2,RequirementID=560},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=31,DegreePlanID=12,TermID=2,RequirementID=560},</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="15.75" customHeight="1">
@@ -5933,14 +5927,14 @@
         <v>555</v>
       </c>
       <c r="E33" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F33" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G33" t="str">
         <f>E33&amp;$A$1&amp;"="&amp;$A$33&amp;","&amp;$B$1&amp;"="&amp;$B$33&amp;","&amp;$C$1&amp;"="&amp;$C$33&amp;","&amp;$D$1&amp;"="&amp;$D$33&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=32,DegreePlanID=12,TermID=2,RequirementID=555},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=32,DegreePlanID=12,TermID=2,RequirementID=555},</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="15.75" customHeight="1">
@@ -5957,14 +5951,14 @@
         <v>618</v>
       </c>
       <c r="E34" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F34" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G34" t="str">
         <f>E34&amp;$A$1&amp;"="&amp;$A$34&amp;","&amp;$B$1&amp;"="&amp;$B$34&amp;","&amp;$C$1&amp;"="&amp;$C$34&amp;","&amp;$D$1&amp;"="&amp;$D$34&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=33,DegreePlanID=12,TermID=2,RequirementID=618},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=33,DegreePlanID=12,TermID=2,RequirementID=618},</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="15.75" customHeight="1">
@@ -5981,14 +5975,14 @@
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F35" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G35" t="str">
         <f>E35&amp;$A$1&amp;"="&amp;$A$35&amp;","&amp;$B$1&amp;"="&amp;$B$35&amp;","&amp;$C$1&amp;"="&amp;$C$35&amp;","&amp;$D$1&amp;"="&amp;$D$35&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=34,DegreePlanID=12,TermID=3,RequirementID=1},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=34,DegreePlanID=12,TermID=3,RequirementID=1},</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="15.75" customHeight="1">
@@ -6005,14 +5999,14 @@
         <v>664</v>
       </c>
       <c r="E36" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F36" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G36" t="str">
         <f>E36&amp;$A$1&amp;"="&amp;$A$36&amp;","&amp;$B$1&amp;"="&amp;$B$36&amp;","&amp;$C$1&amp;"="&amp;$C$36&amp;","&amp;$D$1&amp;"="&amp;$D$36&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=35,DegreePlanID=12,TermID=3,RequirementID=664},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=35,DegreePlanID=12,TermID=3,RequirementID=664},</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="15.75" customHeight="1">
@@ -6029,14 +6023,14 @@
         <v>691</v>
       </c>
       <c r="E37" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F37" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G37" t="str">
         <f>E37&amp;$A$1&amp;"="&amp;$A$37&amp;","&amp;$B$1&amp;"="&amp;$B$37&amp;","&amp;$C$1&amp;"="&amp;$C$37&amp;","&amp;$D$1&amp;"="&amp;$D$37&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=36,DegreePlanID=12,TermID=4,RequirementID=691},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=36,DegreePlanID=12,TermID=4,RequirementID=691},</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="15.75" customHeight="1">
@@ -6053,14 +6047,14 @@
         <v>10</v>
       </c>
       <c r="E38" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F38" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G38" t="str">
         <f>E38&amp;$A$1&amp;"="&amp;$A$38&amp;","&amp;$B$1&amp;"="&amp;$B$38&amp;","&amp;$C$1&amp;"="&amp;$C$38&amp;","&amp;$D$1&amp;"="&amp;$D$38&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=37,DegreePlanID=12,TermID=4,RequirementID=10},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=37,DegreePlanID=12,TermID=4,RequirementID=10},</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="15.75" customHeight="1">
@@ -6077,14 +6071,14 @@
         <v>20</v>
       </c>
       <c r="E39" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F39" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G39" t="str">
         <f>E39&amp;$A$1&amp;"="&amp;$A$39&amp;","&amp;$B$1&amp;"="&amp;$B$39&amp;","&amp;$C$1&amp;"="&amp;$C$39&amp;","&amp;$D$1&amp;"="&amp;$D$39&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=38,DegreePlanID=12,TermID=4,RequirementID=20},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=38,DegreePlanID=12,TermID=4,RequirementID=20},</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="15.75" customHeight="1">
@@ -6101,14 +6095,14 @@
         <v>692</v>
       </c>
       <c r="E40" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F40" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G40" t="str">
         <f>E40&amp;$A$1&amp;"="&amp;$A$40&amp;","&amp;$B$1&amp;"="&amp;$B$40&amp;","&amp;$C$1&amp;"="&amp;$C$40&amp;","&amp;$D$1&amp;"="&amp;$D$40&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=39,DegreePlanID=12,TermID=5,RequirementID=692},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=39,DegreePlanID=12,TermID=5,RequirementID=692},</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="15.75" customHeight="1">
@@ -6125,14 +6119,14 @@
         <v>460</v>
       </c>
       <c r="E41" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F41" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G41" t="str">
         <f>E41&amp;$A$1&amp;"="&amp;$A$41&amp;","&amp;$B$1&amp;"="&amp;$B$41&amp;","&amp;$C$1&amp;"="&amp;$C$41&amp;","&amp;$D$1&amp;"="&amp;$D$41&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=40,DegreePlanID=13,TermID=1,RequirementID=460},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=40,DegreePlanID=13,TermID=1,RequirementID=460},</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="15.75" customHeight="1">
@@ -6149,14 +6143,14 @@
         <v>356</v>
       </c>
       <c r="E42" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F42" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G42" t="str">
         <f>E42&amp;$A$1&amp;"="&amp;$A$42&amp;","&amp;$B$1&amp;"="&amp;$B$42&amp;","&amp;$C$1&amp;"="&amp;$C$42&amp;","&amp;$D$1&amp;"="&amp;$D$42&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=41,DegreePlanID=13,TermID=1,RequirementID=356},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=41,DegreePlanID=13,TermID=1,RequirementID=356},</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="15.75" customHeight="1">
@@ -6173,14 +6167,14 @@
         <v>542</v>
       </c>
       <c r="E43" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F43" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G43" t="str">
         <f>E43&amp;$A$1&amp;"="&amp;$A$43&amp;","&amp;$B$1&amp;"="&amp;$B$43&amp;","&amp;$C$1&amp;"="&amp;$C$43&amp;","&amp;$D$1&amp;"="&amp;$D$43&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=42,DegreePlanID=13,TermID=1,RequirementID=542},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=42,DegreePlanID=13,TermID=1,RequirementID=542},</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="15.75" customHeight="1">
@@ -6197,14 +6191,14 @@
         <v>563</v>
       </c>
       <c r="E44" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F44" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G44" t="str">
         <f>E44&amp;$A$1&amp;"="&amp;$A$44&amp;","&amp;$B$1&amp;"="&amp;$B$44&amp;","&amp;$C$1&amp;"="&amp;$C$44&amp;","&amp;$D$1&amp;"="&amp;$D$44&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=43,DegreePlanID=13,TermID=1,RequirementID=563},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=43,DegreePlanID=13,TermID=1,RequirementID=563},</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="15.75" customHeight="1">
@@ -6221,14 +6215,14 @@
         <v>560</v>
       </c>
       <c r="E45" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F45" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G45" t="str">
         <f>E45&amp;$A$1&amp;"="&amp;$A$45&amp;","&amp;$B$1&amp;"="&amp;$B$45&amp;","&amp;$C$1&amp;"="&amp;$C$45&amp;","&amp;$D$1&amp;"="&amp;$D$45&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=44,DegreePlanID=13,TermID=3,RequirementID=560},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=44,DegreePlanID=13,TermID=3,RequirementID=560},</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="15.75" customHeight="1">
@@ -6245,14 +6239,14 @@
         <v>555</v>
       </c>
       <c r="E46" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F46" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G46" t="str">
         <f>E46&amp;$A$1&amp;"="&amp;$A$46&amp;","&amp;$B$1&amp;"="&amp;$B$46&amp;","&amp;$C$1&amp;"="&amp;$C$46&amp;","&amp;$D$1&amp;"="&amp;$D$46&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=45,DegreePlanID=13,TermID=3,RequirementID=555},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=45,DegreePlanID=13,TermID=3,RequirementID=555},</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="15.75" customHeight="1">
@@ -6269,14 +6263,14 @@
         <v>618</v>
       </c>
       <c r="E47" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F47" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G47" t="str">
         <f>E47&amp;$A$1&amp;"="&amp;$A$47&amp;","&amp;$B$1&amp;"="&amp;$B$47&amp;","&amp;$C$1&amp;"="&amp;$C$47&amp;","&amp;$D$1&amp;"="&amp;$D$47&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=46,DegreePlanID=13,TermID=3,RequirementID=618},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=46,DegreePlanID=13,TermID=3,RequirementID=618},</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="15.75" customHeight="1">
@@ -6293,14 +6287,14 @@
         <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F48" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G48" t="str">
         <f>E48&amp;$A$1&amp;"="&amp;$A$48&amp;","&amp;$B$1&amp;"="&amp;$B$48&amp;","&amp;$C$1&amp;"="&amp;$C$48&amp;","&amp;$D$1&amp;"="&amp;$D$48&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=47,DegreePlanID=13,TermID=4,RequirementID=1},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=47,DegreePlanID=13,TermID=4,RequirementID=1},</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="15.75" customHeight="1">
@@ -6317,14 +6311,14 @@
         <v>664</v>
       </c>
       <c r="E49" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F49" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G49" t="str">
         <f>E49&amp;$A$1&amp;"="&amp;$A$49&amp;","&amp;$B$1&amp;"="&amp;$B$49&amp;","&amp;$C$1&amp;"="&amp;$C$49&amp;","&amp;$D$1&amp;"="&amp;$D$49&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=48,DegreePlanID=13,TermID=4,RequirementID=664},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=48,DegreePlanID=13,TermID=4,RequirementID=664},</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="15.75" customHeight="1">
@@ -6341,14 +6335,14 @@
         <v>691</v>
       </c>
       <c r="E50" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F50" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G50" t="str">
         <f>E50&amp;$A$1&amp;"="&amp;$A$50&amp;","&amp;$B$1&amp;"="&amp;$B$50&amp;","&amp;$C$1&amp;"="&amp;$C$50&amp;","&amp;$D$1&amp;"="&amp;$D$50&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=49,DegreePlanID=13,TermID=4,RequirementID=691},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=49,DegreePlanID=13,TermID=4,RequirementID=691},</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="15.75" customHeight="1">
@@ -6365,14 +6359,14 @@
         <v>10</v>
       </c>
       <c r="E51" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F51" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G51" t="str">
         <f>E51&amp;$A$1&amp;"="&amp;$A$51&amp;","&amp;$B$1&amp;"="&amp;$B$51&amp;","&amp;$C$1&amp;"="&amp;$C$51&amp;","&amp;$D$1&amp;"="&amp;$D$51&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=50,DegreePlanID=13,TermID=5,RequirementID=10},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=50,DegreePlanID=13,TermID=5,RequirementID=10},</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="15.75" customHeight="1">
@@ -6389,14 +6383,14 @@
         <v>20</v>
       </c>
       <c r="E52" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F52" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G52" t="str">
         <f>E52&amp;$A$1&amp;"="&amp;$A$52&amp;","&amp;$B$1&amp;"="&amp;$B$52&amp;","&amp;$C$1&amp; "="&amp;$C$52&amp;","&amp;$D$1&amp;"="&amp;$D$52&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=51,DegreePlanID=13,TermID=5,RequirementID=20},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=51,DegreePlanID=13,TermID=5,RequirementID=20},</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="15.75" customHeight="1">
@@ -6413,14 +6407,14 @@
         <v>692</v>
       </c>
       <c r="E53" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F53" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G53" t="str">
         <f>E53&amp;$A$1&amp;"="&amp;$A$53&amp;","&amp;$B$1&amp;"="&amp;$B$53&amp;","&amp;$C$1&amp;"="&amp;$C$53&amp;","&amp;$D$1&amp;"="&amp;$D$53&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=52,DegreePlanID=13,TermID=5,RequirementID=692},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=52,DegreePlanID=13,TermID=5,RequirementID=692},</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="15.75" customHeight="1">
@@ -6437,14 +6431,14 @@
         <v>460</v>
       </c>
       <c r="E54" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F54" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G54" t="str">
         <f>E54&amp;$A$1&amp;"="&amp;$A$54&amp;","&amp;$B$1&amp;"="&amp;$B$54&amp;","&amp;$C$1&amp;"="&amp;$C$54&amp;","&amp;$D$1&amp;"="&amp;$D$54&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=53,DegreePlanID=18,TermID=1,RequirementID=460},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=53,DegreePlanID=18,TermID=1,RequirementID=460},</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="15.75" customHeight="1">
@@ -6461,14 +6455,14 @@
         <v>356</v>
       </c>
       <c r="E55" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F55" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G55" t="str">
         <f>E55&amp;$A$1&amp;"="&amp;$A$55&amp;","&amp;$B$1&amp;"="&amp;$B$55&amp;","&amp;$C$1&amp;"="&amp;$C$55&amp;","&amp;$D$1&amp;"="&amp;$D$55&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=54,DegreePlanID=18,TermID=1,RequirementID=356},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=54,DegreePlanID=18,TermID=1,RequirementID=356},</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="15.75" customHeight="1">
@@ -6485,14 +6479,14 @@
         <v>542</v>
       </c>
       <c r="E56" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F56" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G56" t="str">
         <f>E56&amp;$A$1&amp;"="&amp;$A$56&amp;","&amp;$B$1&amp;"="&amp;$B$56&amp;","&amp;$C$1&amp;"="&amp;$C$56&amp;","&amp;$D$1&amp;"="&amp;$D$56&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=55,DegreePlanID=18,TermID=1,RequirementID=542},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=55,DegreePlanID=18,TermID=1,RequirementID=542},</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="15.75" customHeight="1">
@@ -6509,14 +6503,14 @@
         <v>563</v>
       </c>
       <c r="E57" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F57" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G57" t="str">
         <f>E57&amp;$A$1&amp;"="&amp;$A$57&amp;","&amp;$B$1&amp;"="&amp;$B$57&amp;","&amp;$C$1&amp;"="&amp;$C$57&amp;","&amp;$D$1&amp;"="&amp;$D$57&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=56,DegreePlanID=18,TermID=1,RequirementID=563},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=56,DegreePlanID=18,TermID=1,RequirementID=563},</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="15.75" customHeight="1">
@@ -6533,14 +6527,14 @@
         <v>560</v>
       </c>
       <c r="E58" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F58" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G58" t="str">
         <f>E58&amp;$A$1&amp;"="&amp;$A$58&amp;","&amp;$B$1&amp;"="&amp;$B$58&amp;","&amp;$C$1&amp;"="&amp;$C$58&amp;","&amp;$D$1&amp;"="&amp;$D$58&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=57,DegreePlanID=18,TermID=2,RequirementID=560},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=57,DegreePlanID=18,TermID=2,RequirementID=560},</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="15.75" customHeight="1">
@@ -6557,14 +6551,14 @@
         <v>555</v>
       </c>
       <c r="E59" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F59" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G59" t="str">
         <f>E59&amp;$A$1&amp;"="&amp;$A$59&amp;","&amp;$B$1&amp;"="&amp;$B$59&amp;","&amp;$C$1&amp;"="&amp;$C$59&amp;","&amp;$D$1&amp;"="&amp;$D$59&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=58,DegreePlanID=18,TermID=2,RequirementID=555},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=58,DegreePlanID=18,TermID=2,RequirementID=555},</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="15.75" customHeight="1">
@@ -6581,14 +6575,14 @@
         <v>618</v>
       </c>
       <c r="E60" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F60" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G60" t="str">
         <f>E60&amp;$A$1&amp;"="&amp;$A$60&amp;","&amp;$B$1&amp;"="&amp;$B$60&amp;","&amp;$C$1&amp;"="&amp;$C$60&amp;","&amp;$D$1&amp;"="&amp;$D$60&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=59,DegreePlanID=18,TermID=2,RequirementID=618},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=59,DegreePlanID=18,TermID=2,RequirementID=618},</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="15.75" customHeight="1">
@@ -6605,14 +6599,14 @@
         <v>1</v>
       </c>
       <c r="E61" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F61" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G61" t="str">
         <f>E61&amp;$A$1&amp;"="&amp;$A$61&amp;","&amp;$B$1&amp;"="&amp;$B$61&amp;","&amp;$C$1&amp;"="&amp;$C$61&amp;","&amp;$D$1&amp;"="&amp;$D$61&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=60,DegreePlanID=18,TermID=3,RequirementID=1},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=60,DegreePlanID=18,TermID=3,RequirementID=1},</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="15.75" customHeight="1">
@@ -6629,14 +6623,14 @@
         <v>664</v>
       </c>
       <c r="E62" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F62" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G62" t="str">
         <f>E62&amp;$A$1&amp;"="&amp;$A$62&amp;","&amp;$B$1&amp;"="&amp;$B$62&amp;","&amp;$C$1&amp;"="&amp;$C$62&amp;","&amp;$D$1&amp;"="&amp;$D$62&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=61,DegreePlanID=18,TermID=3,RequirementID=664},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=61,DegreePlanID=18,TermID=3,RequirementID=664},</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="15.75" customHeight="1">
@@ -6653,14 +6647,14 @@
         <v>691</v>
       </c>
       <c r="E63" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F63" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G63" t="str">
         <f>E63&amp;$A$1&amp;"="&amp;$A$63&amp;","&amp;$B$1&amp;"="&amp;$B$63&amp;","&amp;$C$1&amp;"="&amp;$C$63&amp;","&amp;$D$1&amp;"="&amp;$D$63&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=62,DegreePlanID=18,TermID=4,RequirementID=691},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=62,DegreePlanID=18,TermID=4,RequirementID=691},</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="15.75" customHeight="1">
@@ -6677,14 +6671,14 @@
         <v>10</v>
       </c>
       <c r="E64" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F64" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G64" t="str">
         <f>E64&amp;$A$1&amp;"="&amp;$A$64&amp;","&amp;$B$1&amp;"="&amp;$B$64&amp;","&amp;$C$1&amp;"="&amp;$C$64&amp;","&amp;$D$1&amp;"="&amp;$D$64&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=63,DegreePlanID=18,TermID=4,RequirementID=10},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=63,DegreePlanID=18,TermID=4,RequirementID=10},</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="15.75" customHeight="1">
@@ -6701,14 +6695,14 @@
         <v>20</v>
       </c>
       <c r="E65" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F65" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G65" t="str">
         <f>E65&amp;$A$1&amp;"="&amp;$A$65&amp;","&amp;$B$1&amp;"="&amp;$B$65&amp;","&amp;$C$1&amp;"="&amp;$C$65&amp;","&amp;$D$1&amp;"="&amp;$D$65&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=64,DegreePlanID=18,TermID=4,RequirementID=20},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=64,DegreePlanID=18,TermID=4,RequirementID=20},</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="15.75" customHeight="1">
@@ -6725,14 +6719,14 @@
         <v>692</v>
       </c>
       <c r="E66" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F66" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G66" t="str">
         <f>E66&amp;$A$1&amp;"="&amp;$A$66&amp;","&amp;$B$1&amp;"="&amp;$B$66&amp;","&amp;$C$1&amp;"="&amp;$C$66&amp;","&amp;$D$1&amp;"="&amp;$D$66&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=65,DegreePlanID=18,TermID=5,RequirementID=692},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=65,DegreePlanID=18,TermID=5,RequirementID=692},</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="15.75" customHeight="1">
@@ -6749,14 +6743,14 @@
         <v>460</v>
       </c>
       <c r="E67" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F67" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G67" t="str">
         <f>E67&amp;$A$1&amp;"="&amp;$A$67&amp;","&amp;$B$1&amp;"="&amp;$B$67&amp;","&amp;$C$1&amp;"="&amp;$C$67&amp;","&amp;$D$1&amp;"="&amp;$D$67&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=66,DegreePlanID=19,TermID=1,RequirementID=460},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=66,DegreePlanID=19,TermID=1,RequirementID=460},</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="15.75" customHeight="1">
@@ -6773,14 +6767,14 @@
         <v>356</v>
       </c>
       <c r="E68" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F68" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G68" t="str">
         <f>E68&amp;$A$1&amp;"="&amp;$A$68&amp;","&amp;$B$1&amp;"="&amp;$B$68&amp;","&amp;$C$1&amp;"="&amp;$C$68&amp;","&amp;$D$1&amp;"="&amp;$D$68&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=67,DegreePlanID=19,TermID=1,RequirementID=356},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=67,DegreePlanID=19,TermID=1,RequirementID=356},</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="15.75" customHeight="1">
@@ -6797,14 +6791,14 @@
         <v>542</v>
       </c>
       <c r="E69" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F69" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G69" t="str">
         <f>E69&amp;$A$1&amp;"="&amp;$A$69&amp;","&amp;$B$1&amp;"="&amp;$B$69&amp;","&amp;$C$1&amp;"="&amp;$C$69&amp;","&amp;$D$1&amp;"="&amp;$D$69&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=68,DegreePlanID=19,TermID=1,RequirementID=542},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=68,DegreePlanID=19,TermID=1,RequirementID=542},</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="15.75" customHeight="1">
@@ -6821,14 +6815,14 @@
         <v>563</v>
       </c>
       <c r="E70" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F70" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G70" t="str">
         <f>E70&amp;$A$1&amp;"="&amp;$A$70&amp;","&amp;$B$1&amp;"="&amp;$B$70&amp;","&amp;$C$1&amp;"="&amp;$C$70&amp;","&amp;$D$1&amp;"="&amp;$D$70&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=69,DegreePlanID=19,TermID=1,RequirementID=563},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=69,DegreePlanID=19,TermID=1,RequirementID=563},</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="15.75" customHeight="1">
@@ -6845,14 +6839,14 @@
         <v>560</v>
       </c>
       <c r="E71" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F71" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G71" t="str">
         <f>E71&amp;$A$1&amp;"="&amp;$A$71&amp;","&amp;$B$1&amp;"="&amp;$B$71&amp;","&amp;$C$1&amp;"="&amp;$C$71&amp;","&amp;$D$1&amp;"="&amp;$D$71&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=70,DegreePlanID=19,TermID=3,RequirementID=560},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=70,DegreePlanID=19,TermID=3,RequirementID=560},</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="15.75" customHeight="1">
@@ -6869,14 +6863,14 @@
         <v>555</v>
       </c>
       <c r="E72" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F72" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G72" t="str">
         <f>E72&amp;$A$1&amp;"="&amp;$A$72&amp;","&amp;$B$1&amp;"="&amp;$B$72&amp;","&amp;$C$1&amp;"="&amp;$C$72&amp;","&amp;$D$1&amp;"="&amp;$D$72&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=71,DegreePlanID=19,TermID=3,RequirementID=555},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=71,DegreePlanID=19,TermID=3,RequirementID=555},</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="15.75" customHeight="1">
@@ -6893,14 +6887,14 @@
         <v>618</v>
       </c>
       <c r="E73" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F73" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G73" t="str">
         <f>E73&amp;$A$1&amp;"="&amp;$A$73&amp;","&amp;$B$1&amp;"="&amp;$B$73&amp;","&amp;$C$1&amp;"="&amp;$C$73&amp;","&amp;$D$1&amp;"="&amp;$D$73&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=72,DegreePlanID=19,TermID=3,RequirementID=618},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=72,DegreePlanID=19,TermID=3,RequirementID=618},</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="15.75" customHeight="1">
@@ -6917,14 +6911,14 @@
         <v>1</v>
       </c>
       <c r="E74" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F74" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G74" t="str">
         <f>E74&amp;$A$1&amp;"="&amp;$A$74&amp;","&amp;$B$1&amp;"="&amp;$B$74&amp;","&amp;$C$1&amp;"="&amp;$C$74&amp;","&amp;$D$1&amp;"="&amp;$D$74&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=73,DegreePlanID=19,TermID=4,RequirementID=1},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=73,DegreePlanID=19,TermID=4,RequirementID=1},</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="15.75" customHeight="1">
@@ -6941,14 +6935,14 @@
         <v>664</v>
       </c>
       <c r="E75" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F75" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G75" t="str">
         <f>E75&amp;$A$1&amp;"="&amp;$A$75&amp;","&amp;$B$1&amp;"="&amp;$B$75&amp;","&amp;$C$1&amp;"="&amp;$C$75&amp;","&amp;$D$1&amp;"="&amp;$D$75&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=74,DegreePlanID=19,TermID=4,RequirementID=664},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=74,DegreePlanID=19,TermID=4,RequirementID=664},</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="15.75" customHeight="1">
@@ -6965,14 +6959,14 @@
         <v>691</v>
       </c>
       <c r="E76" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F76" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G76" t="str">
         <f>E76&amp;$A$1&amp;"="&amp;$A$76&amp;","&amp;$B$1&amp;"="&amp;$B$76&amp;","&amp;$C$1&amp;"="&amp;$C$76&amp;","&amp;$D$1&amp;"="&amp;$D$76&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=75,DegreePlanID=19,TermID=4,RequirementID=691},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=75,DegreePlanID=19,TermID=4,RequirementID=691},</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="15.75" customHeight="1">
@@ -6989,14 +6983,14 @@
         <v>10</v>
       </c>
       <c r="E77" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F77" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G77" t="str">
         <f>E77&amp;$A$1&amp;"="&amp;$A$77&amp;","&amp;$B$1&amp;"="&amp;$B$77&amp;","&amp;$C$1&amp;"="&amp;$C$77&amp;","&amp;$D$1&amp;"="&amp;$D$77&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=76,DegreePlanID=19,TermID=5,RequirementID=10},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=76,DegreePlanID=19,TermID=5,RequirementID=10},</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="15.75" customHeight="1">
@@ -7013,14 +7007,14 @@
         <v>20</v>
       </c>
       <c r="E78" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F78" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G78" t="str">
         <f>E78&amp;$A$1&amp;"="&amp;$A$78&amp;","&amp;$B$1&amp;"="&amp;$B$78&amp;","&amp;$C$1&amp;"="&amp;$C$78&amp;","&amp;$D$1&amp;"="&amp;$D$78&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=77,DegreePlanID=19,TermID=5,RequirementID=20},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=77,DegreePlanID=19,TermID=5,RequirementID=20},</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="15.75" customHeight="1">
@@ -7037,14 +7031,14 @@
         <v>692</v>
       </c>
       <c r="E79" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F79" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G79" t="str">
         <f>E79&amp;$A$1&amp;"="&amp;$A$79&amp;","&amp;$B$1&amp;"="&amp;$B$79&amp;","&amp;$C$1&amp;"="&amp;$C$79&amp;","&amp;$D$1&amp;"="&amp;$D$79&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=78,DegreePlanID=19,TermID=5,RequirementID=692},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=78,DegreePlanID=19,TermID=5,RequirementID=692},</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="15.75" customHeight="1">
@@ -7061,14 +7055,14 @@
         <v>460</v>
       </c>
       <c r="E80" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F80" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G80" t="str">
         <f>E80&amp;$A$1&amp;"="&amp;$A$80&amp;","&amp;$B$1&amp;"="&amp;$B$80&amp;","&amp;$C$1&amp;"="&amp;$C$80&amp;","&amp;$D$1&amp;"="&amp;$D$80&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=79,DegreePlanID=16,TermID=1,RequirementID=460},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=79,DegreePlanID=16,TermID=1,RequirementID=460},</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="15.75" customHeight="1">
@@ -7085,14 +7079,14 @@
         <v>356</v>
       </c>
       <c r="E81" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F81" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G81" t="str">
         <f>E81&amp;$A$1&amp;"="&amp;$A$81&amp;","&amp;$B$1&amp;"="&amp;$B$81&amp;","&amp;$C$1&amp;"="&amp;$C$81&amp;","&amp;$D$1&amp;"="&amp;$D$81&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=80,DegreePlanID=16,TermID=1,RequirementID=356},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=80,DegreePlanID=16,TermID=1,RequirementID=356},</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="15.75" customHeight="1">
@@ -7109,14 +7103,14 @@
         <v>542</v>
       </c>
       <c r="E82" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F82" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G82" t="str">
         <f>E82&amp;$A$1&amp;"="&amp;$A$82&amp;","&amp;$B$1&amp;"="&amp;$B$82&amp;","&amp;$C$1&amp;"="&amp;$C$82&amp;","&amp;$D$1&amp;"="&amp;$D$82&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=81,DegreePlanID=16,TermID=1,RequirementID=542},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=81,DegreePlanID=16,TermID=1,RequirementID=542},</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="15.75" customHeight="1">
@@ -7133,14 +7127,14 @@
         <v>563</v>
       </c>
       <c r="E83" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F83" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G83" t="str">
         <f>E83&amp;$A$1&amp;"="&amp;$A$83&amp;","&amp;$B$1&amp;"="&amp;$B$83&amp;","&amp;$C$1&amp;"="&amp;$C$83&amp;","&amp;$D$1&amp;"="&amp;$D$83&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=82,DegreePlanID=16,TermID=1,RequirementID=563},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=82,DegreePlanID=16,TermID=1,RequirementID=563},</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="15.75" customHeight="1">
@@ -7157,14 +7151,14 @@
         <v>560</v>
       </c>
       <c r="E84" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F84" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G84" t="str">
         <f>E84&amp;$A$1&amp;"="&amp;$A$84&amp;","&amp;$B$1&amp;"="&amp;$B$84&amp;","&amp;$C$1&amp;"="&amp;$C$84&amp;","&amp;$D$1&amp;"="&amp;$D$84&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=83,DegreePlanID=16,TermID=2,RequirementID=560},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=83,DegreePlanID=16,TermID=2,RequirementID=560},</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="15.75" customHeight="1">
@@ -7181,14 +7175,14 @@
         <v>555</v>
       </c>
       <c r="E85" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F85" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G85" t="str">
         <f>E85&amp;$A$1&amp;"="&amp;$A$85&amp;","&amp;$B$1&amp;"="&amp;$B$85&amp;","&amp;$C$1&amp;"="&amp;$C$85&amp;","&amp;$D$1&amp;"="&amp;$D$85&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=84,DegreePlanID=16,TermID=2,RequirementID=555},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=84,DegreePlanID=16,TermID=2,RequirementID=555},</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="15.75" customHeight="1">
@@ -7205,14 +7199,14 @@
         <v>618</v>
       </c>
       <c r="E86" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F86" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G86" t="str">
         <f>E86&amp;$A$1&amp;"="&amp;$A$86&amp;","&amp;$B$1&amp;"="&amp;$B$86&amp;","&amp;$C$1&amp;"="&amp;$C$86&amp;","&amp;$D$1&amp;"="&amp;$D$86&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=85,DegreePlanID=16,TermID=2,RequirementID=618},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=85,DegreePlanID=16,TermID=2,RequirementID=618},</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="15.75" customHeight="1">
@@ -7229,14 +7223,14 @@
         <v>1</v>
       </c>
       <c r="E87" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F87" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G87" t="str">
         <f>E87&amp;$A$1&amp;"="&amp;$A$87&amp;","&amp;$B$1&amp;"="&amp;$B$87&amp;","&amp;$C$1&amp;"="&amp;$C$87&amp;","&amp;$D$1&amp;"="&amp;$D$87&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=86,DegreePlanID=16,TermID=3,RequirementID=1},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=86,DegreePlanID=16,TermID=3,RequirementID=1},</v>
       </c>
     </row>
     <row r="88" spans="1:7" ht="15.75" customHeight="1">
@@ -7253,14 +7247,14 @@
         <v>664</v>
       </c>
       <c r="E88" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F88" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G88" t="str">
         <f>E88&amp;$A$1&amp;"="&amp;$A$88&amp;","&amp;$B$1&amp;"="&amp;$B$88&amp;","&amp;$C$1&amp;"="&amp;$C$88&amp;","&amp;$D$1&amp;"="&amp;$D$88&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=87,DegreePlanID=16,TermID=3,RequirementID=664},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=87,DegreePlanID=16,TermID=3,RequirementID=664},</v>
       </c>
     </row>
     <row r="89" spans="1:7" ht="15.75" customHeight="1">
@@ -7277,14 +7271,14 @@
         <v>691</v>
       </c>
       <c r="E89" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F89" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G89" t="str">
         <f>E89&amp;$A$1&amp;"="&amp;$A$89&amp;","&amp;$B$1&amp;"="&amp;$B$89&amp;","&amp;$C$1&amp;"="&amp;$C$89&amp;","&amp;$D$1&amp;"="&amp;$D$89&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=88,DegreePlanID=16,TermID=3,RequirementID=691},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=88,DegreePlanID=16,TermID=3,RequirementID=691},</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="15.75" customHeight="1">
@@ -7301,14 +7295,14 @@
         <v>10</v>
       </c>
       <c r="E90" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F90" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G90" t="str">
         <f>E90&amp;$A$1&amp;"="&amp;$A$90&amp;","&amp;$B$1&amp;"="&amp;$B$90&amp;","&amp;$C$1&amp;"="&amp;$C$90&amp;","&amp;$D$1&amp;"="&amp;$D$90&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=89,DegreePlanID=16,TermID=4,RequirementID=10},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=89,DegreePlanID=16,TermID=4,RequirementID=10},</v>
       </c>
     </row>
     <row r="91" spans="1:7" ht="15.75" customHeight="1">
@@ -7325,14 +7319,14 @@
         <v>20</v>
       </c>
       <c r="E91" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F91" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G91" t="str">
         <f>E91&amp;$A$1&amp;"="&amp;$A$91&amp;","&amp;$B$1&amp;"="&amp;$B$91&amp;","&amp;$C$1&amp;"="&amp;$C$91&amp;","&amp;$D$1&amp;"="&amp;$D$91&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=90,DegreePlanID=16,TermID=4,RequirementID=20},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=90,DegreePlanID=16,TermID=4,RequirementID=20},</v>
       </c>
     </row>
     <row r="92" spans="1:7" ht="15.75" customHeight="1">
@@ -7349,14 +7343,14 @@
         <v>692</v>
       </c>
       <c r="E92" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F92" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G92" t="str">
         <f>E92&amp;$A$1&amp;"="&amp;$A$92&amp;","&amp;$B$1&amp;"="&amp;$B$92&amp;","&amp;$C$1&amp;"="&amp;$C$92&amp;","&amp;$D$1&amp;"="&amp;$D$92&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=91,DegreePlanID=16,TermID=5,RequirementID=692},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=91,DegreePlanID=16,TermID=5,RequirementID=692},</v>
       </c>
     </row>
     <row r="93" spans="1:7" ht="15.75" customHeight="1">
@@ -7373,14 +7367,14 @@
         <v>460</v>
       </c>
       <c r="E93" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F93" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G93" t="str">
         <f>E93&amp;$A$1&amp;"="&amp;$A$93&amp;","&amp;$B$1&amp;"="&amp;$B$93&amp;","&amp;$C$1&amp;"="&amp;$C$93&amp;","&amp;$D$1&amp;"="&amp;$D$93&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=92,DegreePlanID=17,TermID=1,RequirementID=460},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=92,DegreePlanID=17,TermID=1,RequirementID=460},</v>
       </c>
     </row>
     <row r="94" spans="1:7" ht="15.75" customHeight="1">
@@ -7397,14 +7391,14 @@
         <v>356</v>
       </c>
       <c r="E94" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F94" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G94" t="str">
         <f>E94&amp;$A$1&amp;"="&amp;$A$94&amp;","&amp;$B$1&amp;"="&amp;$B$94&amp;","&amp;$C$1&amp;"="&amp;$C$94&amp;","&amp;$D$1&amp;"="&amp;$D$94&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=93,DegreePlanID=17,TermID=1,RequirementID=356},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=93,DegreePlanID=17,TermID=1,RequirementID=356},</v>
       </c>
     </row>
     <row r="95" spans="1:7" ht="15.75" customHeight="1">
@@ -7421,14 +7415,14 @@
         <v>542</v>
       </c>
       <c r="E95" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F95" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G95" t="str">
         <f>E95&amp;$A$1&amp;"="&amp;$A$95&amp;","&amp;$B$1&amp;"="&amp;$B$95&amp;","&amp;$C$1&amp;"="&amp;$C$95&amp;","&amp;$D$1&amp;"="&amp;$D$95&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=94,DegreePlanID=17,TermID=1,RequirementID=542},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=94,DegreePlanID=17,TermID=1,RequirementID=542},</v>
       </c>
     </row>
     <row r="96" spans="1:7" ht="15.75" customHeight="1">
@@ -7445,14 +7439,14 @@
         <v>563</v>
       </c>
       <c r="E96" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F96" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G96" t="str">
         <f>E96&amp;$A$1&amp;"="&amp;$A$96&amp;","&amp;$B$1&amp;"="&amp;$B$96&amp;","&amp;$C$1&amp;"="&amp;$C$96&amp;","&amp;$D$1&amp;"="&amp;$D$96&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=95,DegreePlanID=17,TermID=1,RequirementID=563},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=95,DegreePlanID=17,TermID=1,RequirementID=563},</v>
       </c>
     </row>
     <row r="97" spans="1:7" ht="15.75" customHeight="1">
@@ -7469,14 +7463,14 @@
         <v>560</v>
       </c>
       <c r="E97" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F97" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G97" t="str">
         <f>E97&amp;$A$1&amp;"="&amp;$A$97&amp;","&amp;$B$1&amp;"="&amp;$B$97&amp;","&amp;$C$1&amp;"="&amp;$C$97&amp;","&amp;$D$1&amp;"="&amp;$D$97&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=96,DegreePlanID=17,TermID=2,RequirementID=560},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=96,DegreePlanID=17,TermID=2,RequirementID=560},</v>
       </c>
     </row>
     <row r="98" spans="1:7" ht="15.75" customHeight="1">
@@ -7493,14 +7487,14 @@
         <v>555</v>
       </c>
       <c r="E98" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F98" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G98" t="str">
         <f>E98&amp;$A$1&amp;"="&amp;$A$98&amp;","&amp;$B$1&amp;"="&amp;$B$98&amp;","&amp;$C$1&amp;"="&amp;$C$98&amp;","&amp;$D$1&amp;"="&amp;$D$98&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=97,DegreePlanID=17,TermID=2,RequirementID=555},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=97,DegreePlanID=17,TermID=2,RequirementID=555},</v>
       </c>
     </row>
     <row r="99" spans="1:7" ht="15.75" customHeight="1">
@@ -7517,14 +7511,14 @@
         <v>618</v>
       </c>
       <c r="E99" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F99" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G99" t="str">
         <f>E99&amp;$A$1&amp;"="&amp;$A$99&amp;","&amp;$B$1&amp;"="&amp;$B$99&amp;","&amp;$C$1&amp;"="&amp;$C$99&amp;","&amp;$D$1&amp;"="&amp;$D$99&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=98,DegreePlanID=17,TermID=2,RequirementID=618},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=98,DegreePlanID=17,TermID=2,RequirementID=618},</v>
       </c>
     </row>
     <row r="100" spans="1:7" ht="15.75" customHeight="1">
@@ -7541,14 +7535,14 @@
         <v>1</v>
       </c>
       <c r="E100" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F100" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G100" t="str">
         <f>E100&amp;$A$1&amp;"="&amp;$A$100&amp;","&amp;$B$1&amp;"="&amp;$B$100&amp;","&amp;$C$1&amp;"="&amp;$C$100&amp;","&amp;$D$1&amp;"="&amp;$D$100&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=99,DegreePlanID=17,TermID=4,RequirementID=1},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=99,DegreePlanID=17,TermID=4,RequirementID=1},</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="15.75" customHeight="1">
@@ -7565,14 +7559,14 @@
         <v>664</v>
       </c>
       <c r="E101" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F101" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G101" t="str">
         <f>E101&amp;$A$1&amp;"="&amp;$A$101&amp;","&amp;$B$1&amp;"="&amp;$B$101&amp;","&amp;$C$1&amp;"="&amp;$C$101&amp;","&amp;$D$1&amp;"="&amp;$D$101&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=100,DegreePlanID=17,TermID=4,RequirementID=664},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=100,DegreePlanID=17,TermID=4,RequirementID=664},</v>
       </c>
     </row>
     <row r="102" spans="1:7" ht="15.75" customHeight="1">
@@ -7589,14 +7583,14 @@
         <v>691</v>
       </c>
       <c r="E102" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F102" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G102" t="str">
         <f>E102&amp;$A$1&amp;"="&amp;$A$102&amp;","&amp;$B$1&amp;"="&amp;$B$102&amp;","&amp;$C$1&amp;"="&amp;$C$102&amp;","&amp;$D$1&amp;"="&amp;$D$102&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=101,DegreePlanID=17,TermID=4,RequirementID=691},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=101,DegreePlanID=17,TermID=4,RequirementID=691},</v>
       </c>
     </row>
     <row r="103" spans="1:7" ht="15.75" customHeight="1">
@@ -7613,14 +7607,14 @@
         <v>10</v>
       </c>
       <c r="E103" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F103" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G103" t="str">
         <f>E103&amp;$A$1&amp;"="&amp;$A$103&amp;","&amp;$B$1&amp;"="&amp;$B$103&amp;","&amp;$C$1&amp;"="&amp;$C$103&amp;","&amp;$D$1&amp;"="&amp;$D$103&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=102,DegreePlanID=17,TermID=5,RequirementID=10},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=102,DegreePlanID=17,TermID=5,RequirementID=10},</v>
       </c>
     </row>
     <row r="104" spans="1:7" ht="15.75" customHeight="1">
@@ -7637,14 +7631,14 @@
         <v>20</v>
       </c>
       <c r="E104" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F104" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G104" t="str">
         <f>E104&amp;$A$1&amp;"="&amp;$A$104&amp;","&amp;$B$1&amp;"="&amp;$B$104&amp;","&amp;$C$1&amp;"="&amp;$C$104&amp;","&amp;$D$1&amp;"="&amp;$D$104&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=103,DegreePlanID=17,TermID=5,RequirementID=20},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=103,DegreePlanID=17,TermID=5,RequirementID=20},</v>
       </c>
     </row>
     <row r="105" spans="1:7" ht="15.75" customHeight="1">
@@ -7661,14 +7655,14 @@
         <v>692</v>
       </c>
       <c r="E105" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F105" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G105" t="str">
         <f>E105&amp;$A$1&amp;"="&amp;$A$105&amp;","&amp;$B$1&amp;"="&amp;$B$105&amp;","&amp;$C$1&amp;"="&amp;$C$105&amp;","&amp;$D$1&amp;"="&amp;$D$105&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=104,DegreePlanID=17,TermID=5,RequirementID=692},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=104,DegreePlanID=17,TermID=5,RequirementID=692},</v>
       </c>
     </row>
     <row r="106" spans="1:7" ht="15.75" customHeight="1">
@@ -7685,14 +7679,14 @@
         <v>460</v>
       </c>
       <c r="E106" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F106" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G106" t="str">
         <f>E106&amp;$A$1&amp;"="&amp;$A$106&amp;","&amp;$B$1&amp;"="&amp;$B$106&amp;","&amp;$C$1&amp;"="&amp;$C$106&amp;","&amp;$D$1&amp;"="&amp;$D$106&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=105,DegreePlanID=14,TermID=1,RequirementID=460},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=105,DegreePlanID=14,TermID=1,RequirementID=460},</v>
       </c>
     </row>
     <row r="107" spans="1:7" ht="15.75" customHeight="1">
@@ -7709,14 +7703,14 @@
         <v>356</v>
       </c>
       <c r="E107" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F107" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G107" t="str">
         <f>E107&amp;$A$1&amp;"="&amp;$A$107&amp;","&amp;$B$1&amp;"="&amp;$B$107&amp;","&amp;$C$1&amp;"="&amp;$C$107&amp;","&amp;$D$1&amp;"="&amp;$D$107&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=106,DegreePlanID=14,TermID=1,RequirementID=356},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=106,DegreePlanID=14,TermID=1,RequirementID=356},</v>
       </c>
     </row>
     <row r="108" spans="1:7" ht="15.75" customHeight="1">
@@ -7733,14 +7727,14 @@
         <v>542</v>
       </c>
       <c r="E108" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F108" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G108" t="str">
         <f>E108&amp;$A$1&amp;"="&amp;$A$108&amp;","&amp;$B$1&amp;"="&amp;$B$108&amp;","&amp;$C$1&amp;"="&amp;$C$108&amp;","&amp;$D$1&amp;"="&amp;$D$108&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=107,DegreePlanID=15,TermID=1,RequirementID=542},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=107,DegreePlanID=15,TermID=1,RequirementID=542},</v>
       </c>
     </row>
     <row r="109" spans="1:7" ht="15.75" customHeight="1">
@@ -7757,14 +7751,14 @@
         <v>563</v>
       </c>
       <c r="E109" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F109" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G109" t="str">
         <f>E109&amp;$A$1&amp;"="&amp;$A$109&amp;","&amp;$B$1&amp;"="&amp;$B$109&amp;","&amp;$C$1&amp;"="&amp;$C$109&amp;","&amp;$D$1&amp;"="&amp;$D$109&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=108,DegreePlanID=15,TermID=1,RequirementID=563},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=108,DegreePlanID=15,TermID=1,RequirementID=563},</v>
       </c>
     </row>
     <row r="110" spans="1:7" ht="15.75" customHeight="1">
@@ -7781,14 +7775,14 @@
         <v>560</v>
       </c>
       <c r="E110" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F110" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G110" t="str">
         <f>E110&amp;$A$1&amp;"="&amp;$A$110&amp;","&amp;$B$1&amp;"="&amp;$B$110&amp;","&amp;$C$1&amp;"="&amp;$C$110&amp;","&amp;$D$1&amp;"="&amp;$D$110&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=109,DegreePlanID=15,TermID=2,RequirementID=560},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=109,DegreePlanID=15,TermID=2,RequirementID=560},</v>
       </c>
     </row>
     <row r="111" spans="1:7" ht="15.75" customHeight="1">
@@ -7805,14 +7799,14 @@
         <v>555</v>
       </c>
       <c r="E111" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F111" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G111" t="str">
         <f>E111&amp;$A$1&amp;"="&amp;$A$111&amp;","&amp;$B$1&amp;"="&amp;$B$111&amp;","&amp;$C$1&amp;"="&amp;$C$111&amp;","&amp;$D$1&amp;"="&amp;$D$111&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=110,DegreePlanID=15,TermID=2,RequirementID=555},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=110,DegreePlanID=15,TermID=2,RequirementID=555},</v>
       </c>
     </row>
     <row r="112" spans="1:7" ht="15.75" customHeight="1">
@@ -7829,14 +7823,14 @@
         <v>618</v>
       </c>
       <c r="E112" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F112" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G112" t="str">
         <f>E112&amp;$A$1&amp;"="&amp;$A$112&amp;","&amp;$B$1&amp;"="&amp;$B$112&amp;","&amp;$C$1&amp;"="&amp;$C$112&amp;","&amp;$D$1&amp;"="&amp;$D$112&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=111,DegreePlanID=15,TermID=2,RequirementID=618},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=111,DegreePlanID=15,TermID=2,RequirementID=618},</v>
       </c>
     </row>
     <row r="113" spans="1:7" ht="15.75" customHeight="1">
@@ -7853,14 +7847,14 @@
         <v>1</v>
       </c>
       <c r="E113" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F113" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G113" t="str">
         <f>E113&amp;$A$1&amp;"="&amp;$A$113&amp;","&amp;$B$1&amp;"="&amp;$B$113&amp;","&amp;$C$1&amp;"="&amp;$C$113&amp;","&amp;$D$1&amp;"="&amp;$D$113&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=112,DegreePlanID=15,TermID=3,RequirementID=1},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=112,DegreePlanID=15,TermID=3,RequirementID=1},</v>
       </c>
     </row>
     <row r="114" spans="1:7" ht="15.75" customHeight="1">
@@ -7877,14 +7871,14 @@
         <v>664</v>
       </c>
       <c r="E114" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F114" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G114" t="str">
         <f>E114&amp;$A$1&amp;"="&amp;$A$114&amp;","&amp;$B$1&amp;"="&amp;$B$114&amp;","&amp;$C$1&amp;"="&amp;$C$114&amp;","&amp;$D$1&amp;"="&amp;$D$114&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=113,DegreePlanID=15,TermID=3,RequirementID=664},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=113,DegreePlanID=15,TermID=3,RequirementID=664},</v>
       </c>
     </row>
     <row r="115" spans="1:7" ht="15.75" customHeight="1">
@@ -7901,14 +7895,14 @@
         <v>691</v>
       </c>
       <c r="E115" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F115" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G115" t="str">
         <f>E115&amp;$A$1&amp;"="&amp;$A$115&amp;","&amp;$B$1&amp;"="&amp;$B$115&amp;","&amp;$C$1&amp;"="&amp;$C$115&amp;","&amp;$D$1&amp;"="&amp;$D$115&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=114,DegreePlanID=15,TermID=4,RequirementID=691},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=114,DegreePlanID=15,TermID=4,RequirementID=691},</v>
       </c>
     </row>
     <row r="116" spans="1:7" ht="15.75" customHeight="1">
@@ -7925,14 +7919,14 @@
         <v>10</v>
       </c>
       <c r="E116" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F116" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G116" t="str">
         <f>E116&amp;$A$1&amp;"="&amp;$A$116&amp;","&amp;$B$1&amp;"="&amp;$B$116&amp;","&amp;$C$1&amp;"="&amp;$C$116&amp;","&amp;$D$1&amp;"="&amp;$D$116&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=115,DegreePlanID=15,TermID=4,RequirementID=10},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=115,DegreePlanID=15,TermID=4,RequirementID=10},</v>
       </c>
     </row>
     <row r="117" spans="1:7" ht="15.75" customHeight="1">
@@ -7949,14 +7943,14 @@
         <v>20</v>
       </c>
       <c r="E117" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F117" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G117" t="str">
         <f>E117&amp;$A$1&amp;"="&amp;$A$117&amp;","&amp;$B$1&amp;"="&amp;$B$117&amp;","&amp;$C$1&amp;"="&amp;$C$117&amp;","&amp;$D$1&amp;"="&amp;$D$117&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=116,DegreePlanID=15,TermID=4,RequirementID=20},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=116,DegreePlanID=15,TermID=4,RequirementID=20},</v>
       </c>
     </row>
     <row r="118" spans="1:7" ht="15.75" customHeight="1">
@@ -7973,14 +7967,14 @@
         <v>692</v>
       </c>
       <c r="E118" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F118" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G118" t="str">
         <f>E118&amp;$A$1&amp;"="&amp;$A$118&amp;","&amp;$B$1&amp;"="&amp;$B$118&amp;","&amp;$C$1&amp;"="&amp;$C$118&amp;","&amp;$D$1&amp;"="&amp;$D$118&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=117,DegreePlanID=15,TermID=5,RequirementID=692},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=117,DegreePlanID=15,TermID=5,RequirementID=692},</v>
       </c>
     </row>
     <row r="119" spans="1:7" ht="15.75" customHeight="1">
@@ -7997,14 +7991,14 @@
         <v>460</v>
       </c>
       <c r="E119" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F119" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G119" t="str">
         <f>E119&amp;$A$1&amp;"="&amp;$A$119&amp;","&amp;$B$1&amp;"="&amp;$B$119&amp;","&amp;$C$1&amp;"="&amp;$C$119&amp;","&amp;$D$1&amp;"="&amp;$D$119&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=118,DegreePlanID=15,TermID=1,RequirementID=460},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=118,DegreePlanID=15,TermID=1,RequirementID=460},</v>
       </c>
     </row>
     <row r="120" spans="1:7" ht="15.75" customHeight="1">
@@ -8021,14 +8015,14 @@
         <v>356</v>
       </c>
       <c r="E120" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F120" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G120" t="str">
         <f>E120&amp;$A$1&amp;"="&amp;$A$120&amp;","&amp;$B$1&amp;"="&amp;$B$120&amp;","&amp;$C$1&amp;"="&amp;$C$120&amp;","&amp;$D$1&amp;"="&amp;$D$120&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=119,DegreePlanID=15,TermID=1,RequirementID=356},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=119,DegreePlanID=15,TermID=1,RequirementID=356},</v>
       </c>
     </row>
     <row r="121" spans="1:7" ht="15.75" customHeight="1">
@@ -8045,14 +8039,14 @@
         <v>542</v>
       </c>
       <c r="E121" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F121" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G121" t="str">
         <f>E121&amp;$A$1&amp;"="&amp;$A$121&amp;","&amp;$B$1&amp;"="&amp;$B$121&amp;","&amp;$C$1&amp;"="&amp;$C$121&amp;","&amp;$D$1&amp;"="&amp;$D$121&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=120,DegreePlanID=15,TermID=1,RequirementID=542},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=120,DegreePlanID=15,TermID=1,RequirementID=542},</v>
       </c>
     </row>
     <row r="122" spans="1:7" ht="15.75" customHeight="1">
@@ -8069,14 +8063,14 @@
         <v>563</v>
       </c>
       <c r="E122" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F122" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G122" t="str">
         <f>E122&amp;$A$1&amp;"="&amp;$A$122&amp;","&amp;$B$1&amp;"="&amp;$B$122&amp;","&amp;$C$1&amp;"="&amp;$C$122&amp;","&amp;$D$1&amp;"="&amp;$D$122&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=121,DegreePlanID=15,TermID=1,RequirementID=563},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=121,DegreePlanID=15,TermID=1,RequirementID=563},</v>
       </c>
     </row>
     <row r="123" spans="1:7" ht="15.75" customHeight="1">
@@ -8093,14 +8087,14 @@
         <v>560</v>
       </c>
       <c r="E123" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F123" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G123" t="str">
         <f>E123&amp;$A$1&amp;"="&amp;$A$123&amp;","&amp;$B$1&amp;"="&amp;$B$123&amp;","&amp;$C$1&amp;"="&amp;$C$123&amp;","&amp;$D$1&amp;"="&amp;$D$123&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=122,DegreePlanID=15,TermID=3,RequirementID=560},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=122,DegreePlanID=15,TermID=3,RequirementID=560},</v>
       </c>
     </row>
     <row r="124" spans="1:7" ht="15.75" customHeight="1">
@@ -8117,14 +8111,14 @@
         <v>555</v>
       </c>
       <c r="E124" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F124" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G124" t="str">
         <f>E124&amp;$A$1&amp;"="&amp;$A$124&amp;","&amp;$B$1&amp;"="&amp;$B$124&amp;","&amp;$C$1&amp;"="&amp;$C$124&amp;","&amp;$D$1&amp;"="&amp;$D$124&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=123,DegreePlanID=15,TermID=3,RequirementID=555},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=123,DegreePlanID=15,TermID=3,RequirementID=555},</v>
       </c>
     </row>
     <row r="125" spans="1:7" ht="15.75" customHeight="1">
@@ -8141,14 +8135,14 @@
         <v>618</v>
       </c>
       <c r="E125" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F125" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G125" t="str">
         <f>E125&amp;$A$1&amp;"="&amp;$A$125&amp;","&amp;$B$1&amp;"="&amp;$B$125&amp;","&amp;$C$1&amp;"="&amp;$C$125&amp;","&amp;$D$1&amp;"="&amp;$D$125&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=124,DegreePlanID=15,TermID=3,RequirementID=618},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=124,DegreePlanID=15,TermID=3,RequirementID=618},</v>
       </c>
     </row>
     <row r="126" spans="1:7" ht="15.75" customHeight="1">
@@ -8165,14 +8159,14 @@
         <v>1</v>
       </c>
       <c r="E126" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F126" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G126" t="str">
         <f>E126&amp;$A$1&amp;"="&amp;$A$126&amp;","&amp;$B$1&amp;"="&amp;$B$126&amp;","&amp;$C$1&amp;"="&amp;$C$126&amp;","&amp;$D$1&amp;"="&amp;$D$126&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=125,DegreePlanID=15,TermID=4,RequirementID=1},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=125,DegreePlanID=15,TermID=4,RequirementID=1},</v>
       </c>
     </row>
     <row r="127" spans="1:7" ht="15.75" customHeight="1">
@@ -8189,14 +8183,14 @@
         <v>664</v>
       </c>
       <c r="E127" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F127" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G127" t="str">
         <f>E127&amp;$A$1&amp;"="&amp;$A$127&amp;","&amp;$B$1&amp;"="&amp;$B$127&amp;","&amp;$C$1&amp;"="&amp;$C$127&amp;","&amp;$D$1&amp;"="&amp;$D$127&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=126,DegreePlanID=15,TermID=4,RequirementID=664},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=126,DegreePlanID=15,TermID=4,RequirementID=664},</v>
       </c>
     </row>
     <row r="128" spans="1:7" ht="15.75" customHeight="1">
@@ -8213,14 +8207,14 @@
         <v>691</v>
       </c>
       <c r="E128" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F128" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G128" t="str">
         <f>E128&amp;$A$1&amp;"="&amp;$A$128&amp;","&amp;$B$1&amp;"="&amp;$B$128&amp;","&amp;$C$1&amp;"="&amp;$C$128&amp;","&amp;$D$1&amp;"="&amp;$D$128&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=127,DegreePlanID=15,TermID=4,RequirementID=691},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=127,DegreePlanID=15,TermID=4,RequirementID=691},</v>
       </c>
     </row>
     <row r="129" spans="1:7" ht="15.75" customHeight="1">
@@ -8237,14 +8231,14 @@
         <v>10</v>
       </c>
       <c r="E129" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F129" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G129" t="str">
         <f>E129&amp;$A$1&amp;"="&amp;$A$129&amp;","&amp;$B$1&amp;"="&amp;$B$129&amp;","&amp;$C$1&amp;"="&amp;$C$129&amp;","&amp;$D$1&amp;"="&amp;$D$129&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=128,DegreePlanID=15,TermID=5,RequirementID=10},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=128,DegreePlanID=15,TermID=5,RequirementID=10},</v>
       </c>
     </row>
     <row r="130" spans="1:7" ht="15.75" customHeight="1">
@@ -8261,14 +8255,14 @@
         <v>20</v>
       </c>
       <c r="E130" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F130" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G130" t="str">
         <f>E130&amp;$A$1&amp;"="&amp;$A$130&amp;","&amp;$B$1&amp;"="&amp;$B$130&amp;","&amp;$C$1&amp;"="&amp;$C$130&amp;","&amp;$D$1&amp;"="&amp;$D$130&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=129,DegreePlanID=15,TermID=5,RequirementID=20},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=129,DegreePlanID=15,TermID=5,RequirementID=20},</v>
       </c>
     </row>
     <row r="131" spans="1:7" ht="15.75" customHeight="1">
@@ -8285,14 +8279,14 @@
         <v>692</v>
       </c>
       <c r="E131" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F131" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G131" t="str">
         <f>E131&amp;$A$1&amp;"="&amp;$A$131&amp;","&amp;$B$1&amp;"="&amp;$B$131&amp;","&amp;$C$1&amp;"="&amp;$C$131&amp;","&amp;$D$1&amp;"="&amp;$D$131&amp;$F$2</f>
-        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementId=130,DegreePlanID=15,TermID=5,RequirementID=692},</v>
+        <v>new Models.DegreePlanTermRequirement {DegreePlanTermRequirementID=130,DegreePlanID=15,TermID=5,RequirementID=692},</v>
       </c>
     </row>
     <row r="132" spans="1:7" ht="15.75" customHeight="1"/>
@@ -9174,11 +9168,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H11"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -9194,28 +9188,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" t="s">
         <v>37</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>38</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>39</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>40</v>
       </c>
-      <c r="E1" t="s">
-        <v>41</v>
-      </c>
       <c r="F1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="G1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="H1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -9226,23 +9220,23 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H2" t="str">
         <f>F2&amp;$A$1&amp;"="&amp;A2&amp;","&amp;$B$1&amp;"="&amp;B2&amp;","&amp;$C$1&amp;"="&amp;C2&amp;","&amp;$D$1&amp;"="&amp;D2&amp;""&amp;$E$1&amp;"="""&amp;E2&amp;G2</f>
-        <v>new Models.DegreePlan{DegreePlanId=12,DegreeID=1,StudentId=S531494,DegreePlanAbbrev(u,8)=NSODegreePlanName(u,20)="No summer off},</v>
+        <v>new Models.DegreePlan{DegreePlanID=12,DegreeID=1,StudentId=S531494,DegreePlanAbbrev(u,8)=NSODegreePlanName(u,20)="No summer off},</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -9253,23 +9247,23 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H3" t="str">
         <f t="shared" ref="H3:H11" si="0">F3&amp;$A$1&amp;"="&amp;A3&amp;","&amp;$B$1&amp;"="&amp;B3&amp;","&amp;$C$1&amp;"="&amp;C3&amp;","&amp;$D$1&amp;"="&amp;D3&amp;""&amp;$E$1&amp;"="""&amp;E3&amp;G3</f>
-        <v>new Models.DegreePlan{DegreePlanId=13,DegreeID=1,StudentId=S531494,DegreePlanAbbrev(u,8)=SODegreePlanName(u,20)="summer off},</v>
+        <v>new Models.DegreePlan{DegreePlanID=13,DegreeID=1,StudentId=S531494,DegreePlanAbbrev(u,8)=SODegreePlanName(u,20)="summer off},</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -9280,23 +9274,23 @@
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.DegreePlan{DegreePlanId=14,DegreeID=1,StudentId=s531507,DegreePlanAbbrev(u,8)=SODegreePlanName(u,20)="summer off},</v>
+        <v>new Models.DegreePlan{DegreePlanID=14,DegreeID=1,StudentId=s531507,DegreePlanAbbrev(u,8)=SODegreePlanName(u,20)="summer off},</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -9307,23 +9301,23 @@
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H5" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.DegreePlan{DegreePlanId=15,DegreeID=1,StudentId=s531507,DegreePlanAbbrev(u,8)=NSODegreePlanName(u,20)="No summer off},</v>
+        <v>new Models.DegreePlan{DegreePlanID=15,DegreeID=1,StudentId=s531507,DegreePlanAbbrev(u,8)=NSODegreePlanName(u,20)="No summer off},</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -9334,23 +9328,23 @@
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G6" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.DegreePlan{DegreePlanId=16,DegreeID=1,StudentId=s533707,DegreePlanAbbrev(u,8)=SODegreePlanName(u,20)="summer off},</v>
+        <v>new Models.DegreePlan{DegreePlanID=16,DegreeID=1,StudentId=s533707,DegreePlanAbbrev(u,8)=SODegreePlanName(u,20)="summer off},</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -9361,23 +9355,23 @@
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F7" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G7" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.DegreePlan{DegreePlanId=17,DegreeID=1,StudentId=s533707,DegreePlanAbbrev(u,8)=NSODegreePlanName(u,20)="No summer off},</v>
+        <v>new Models.DegreePlan{DegreePlanID=17,DegreeID=1,StudentId=s533707,DegreePlanAbbrev(u,8)=NSODegreePlanName(u,20)="No summer off},</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -9388,23 +9382,23 @@
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F8" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G8" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.DegreePlan{DegreePlanId=18,DegreeID=1,StudentId=s531384,DegreePlanAbbrev(u,8)=NSODegreePlanName(u,20)="No summer off},</v>
+        <v>new Models.DegreePlan{DegreePlanID=18,DegreeID=1,StudentId=s531384,DegreePlanAbbrev(u,8)=NSODegreePlanName(u,20)="No summer off},</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -9415,23 +9409,23 @@
         <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F9" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G9" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.DegreePlan{DegreePlanId=19,DegreeID=1,StudentId=s531384,DegreePlanAbbrev(u,8)=SODegreePlanName(u,20)="summer off},</v>
+        <v>new Models.DegreePlan{DegreePlanID=19,DegreeID=1,StudentId=s531384,DegreePlanAbbrev(u,8)=SODegreePlanName(u,20)="summer off},</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -9442,23 +9436,23 @@
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>52</v>
-      </c>
       <c r="F10" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G10" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.DegreePlan{DegreePlanId=20,DegreeID=1,StudentId=S531503,DegreePlanAbbrev(u,8)=NSODegreePlanName(u,20)="No summer off},</v>
+        <v>new Models.DegreePlan{DegreePlanID=20,DegreeID=1,StudentId=S531503,DegreePlanAbbrev(u,8)=NSODegreePlanName(u,20)="No summer off},</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -9469,23 +9463,23 @@
         <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F11" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G11" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.DegreePlan{DegreePlanId=21,DegreeID=1,StudentId=s531503,DegreePlanAbbrev(u,8)=SODegreePlanName(u,20)="summer off},</v>
+        <v>new Models.DegreePlan{DegreePlanID=21,DegreeID=1,StudentId=s531503,DegreePlanAbbrev(u,8)=SODegreePlanName(u,20)="summer off},</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -10475,12 +10469,10 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -10493,28 +10485,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="B1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="G1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="H1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -10522,26 +10514,26 @@
         <v>531494</v>
       </c>
       <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
         <v>45</v>
-      </c>
-      <c r="C2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2" t="s">
-        <v>47</v>
       </c>
       <c r="E2">
         <v>919564348</v>
       </c>
       <c r="F2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H2" t="str">
         <f>$F$2&amp;$A$1&amp;"="&amp;$A$2&amp;","&amp;$B$1&amp;"="&amp;$B$2&amp;","&amp;$C$1&amp;"="&amp;$C$2&amp;","&amp;$D$1&amp;"="&amp;$D$2&amp;","&amp;$E$1&amp;"="&amp;$E$2&amp;$G$2</f>
-        <v>new Models.Student{StudentId=531494,FirstName=Shivani,LastName=Busireddy,Snumber=S531494,NineOneNineNumber=919564348},</v>
+        <v>new Models.Student{StudentID=531494,FirstName=Shivani,LastName=Busireddy,Snumber=S531494,NineOneNineNumber=919564348},</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -10549,26 +10541,26 @@
         <v>531503</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="E3" s="2">
         <v>919561527</v>
       </c>
       <c r="F3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H3" t="str">
         <f>$F$2&amp;$A$1&amp;"="&amp;$A$3&amp;","&amp;$B$1&amp;"="&amp;$B$3&amp;","&amp;$C$1&amp;"="&amp;$C$3&amp;","&amp;$D$1&amp;"="&amp;$D$3&amp;","&amp;$E$1&amp;"="&amp;$E$3&amp;$G$2</f>
-        <v>new Models.Student{StudentId=531503,FirstName=Santosh ,LastName=Muchkur,Snumber=S531503,NineOneNineNumber=919561527},</v>
+        <v>new Models.Student{StudentID=531503,FirstName=Santosh ,LastName=Muchkur,Snumber=S531503,NineOneNineNumber=919561527},</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -10576,26 +10568,26 @@
         <v>531384</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E4" s="2">
         <v>919561950</v>
       </c>
       <c r="F4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H4" t="str">
         <f>$F$2&amp;$A$1&amp;"="&amp;$A$4&amp;","&amp;$B$1&amp;"="&amp;$B$4&amp;","&amp;$C$1&amp;"="&amp;$C$4&amp;","&amp;$D$1&amp;"="&amp;$D$4&amp;","&amp;$E$1&amp;"="&amp;$E$4&amp;$G$2</f>
-        <v>new Models.Student{StudentId=531384,FirstName=Srimai Reddy ,LastName=Yanala,Snumber=s531384,NineOneNineNumber=919561950},</v>
+        <v>new Models.Student{StudentID=531384,FirstName=Srimai Reddy ,LastName=Yanala,Snumber=s531384,NineOneNineNumber=919561950},</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -10603,26 +10595,26 @@
         <v>533707</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="E5" s="2">
         <v>919571235</v>
       </c>
       <c r="F5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H5" t="str">
         <f>$F$2&amp;$A$1&amp;"="&amp;$A$5&amp;","&amp;$B$1&amp;"="&amp;$B$5&amp;","&amp;$C$1&amp;"="&amp;$C$5&amp;","&amp;$D$1&amp;"="&amp;$D$5&amp;","&amp;$E$1&amp;"="&amp;$E$5&amp;$G$2</f>
-        <v>new Models.Student{StudentId=533707,FirstName=Lakshmi Seshu,LastName=Kalvakuri,Snumber=s533707,NineOneNineNumber=919571235},</v>
+        <v>new Models.Student{StudentID=533707,FirstName=Lakshmi Seshu,LastName=Kalvakuri,Snumber=s533707,NineOneNineNumber=919571235},</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -10630,26 +10622,26 @@
         <v>531507</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>64</v>
       </c>
       <c r="E6" s="2">
         <v>919564693</v>
       </c>
       <c r="F6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G6" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H6" t="str">
         <f>$F$2&amp;$A$1&amp;"="&amp;$A$6&amp;","&amp;$B$1&amp;"="&amp;$B$6&amp;","&amp;$C$1&amp;"="&amp;$C$6&amp;","&amp;$D$1&amp;"="&amp;$D$6&amp;","&amp;$E$1&amp;"="&amp;$E$6&amp;$G$2</f>
-        <v>new Models.Student{StudentId=531507,FirstName=Vijay,LastName=Thupakala,Snumber=S531507,NineOneNineNumber=919564693},</v>
+        <v>new Models.Student{StudentID=531507,FirstName=Vijay,LastName=Thupakala,Snumber=S531507,NineOneNineNumber=919564693},</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -11639,12 +11631,10 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H995"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -11657,28 +11647,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>108</v>
       </c>
       <c r="B1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" t="s">
         <v>101</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E1" t="s">
-        <v>97</v>
-      </c>
-      <c r="F1" t="s">
-        <v>104</v>
-      </c>
       <c r="G1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="H1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -11692,20 +11682,20 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H2" t="str">
         <f>F2&amp;$A$1&amp;"="&amp;$A2&amp;","&amp;$B$1&amp;"="&amp;B2&amp;","&amp;$C$1&amp;"="&amp;C2&amp;","&amp;$D$1&amp;"="&amp;D2&amp;","&amp;$E$1&amp;"="&amp;E2&amp;$G$2</f>
-        <v>new Models.StudentTerm{StudentTermId=1,StudentID=531494,TermID=1,TermAbbrev=S18,TermLabel=Spring 2018},</v>
+        <v>new Models.StudentTerm{StudentTermID=1,StudentID=531494,TermID=1,TermAbbrev=S18,TermLabel=Spring 2018},</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -11719,20 +11709,20 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H3" t="str">
         <f t="shared" ref="H3:H26" si="0">F3&amp;$A$1&amp;"="&amp;$A3&amp;","&amp;$B$1&amp;"="&amp;B3&amp;","&amp;$C$1&amp;"="&amp;C3&amp;","&amp;$D$1&amp;"="&amp;D3&amp;","&amp;$E$1&amp;"="&amp;E3&amp;$G$2</f>
-        <v>new Models.StudentTerm{StudentTermId=2,StudentID=531494,TermID=2,TermAbbrev=Su18,TermLabel=Summer 2018},</v>
+        <v>new Models.StudentTerm{StudentTermID=2,StudentID=531494,TermID=2,TermAbbrev=Su18,TermLabel=Summer 2018},</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -11746,20 +11736,20 @@
         <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.StudentTerm{StudentTermId=3,StudentID=531494,TermID=3,TermAbbrev=F18,TermLabel=Fall 2018},</v>
+        <v>new Models.StudentTerm{StudentTermID=3,StudentID=531494,TermID=3,TermAbbrev=F18,TermLabel=Fall 2018},</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -11773,20 +11763,20 @@
         <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H5" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.StudentTerm{StudentTermId=4,StudentID=531494,TermID=4,TermAbbrev=S19,TermLabel=Spring 2019},</v>
+        <v>new Models.StudentTerm{StudentTermID=4,StudentID=531494,TermID=4,TermAbbrev=S19,TermLabel=Spring 2019},</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -11800,20 +11790,20 @@
         <v>5</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G6" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.StudentTerm{StudentTermId=5,StudentID=531494,TermID=5,TermAbbrev=Su19,TermLabel=Summer2019},</v>
+        <v>new Models.StudentTerm{StudentTermID=5,StudentID=531494,TermID=5,TermAbbrev=Su19,TermLabel=Summer2019},</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -11827,20 +11817,20 @@
         <v>1</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G7" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.StudentTerm{StudentTermId=6,StudentID=531503,TermID=1,TermAbbrev=F17,TermLabel=Fall 2017},</v>
+        <v>new Models.StudentTerm{StudentTermID=6,StudentID=531503,TermID=1,TermAbbrev=F17,TermLabel=Fall 2017},</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -11854,20 +11844,20 @@
         <v>2</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F8" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G8" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.StudentTerm{StudentTermId=7,StudentID=531503,TermID=2,TermAbbrev=S18,TermLabel=Spring 2018},</v>
+        <v>new Models.StudentTerm{StudentTermID=7,StudentID=531503,TermID=2,TermAbbrev=S18,TermLabel=Spring 2018},</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -11881,20 +11871,20 @@
         <v>3</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E9" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F9" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G9" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.StudentTerm{StudentTermId=8,StudentID=531503,TermID=3,TermAbbrev=Su18,TermLabel=Summer 2018},</v>
+        <v>new Models.StudentTerm{StudentTermID=8,StudentID=531503,TermID=3,TermAbbrev=Su18,TermLabel=Summer 2018},</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -11908,20 +11898,20 @@
         <v>4</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E10" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F10" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G10" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.StudentTerm{StudentTermId=9,StudentID=531503,TermID=4,TermAbbrev=F18,TermLabel=Fall 2018},</v>
+        <v>new Models.StudentTerm{StudentTermID=9,StudentID=531503,TermID=4,TermAbbrev=F18,TermLabel=Fall 2018},</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -11935,20 +11925,20 @@
         <v>5</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E11" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F11" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G11" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.StudentTerm{StudentTermId=10,StudentID=531503,TermID=5,TermAbbrev=S19,TermLabel=Spring 2019},</v>
+        <v>new Models.StudentTerm{StudentTermID=10,StudentID=531503,TermID=5,TermAbbrev=S19,TermLabel=Spring 2019},</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -11962,20 +11952,20 @@
         <v>1</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F12" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G12" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.StudentTerm{StudentTermId=11,StudentID=531384,TermID=1,TermAbbrev=S18,TermLabel=Fall 2019},</v>
+        <v>new Models.StudentTerm{StudentTermID=11,StudentID=531384,TermID=1,TermAbbrev=S18,TermLabel=Fall 2019},</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -11989,20 +11979,20 @@
         <v>2</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F13" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G13" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.StudentTerm{StudentTermId=12,StudentID=531384,TermID=2,TermAbbrev=Su18,TermLabel=Spring 2020},</v>
+        <v>new Models.StudentTerm{StudentTermID=12,StudentID=531384,TermID=2,TermAbbrev=Su18,TermLabel=Spring 2020},</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -12016,20 +12006,20 @@
         <v>3</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F14" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G14" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.StudentTerm{StudentTermId=13,StudentID=531384,TermID=3,TermAbbrev=F18,TermLabel=Summer 2020},</v>
+        <v>new Models.StudentTerm{StudentTermID=13,StudentID=531384,TermID=3,TermAbbrev=F18,TermLabel=Summer 2020},</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -12043,20 +12033,20 @@
         <v>4</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F15" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G15" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.StudentTerm{StudentTermId=14,StudentID=531384,TermID=4,TermAbbrev=S19,TermLabel=Fall 2020},</v>
+        <v>new Models.StudentTerm{StudentTermID=14,StudentID=531384,TermID=4,TermAbbrev=S19,TermLabel=Fall 2020},</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" customHeight="1">
@@ -12070,20 +12060,20 @@
         <v>5</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F16" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G16" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.StudentTerm{StudentTermId=15,StudentID=531384,TermID=5,TermAbbrev=Su19,TermLabel=Spring 2021},</v>
+        <v>new Models.StudentTerm{StudentTermID=15,StudentID=531384,TermID=5,TermAbbrev=Su19,TermLabel=Spring 2021},</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15.75" customHeight="1">
@@ -12097,20 +12087,20 @@
         <v>1</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F17" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G17" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H17" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.StudentTerm{StudentTermId=16,StudentID=533707,TermID=1,TermAbbrev=F18,TermLabel=Fall 2018},</v>
+        <v>new Models.StudentTerm{StudentTermID=16,StudentID=533707,TermID=1,TermAbbrev=F18,TermLabel=Fall 2018},</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1">
@@ -12124,20 +12114,20 @@
         <v>2</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F18" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H18" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.StudentTerm{StudentTermId=17,StudentID=533707,TermID=2,TermAbbrev=S19,TermLabel=spring 2019},</v>
+        <v>new Models.StudentTerm{StudentTermID=17,StudentID=533707,TermID=2,TermAbbrev=S19,TermLabel=spring 2019},</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="15.75" customHeight="1">
@@ -12151,20 +12141,20 @@
         <v>3</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F19" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G19" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.StudentTerm{StudentTermId=18,StudentID=533707,TermID=3,TermAbbrev=Su19,TermLabel=summer 2019},</v>
+        <v>new Models.StudentTerm{StudentTermID=18,StudentID=533707,TermID=3,TermAbbrev=Su19,TermLabel=summer 2019},</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="15.75" customHeight="1">
@@ -12178,20 +12168,20 @@
         <v>4</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F20" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G20" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.StudentTerm{StudentTermId=19,StudentID=533707,TermID=4,TermAbbrev=F19,TermLabel=Fall 2019},</v>
+        <v>new Models.StudentTerm{StudentTermID=19,StudentID=533707,TermID=4,TermAbbrev=F19,TermLabel=Fall 2019},</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="15.75" customHeight="1">
@@ -12205,20 +12195,20 @@
         <v>5</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F21" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G21" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.StudentTerm{StudentTermId=20,StudentID=533707,TermID=5,TermAbbrev=S20,TermLabel=Spring 2020},</v>
+        <v>new Models.StudentTerm{StudentTermID=20,StudentID=533707,TermID=5,TermAbbrev=S20,TermLabel=Spring 2020},</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="15.75" customHeight="1">
@@ -12232,20 +12222,20 @@
         <v>1</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F22" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G22" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.StudentTerm{StudentTermId=21,StudentID=531507,TermID=1,TermAbbrev=S19,TermLabel=Spring 2019},</v>
+        <v>new Models.StudentTerm{StudentTermID=21,StudentID=531507,TermID=1,TermAbbrev=S19,TermLabel=Spring 2019},</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="15.75" customHeight="1">
@@ -12259,20 +12249,20 @@
         <v>2</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F23" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G23" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H23" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.StudentTerm{StudentTermId=22,StudentID=531507,TermID=2,TermAbbrev=Su19,TermLabel=Summer 2019},</v>
+        <v>new Models.StudentTerm{StudentTermID=22,StudentID=531507,TermID=2,TermAbbrev=Su19,TermLabel=Summer 2019},</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15.75" customHeight="1">
@@ -12286,20 +12276,20 @@
         <v>3</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F24" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G24" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H24" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.StudentTerm{StudentTermId=23,StudentID=531507,TermID=3,TermAbbrev=F19,TermLabel=Fall 2019},</v>
+        <v>new Models.StudentTerm{StudentTermID=23,StudentID=531507,TermID=3,TermAbbrev=F19,TermLabel=Fall 2019},</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1">
@@ -12313,20 +12303,20 @@
         <v>4</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F25" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G25" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H25" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.StudentTerm{StudentTermId=24,StudentID=531507,TermID=4,TermAbbrev=S20,TermLabel=Spring 2020},</v>
+        <v>new Models.StudentTerm{StudentTermID=24,StudentID=531507,TermID=4,TermAbbrev=S20,TermLabel=Spring 2020},</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="15.75" customHeight="1">
@@ -12340,20 +12330,20 @@
         <v>5</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F26" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G26" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H26" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.StudentTerm{StudentTermId=25,StudentID=531507,TermID=5,TermAbbrev=Su20,TermLabel=Summer 2020},</v>
+        <v>new Models.StudentTerm{StudentTermID=25,StudentID=531507,TermID=5,TermAbbrev=Su20,TermLabel=Summer 2020},</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="15.75" customHeight="1"/>

</xml_diff>